<commit_message>
Remove bower_components tracking from repo
This is a generated file and doesn't need to be tracked in the repo.
Add `bower install` instruction to README  --bower components do need
to be installed for the framework to run correctly locally.
</commit_message>
<xml_diff>
--- a/_data/_data.xlsx
+++ b/_data/_data.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26330"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andy.fitzgerald/Dropbox/Web/CFP-Framework/_data/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="8680" windowWidth="27300" windowHeight="14800" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="2080" yWindow="7620" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="navigation" sheetId="4" r:id="rId1"/>
@@ -23,7 +18,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">feed!$A$1:$D$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">navigation!$A$1:$D$1</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -660,7 +655,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -674,7 +669,7 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="24" customWidth="1"/>
     <col min="2" max="2" width="48" customWidth="1"/>
@@ -682,7 +677,7 @@
     <col min="4" max="4" width="48" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" s="10" t="s">
         <v>9</v>
       </c>
@@ -696,7 +691,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" s="7" t="s">
         <v>17</v>
       </c>
@@ -708,7 +703,7 @@
       <c r="E2" s="7"/>
       <c r="F2" s="9"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -717,7 +712,7 @@
       </c>
       <c r="C3" s="16"/>
     </row>
-    <row r="4" spans="1:6" s="26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" s="26" customFormat="1">
       <c r="A4" s="26" t="s">
         <v>22</v>
       </c>
@@ -726,7 +721,7 @@
       </c>
       <c r="C4" s="27"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -735,12 +730,17 @@
       </c>
       <c r="C5" s="16"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="C6" s="16"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:D1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -750,10 +750,10 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="24" style="18" customWidth="1"/>
     <col min="2" max="2" width="48" style="18" customWidth="1"/>
@@ -762,7 +762,7 @@
     <col min="6" max="16384" width="10.83203125" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="23" customFormat="1">
       <c r="A1" s="24" t="s">
         <v>30</v>
       </c>
@@ -779,7 +779,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" s="17" t="s">
         <v>29</v>
       </c>
@@ -789,101 +789,106 @@
       <c r="D2" s="17"/>
       <c r="E2" s="25"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" s="17"/>
       <c r="B3" s="22"/>
       <c r="D3" s="17"/>
       <c r="E3" s="17"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" s="17"/>
       <c r="B4" s="22"/>
       <c r="C4" s="18"/>
       <c r="D4" s="17"/>
       <c r="E4" s="17"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" s="17"/>
       <c r="B5" s="22"/>
       <c r="C5" s="18"/>
       <c r="D5" s="17"/>
       <c r="E5" s="17"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" s="17"/>
       <c r="B6" s="22"/>
       <c r="D6" s="17"/>
       <c r="E6" s="17"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="B7" s="22"/>
       <c r="D7" s="17"/>
       <c r="E7" s="17"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="B8" s="22"/>
       <c r="D8" s="17"/>
       <c r="E8" s="17"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="B9" s="22"/>
       <c r="D9" s="17"/>
       <c r="E9" s="17"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="B10" s="22"/>
       <c r="E10" s="17"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="B11" s="22"/>
       <c r="D11" s="17"/>
       <c r="E11" s="17"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="B12" s="22"/>
       <c r="D12" s="17"/>
       <c r="E12" s="17"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5">
       <c r="B13" s="22"/>
       <c r="D13" s="17"/>
       <c r="E13" s="17"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5">
       <c r="B14" s="22"/>
       <c r="D14" s="17"/>
       <c r="E14" s="17"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5">
       <c r="B15" s="22"/>
       <c r="D15" s="17"/>
       <c r="E15" s="17"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5">
       <c r="B16" s="22"/>
       <c r="D16" s="17"/>
       <c r="E16" s="17"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:5">
       <c r="B17" s="22"/>
     </row>
-    <row r="18" spans="2:5" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:5" s="17" customFormat="1">
       <c r="B18" s="22"/>
       <c r="E18" s="18"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:5">
       <c r="B19" s="22"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:5">
       <c r="B20" s="22"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:5">
       <c r="B21" s="22"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:E2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -895,7 +900,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="3" width="24" style="4" customWidth="1"/>
     <col min="4" max="4" width="48" style="6" customWidth="1"/>
@@ -904,7 +909,7 @@
     <col min="7" max="16384" width="10.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="1" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -924,7 +929,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" s="4" t="s">
         <v>25</v>
       </c>
@@ -940,112 +945,117 @@
       </c>
       <c r="E2" s="20"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="4"/>
       <c r="E3" s="20"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
       <c r="D4" s="2"/>
       <c r="E4" s="20"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="D5" s="4"/>
       <c r="E5" s="13"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="4"/>
       <c r="E6" s="13"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="8"/>
       <c r="E7" s="14"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="4"/>
       <c r="E8" s="13"/>
     </row>
-    <row r="9" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" s="4" customFormat="1">
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="E9" s="13"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="15"/>
       <c r="E10" s="13"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6">
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6">
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
     </row>
-    <row r="17" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:3" s="6" customFormat="1">
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
     </row>
-    <row r="18" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:3" s="6" customFormat="1">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
     </row>
-    <row r="19" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:3" s="6" customFormat="1">
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
     </row>
-    <row r="20" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:3" s="6" customFormat="1">
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
     </row>
-    <row r="21" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:3" s="6" customFormat="1">
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
     </row>
-    <row r="22" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:3" s="6" customFormat="1">
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
     </row>
-    <row r="23" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:3" s="6" customFormat="1">
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
     </row>
-    <row r="24" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:3" s="6" customFormat="1">
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:F1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1057,14 +1067,14 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="3" width="24" style="7" customWidth="1"/>
     <col min="4" max="4" width="48" style="9" customWidth="1"/>
     <col min="5" max="16384" width="10.83203125" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" s="11" customFormat="1">
       <c r="A1" s="10" t="s">
         <v>2</v>
       </c>
@@ -1078,7 +1088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
         <v>28</v>
       </c>
@@ -1090,63 +1100,68 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="B3" s="5"/>
       <c r="C3" s="12"/>
       <c r="D3" s="19"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="B4" s="5"/>
       <c r="C4" s="12"/>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="B5" s="5"/>
       <c r="C5" s="12"/>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="B6" s="5"/>
       <c r="C6" s="12"/>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4">
       <c r="C7" s="12"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4">
       <c r="C8" s="12"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4">
       <c r="A9" s="22"/>
       <c r="B9" s="22"/>
       <c r="C9" s="12"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4">
       <c r="C10" s="12"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4">
       <c r="C11" s="12"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4">
       <c r="C12" s="12"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4">
       <c r="C13" s="12"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4">
       <c r="C14" s="12"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4">
       <c r="C15" s="12"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4">
       <c r="C16" s="12"/>
     </row>
-    <row r="17" spans="3:3" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:3" s="9" customFormat="1">
       <c r="C17" s="12"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:D1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix markdown formatting error in README
</commit_message>
<xml_diff>
--- a/_data/_data.xlsx
+++ b/_data/_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26330"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2080" yWindow="7620" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="navigation" sheetId="4" r:id="rId1"/>
@@ -655,7 +655,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -750,7 +750,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Commit saved version of _data.xlsx
File was closed after last final commit of the day.
</commit_message>
<xml_diff>
--- a/_data/_data.xlsx
+++ b/_data/_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26330"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="19740" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="19740" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="navigation" sheetId="4" r:id="rId1"/>
@@ -1359,7 +1359,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M124"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
     </sheetView>
@@ -3529,9 +3529,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K124"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A109" sqref="A109"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3590,23 +3590,23 @@
         <v>77</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="E2" s="12"/>
       <c r="F2" s="18"/>
       <c r="G2" s="14"/>
       <c r="H2" s="12"/>
-      <c r="I2" s="13" t="s">
-        <v>61</v>
+      <c r="I2" s="12" t="s">
+        <v>72</v>
       </c>
       <c r="J2" s="12" t="s">
         <v>73</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -3617,349 +3617,371 @@
         <v>77</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="E3" s="12"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="14"/>
+        <v>23</v>
+      </c>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
       <c r="H3" s="12"/>
-      <c r="I3" s="13" t="s">
-        <v>61</v>
+      <c r="I3" s="12" t="s">
+        <v>19</v>
       </c>
       <c r="J3" s="12" t="s">
         <v>73</v>
       </c>
       <c r="K3" s="12" t="s">
-        <v>84</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="12" t="s">
-        <v>76</v>
+        <v>21</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>85</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="D4" s="12"/>
       <c r="E4" s="12"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="12"/>
+      <c r="F4" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12" t="s">
+        <v>21</v>
+      </c>
       <c r="I4" s="12" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="J4" s="12" t="s">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="K4" s="12" t="s">
-        <v>85</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="12" t="s">
-        <v>76</v>
+        <v>21</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>86</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="D5" s="12"/>
       <c r="E5" s="12"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="12"/>
+      <c r="F5" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12" t="s">
+        <v>21</v>
+      </c>
       <c r="I5" s="12" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>86</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="12" t="s">
-        <v>76</v>
+        <v>21</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="12" t="s">
-        <v>87</v>
-      </c>
+      <c r="D6" s="12"/>
       <c r="E6" s="12"/>
-      <c r="F6" s="18"/>
+      <c r="F6" s="12" t="s">
+        <v>33</v>
+      </c>
       <c r="G6" s="14"/>
-      <c r="H6" s="12"/>
+      <c r="H6" s="12" t="s">
+        <v>21</v>
+      </c>
       <c r="I6" s="12" t="s">
-        <v>72</v>
+        <v>25</v>
       </c>
       <c r="J6" s="12" t="s">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="K6" s="12" t="s">
-        <v>87</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="12" t="s">
-        <v>76</v>
+        <v>21</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>88</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="D7" s="12"/>
       <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
+      <c r="F7" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="G7" s="14"/>
-      <c r="H7" s="12"/>
+      <c r="H7" s="12" t="s">
+        <v>21</v>
+      </c>
       <c r="I7" s="12" t="s">
-        <v>72</v>
+        <v>25</v>
       </c>
       <c r="J7" s="12" t="s">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="K7" s="12" t="s">
-        <v>88</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="12" t="s">
-        <v>76</v>
+        <v>21</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>89</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="D8" s="12"/>
       <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
+      <c r="F8" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" s="14"/>
+      <c r="H8" s="12" t="s">
+        <v>21</v>
+      </c>
       <c r="I8" s="12" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="K8" s="12" t="s">
-        <v>89</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="12" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D9" s="12"/>
-      <c r="E9" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12" t="s">
+        <v>57</v>
+      </c>
       <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
+      <c r="H9" s="12" t="s">
+        <v>56</v>
+      </c>
       <c r="I9" s="12" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="J9" s="12" t="s">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="K9" s="12" t="s">
-        <v>18</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="12" t="s">
-        <v>76</v>
+        <v>119</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>90</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="D10" s="12"/>
       <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="12"/>
+      <c r="F10" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12" t="s">
+        <v>119</v>
+      </c>
       <c r="I10" s="12" t="s">
-        <v>72</v>
+        <v>39</v>
       </c>
       <c r="J10" s="12" t="s">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="K10" s="12" t="s">
-        <v>90</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="12" t="s">
-        <v>76</v>
+        <v>21</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>77</v>
+        <v>22</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>91</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="D11" s="12"/>
       <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="12"/>
+      <c r="F11" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12" t="s">
+        <v>21</v>
+      </c>
       <c r="I11" s="12" t="s">
-        <v>72</v>
+        <v>25</v>
       </c>
       <c r="J11" s="12" t="s">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="K11" s="12" t="s">
-        <v>91</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="12" t="s">
-        <v>76</v>
+        <v>21</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>77</v>
+        <v>22</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>92</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="D12" s="12"/>
       <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="12"/>
+      <c r="F12" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12" t="s">
+        <v>21</v>
+      </c>
       <c r="I12" s="12" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="J12" s="12" t="s">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="K12" s="12" t="s">
-        <v>92</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="12" t="s">
-        <v>76</v>
+        <v>21</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>77</v>
+        <v>22</v>
       </c>
       <c r="C13" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D13" s="12"/>
-      <c r="E13" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="F13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
+      <c r="H13" s="12" t="s">
+        <v>21</v>
+      </c>
       <c r="I13" s="12" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="J13" s="12" t="s">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="K13" s="12" t="s">
-        <v>117</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="12" t="s">
-        <v>76</v>
+        <v>21</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>77</v>
+        <v>22</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>93</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="D14" s="12"/>
       <c r="E14" s="12"/>
-      <c r="F14" s="18"/>
+      <c r="F14" s="12" t="s">
+        <v>28</v>
+      </c>
       <c r="G14" s="12"/>
       <c r="H14" s="12" t="s">
-        <v>94</v>
+        <v>21</v>
       </c>
       <c r="I14" s="12" t="s">
-        <v>72</v>
+        <v>25</v>
       </c>
       <c r="J14" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="K14" s="18" t="s">
-        <v>93</v>
+        <v>20</v>
+      </c>
+      <c r="K14" s="12" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="12" t="s">
-        <v>76</v>
+        <v>21</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>77</v>
+        <v>30</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>58</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="D15" s="12"/>
       <c r="E15" s="12"/>
-      <c r="F15" s="18"/>
+      <c r="F15" s="12" t="s">
+        <v>31</v>
+      </c>
       <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
+      <c r="H15" s="12" t="s">
+        <v>21</v>
+      </c>
       <c r="I15" s="12" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="J15" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="K15" s="18" t="s">
-        <v>58</v>
+        <v>20</v>
+      </c>
+      <c r="K15" s="12" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -3970,513 +3992,545 @@
         <v>77</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>205</v>
-      </c>
-      <c r="E16" s="12"/>
-      <c r="F16" s="18"/>
+        <v>18</v>
+      </c>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" s="12"/>
       <c r="G16" s="12"/>
       <c r="H16" s="12"/>
       <c r="I16" s="12" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="J16" s="12" t="s">
         <v>73</v>
       </c>
       <c r="K16" s="12" t="s">
-        <v>205</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="12" t="s">
-        <v>76</v>
+        <v>16</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>206</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="D17" s="12"/>
       <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
+      <c r="F17" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17" s="14"/>
+      <c r="H17" s="12" t="s">
+        <v>16</v>
+      </c>
       <c r="I17" s="12" t="s">
-        <v>72</v>
+        <v>19</v>
       </c>
       <c r="J17" s="12" t="s">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="K17" s="12" t="s">
-        <v>206</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:11" s="7" customFormat="1">
       <c r="A18" s="12" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>95</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="D18" s="12"/>
       <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
+      <c r="F18" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G18" s="14"/>
+      <c r="H18" s="12" t="s">
+        <v>40</v>
+      </c>
       <c r="I18" s="12" t="s">
-        <v>61</v>
+        <v>19</v>
       </c>
       <c r="J18" s="12" t="s">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="K18" s="12" t="s">
-        <v>95</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="12" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>96</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="D19" s="12"/>
       <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
+      <c r="F19" s="12" t="s">
+        <v>42</v>
+      </c>
       <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
+      <c r="H19" s="12" t="s">
+        <v>40</v>
+      </c>
       <c r="I19" s="12" t="s">
-        <v>61</v>
+        <v>19</v>
       </c>
       <c r="J19" s="12" t="s">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="K19" s="12" t="s">
-        <v>96</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="12" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>97</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="D20" s="12"/>
       <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
+      <c r="F20" s="12" t="s">
+        <v>43</v>
+      </c>
       <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
+      <c r="H20" s="12" t="s">
+        <v>40</v>
+      </c>
       <c r="I20" s="12" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="J20" s="12" t="s">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="K20" s="12" t="s">
-        <v>97</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="12" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="D21" s="12" t="s">
-        <v>207</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="D21" s="18"/>
       <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
+      <c r="F21" s="12" t="s">
+        <v>44</v>
+      </c>
       <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
+      <c r="H21" s="12" t="s">
+        <v>40</v>
+      </c>
       <c r="I21" s="12" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="J21" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="K21" s="12" t="s">
-        <v>207</v>
+        <v>20</v>
+      </c>
+      <c r="K21" s="18" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:11">
       <c r="A22" s="12" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>98</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="D22" s="12"/>
       <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
+      <c r="F22" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="G22" s="14"/>
+      <c r="H22" s="12" t="s">
+        <v>40</v>
+      </c>
       <c r="I22" s="12" t="s">
-        <v>61</v>
+        <v>19</v>
       </c>
       <c r="J22" s="12" t="s">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="K22" s="12" t="s">
-        <v>98</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="12" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="D23" s="18" t="s">
-        <v>99</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="D23" s="12"/>
       <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
+      <c r="F23" s="12" t="s">
+        <v>49</v>
+      </c>
       <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
+      <c r="H23" s="12" t="s">
+        <v>40</v>
+      </c>
       <c r="I23" s="12" t="s">
-        <v>61</v>
+        <v>19</v>
       </c>
       <c r="J23" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="K23" s="18" t="s">
-        <v>99</v>
+        <v>20</v>
+      </c>
+      <c r="K23" s="12" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="12" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="D24" s="12" t="s">
-        <v>100</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="D24" s="12"/>
       <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
+      <c r="F24" s="12" t="s">
+        <v>51</v>
+      </c>
       <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
+      <c r="H24" s="12" t="s">
+        <v>40</v>
+      </c>
       <c r="I24" s="12" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="J24" s="12" t="s">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="K24" s="12" t="s">
-        <v>100</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:11">
       <c r="A25" s="12" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="D25" s="12" t="s">
-        <v>101</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="D25" s="12"/>
       <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
+      <c r="F25" s="12" t="s">
+        <v>53</v>
+      </c>
       <c r="G25" s="12"/>
-      <c r="H25" s="12"/>
+      <c r="H25" s="12" t="s">
+        <v>53</v>
+      </c>
       <c r="I25" s="12" t="s">
-        <v>61</v>
+        <v>19</v>
       </c>
       <c r="J25" s="12" t="s">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="K25" s="12" t="s">
-        <v>101</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:11">
       <c r="A26" s="12" t="s">
-        <v>76</v>
+        <v>142</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="D26" s="18" t="s">
-        <v>70</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="D26" s="12"/>
       <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
+      <c r="F26" s="12" t="s">
+        <v>142</v>
+      </c>
       <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
+      <c r="H26" s="12" t="s">
+        <v>142</v>
+      </c>
       <c r="I26" s="12" t="s">
-        <v>72</v>
+        <v>19</v>
       </c>
       <c r="J26" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="K26" s="18" t="s">
-        <v>70</v>
+        <v>20</v>
+      </c>
+      <c r="K26" s="12" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="27" spans="1:11">
       <c r="A27" s="12" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>77</v>
+        <v>22</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="D27" s="12" t="s">
-        <v>102</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="D27" s="12"/>
       <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
+      <c r="F27" s="12" t="s">
+        <v>50</v>
+      </c>
       <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
+      <c r="H27" s="12" t="s">
+        <v>40</v>
+      </c>
       <c r="I27" s="12" t="s">
-        <v>61</v>
+        <v>19</v>
       </c>
       <c r="J27" s="12" t="s">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="K27" s="12" t="s">
-        <v>102</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="12" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>77</v>
+        <v>22</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="D28" s="12" t="s">
-        <v>103</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="D28" s="12"/>
       <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
+      <c r="F28" s="12" t="s">
+        <v>53</v>
+      </c>
       <c r="G28" s="12"/>
-      <c r="H28" s="12"/>
+      <c r="H28" s="12" t="s">
+        <v>53</v>
+      </c>
       <c r="I28" s="12" t="s">
-        <v>61</v>
+        <v>19</v>
       </c>
       <c r="J28" s="12" t="s">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="K28" s="12" t="s">
-        <v>103</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:11">
       <c r="A29" s="12" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>77</v>
+        <v>45</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="D29" s="12" t="s">
-        <v>104</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="D29" s="12"/>
       <c r="E29" s="12"/>
-      <c r="F29" s="12"/>
+      <c r="F29" s="12" t="s">
+        <v>46</v>
+      </c>
       <c r="G29" s="12"/>
       <c r="H29" s="12" t="s">
-        <v>94</v>
+        <v>40</v>
       </c>
       <c r="I29" s="12" t="s">
-        <v>72</v>
+        <v>19</v>
       </c>
       <c r="J29" s="12" t="s">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="K29" s="12" t="s">
-        <v>104</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:11">
       <c r="A30" s="12" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>77</v>
+        <v>45</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="D30" s="12" t="s">
-        <v>105</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="D30" s="12"/>
       <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
+      <c r="F30" s="12" t="s">
+        <v>48</v>
+      </c>
       <c r="G30" s="12"/>
       <c r="H30" s="12" t="s">
-        <v>94</v>
+        <v>40</v>
       </c>
       <c r="I30" s="12" t="s">
-        <v>72</v>
+        <v>19</v>
       </c>
       <c r="J30" s="12" t="s">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="K30" s="12" t="s">
-        <v>105</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31" spans="1:11">
       <c r="A31" s="12" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>77</v>
+        <v>45</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="D31" s="12" t="s">
-        <v>106</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="D31" s="12"/>
       <c r="E31" s="12"/>
-      <c r="F31" s="12"/>
+      <c r="F31" s="12" t="s">
+        <v>52</v>
+      </c>
       <c r="G31" s="12"/>
-      <c r="H31" s="12"/>
+      <c r="H31" s="12" t="s">
+        <v>40</v>
+      </c>
       <c r="I31" s="12" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="J31" s="12" t="s">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="K31" s="12" t="s">
-        <v>106</v>
+        <v>52</v>
       </c>
     </row>
     <row r="32" spans="1:11">
       <c r="A32" s="12" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>77</v>
+        <v>45</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="D32" s="12" t="s">
-        <v>107</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="D32" s="12"/>
       <c r="E32" s="12"/>
-      <c r="F32" s="12"/>
+      <c r="F32" s="12" t="s">
+        <v>53</v>
+      </c>
       <c r="G32" s="12"/>
-      <c r="H32" s="12"/>
+      <c r="H32" s="12" t="s">
+        <v>53</v>
+      </c>
       <c r="I32" s="12" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="J32" s="12" t="s">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="K32" s="12" t="s">
-        <v>107</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33" spans="1:11">
       <c r="A33" s="12" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>77</v>
+        <v>45</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="D33" s="12" t="s">
-        <v>108</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="D33" s="12"/>
       <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
+      <c r="F33" s="12" t="s">
+        <v>54</v>
+      </c>
       <c r="G33" s="12"/>
-      <c r="H33" s="12"/>
+      <c r="H33" s="12" t="s">
+        <v>53</v>
+      </c>
       <c r="I33" s="12" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="J33" s="12" t="s">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="K33" s="12" t="s">
-        <v>108</v>
+        <v>54</v>
       </c>
     </row>
     <row r="34" spans="1:11">
       <c r="A34" s="12" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>77</v>
+        <v>45</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>63</v>
+        <v>18</v>
       </c>
       <c r="D34" s="12"/>
       <c r="E34" s="12"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="H34" s="12"/>
+      <c r="F34" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="G34" s="12"/>
+      <c r="H34" s="12" t="s">
+        <v>53</v>
+      </c>
       <c r="I34" s="12" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="J34" s="12" t="s">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="K34" s="12" t="s">
-        <v>78</v>
+        <v>55</v>
       </c>
     </row>
     <row r="35" spans="1:11">
@@ -4487,10 +4541,10 @@
         <v>77</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="D35" s="12" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="E35" s="12"/>
       <c r="F35" s="12"/>
@@ -4503,7 +4557,7 @@
         <v>73</v>
       </c>
       <c r="K35" s="12" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
     </row>
     <row r="36" spans="1:11">
@@ -4514,77 +4568,81 @@
         <v>77</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="D36" s="12"/>
+        <v>65</v>
+      </c>
+      <c r="D36" s="12" t="s">
+        <v>113</v>
+      </c>
       <c r="E36" s="12"/>
       <c r="F36" s="18"/>
-      <c r="G36" s="12" t="s">
-        <v>79</v>
-      </c>
+      <c r="G36" s="12"/>
       <c r="H36" s="12"/>
       <c r="I36" s="12" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="J36" s="12" t="s">
         <v>73</v>
       </c>
       <c r="K36" s="12" t="s">
-        <v>79</v>
+        <v>113</v>
       </c>
     </row>
     <row r="37" spans="1:11">
       <c r="A37" s="12" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D37" s="12"/>
       <c r="E37" s="12"/>
-      <c r="F37" s="15"/>
-      <c r="G37" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="H37" s="12"/>
+      <c r="F37" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="G37" s="12"/>
+      <c r="H37" s="12" t="s">
+        <v>64</v>
+      </c>
       <c r="I37" s="12" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="J37" s="12" t="s">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="K37" s="15" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
     </row>
     <row r="38" spans="1:11">
       <c r="A38" s="12" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="D38" s="12" t="s">
-        <v>110</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="D38" s="12"/>
       <c r="E38" s="12"/>
-      <c r="F38" s="15"/>
+      <c r="F38" s="15" t="s">
+        <v>67</v>
+      </c>
       <c r="G38" s="12"/>
-      <c r="H38" s="12"/>
+      <c r="H38" s="12" t="s">
+        <v>64</v>
+      </c>
       <c r="I38" s="12" t="s">
         <v>61</v>
       </c>
       <c r="J38" s="12" t="s">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="K38" s="15" t="s">
-        <v>110</v>
+        <v>67</v>
       </c>
     </row>
     <row r="39" spans="1:11">
@@ -4595,14 +4653,14 @@
         <v>77</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="D39" s="12"/>
+        <v>63</v>
+      </c>
+      <c r="D39" s="12" t="s">
+        <v>205</v>
+      </c>
       <c r="E39" s="12"/>
       <c r="F39" s="15"/>
-      <c r="G39" s="12" t="s">
-        <v>81</v>
-      </c>
+      <c r="G39" s="12"/>
       <c r="H39" s="12"/>
       <c r="I39" s="12" t="s">
         <v>39</v>
@@ -4611,7 +4669,7 @@
         <v>73</v>
       </c>
       <c r="K39" s="15" t="s">
-        <v>81</v>
+        <v>205</v>
       </c>
     </row>
     <row r="40" spans="1:11">
@@ -4624,10 +4682,10 @@
       <c r="C40" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="D40" s="12"/>
-      <c r="E40" s="12" t="s">
-        <v>118</v>
-      </c>
+      <c r="D40" s="12" t="s">
+        <v>207</v>
+      </c>
+      <c r="E40" s="12"/>
       <c r="F40" s="15"/>
       <c r="G40" s="12"/>
       <c r="H40" s="12"/>
@@ -4638,7 +4696,7 @@
         <v>73</v>
       </c>
       <c r="K40" s="12" t="s">
-        <v>118</v>
+        <v>207</v>
       </c>
     </row>
     <row r="41" spans="1:11">
@@ -4649,23 +4707,23 @@
         <v>77</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D41" s="12" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="E41" s="12"/>
       <c r="F41" s="15"/>
       <c r="G41" s="12"/>
       <c r="H41" s="12"/>
       <c r="I41" s="12" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="J41" s="12" t="s">
         <v>73</v>
       </c>
       <c r="K41" s="12" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
     </row>
     <row r="42" spans="1:11">
@@ -4679,7 +4737,7 @@
         <v>63</v>
       </c>
       <c r="D42" s="12" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="E42" s="12"/>
       <c r="F42" s="15"/>
@@ -4692,7 +4750,7 @@
         <v>73</v>
       </c>
       <c r="K42" s="12" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="43" spans="1:11">
@@ -4703,23 +4761,23 @@
         <v>77</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="D43" s="12" t="s">
-        <v>113</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="D43" s="12"/>
       <c r="E43" s="12"/>
       <c r="F43" s="15"/>
-      <c r="G43" s="12"/>
+      <c r="G43" s="12" t="s">
+        <v>78</v>
+      </c>
       <c r="H43" s="12"/>
       <c r="I43" s="12" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="J43" s="12" t="s">
         <v>73</v>
       </c>
       <c r="K43" s="12" t="s">
-        <v>113</v>
+        <v>78</v>
       </c>
     </row>
     <row r="44" spans="1:11">
@@ -4730,23 +4788,23 @@
         <v>77</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="D44" s="12" t="s">
-        <v>114</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="D44" s="12"/>
       <c r="E44" s="12"/>
       <c r="F44" s="15"/>
-      <c r="G44" s="12"/>
+      <c r="G44" s="12" t="s">
+        <v>79</v>
+      </c>
       <c r="H44" s="12"/>
       <c r="I44" s="12" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="J44" s="12" t="s">
         <v>73</v>
       </c>
       <c r="K44" s="12" t="s">
-        <v>114</v>
+        <v>79</v>
       </c>
     </row>
     <row r="45" spans="1:11">
@@ -4757,23 +4815,23 @@
         <v>77</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="D45" s="12" t="s">
-        <v>115</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="D45" s="12"/>
       <c r="E45" s="12"/>
-      <c r="F45" s="12"/>
-      <c r="G45" s="12"/>
+      <c r="F45" s="18"/>
+      <c r="G45" s="12" t="s">
+        <v>80</v>
+      </c>
       <c r="H45" s="12"/>
       <c r="I45" s="12" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="J45" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="K45" s="12" t="s">
-        <v>115</v>
+      <c r="K45" s="18" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="46" spans="1:11">
@@ -4787,11 +4845,11 @@
         <v>63</v>
       </c>
       <c r="D46" s="12"/>
-      <c r="E46" s="12"/>
+      <c r="E46" s="12" t="s">
+        <v>118</v>
+      </c>
       <c r="F46" s="18"/>
-      <c r="G46" s="12" t="s">
-        <v>82</v>
-      </c>
+      <c r="G46" s="12"/>
       <c r="H46" s="12"/>
       <c r="I46" s="12" t="s">
         <v>39</v>
@@ -4800,7 +4858,7 @@
         <v>73</v>
       </c>
       <c r="K46" s="12" t="s">
-        <v>82</v>
+        <v>118</v>
       </c>
     </row>
     <row r="47" spans="1:11">
@@ -4811,333 +4869,321 @@
         <v>77</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D47" s="12" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E47" s="12"/>
-      <c r="F47" s="12"/>
+      <c r="F47" s="18"/>
       <c r="G47" s="12"/>
       <c r="H47" s="12"/>
       <c r="I47" s="12" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="J47" s="12" t="s">
         <v>73</v>
       </c>
       <c r="K47" s="12" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="48" spans="1:11">
       <c r="A48" s="12" t="s">
-        <v>16</v>
+        <v>76</v>
       </c>
       <c r="B48" s="12" t="s">
-        <v>17</v>
+        <v>77</v>
       </c>
       <c r="C48" s="12" t="s">
-        <v>18</v>
+        <v>63</v>
       </c>
       <c r="D48" s="12"/>
       <c r="E48" s="12"/>
-      <c r="F48" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="G48" s="14"/>
-      <c r="H48" s="12" t="s">
-        <v>16</v>
-      </c>
+      <c r="F48" s="18"/>
+      <c r="G48" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="H48" s="12"/>
       <c r="I48" s="12" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="J48" s="12" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="K48" s="12" t="s">
-        <v>16</v>
+        <v>82</v>
       </c>
     </row>
     <row r="49" spans="1:11">
       <c r="A49" s="12" t="s">
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="B49" s="12" t="s">
         <v>17</v>
       </c>
       <c r="C49" s="12" t="s">
-        <v>23</v>
+        <v>63</v>
       </c>
       <c r="D49" s="12"/>
       <c r="E49" s="12"/>
-      <c r="F49" s="12" t="s">
-        <v>29</v>
+      <c r="F49" s="18" t="s">
+        <v>62</v>
       </c>
       <c r="G49" s="12"/>
       <c r="H49" s="12" t="s">
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="I49" s="12" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="J49" s="12" t="s">
         <v>20</v>
       </c>
       <c r="K49" s="12" t="s">
-        <v>29</v>
+        <v>62</v>
       </c>
     </row>
     <row r="50" spans="1:11">
       <c r="A50" s="12" t="s">
-        <v>21</v>
+        <v>75</v>
       </c>
       <c r="B50" s="12" t="s">
         <v>17</v>
       </c>
       <c r="C50" s="12" t="s">
-        <v>23</v>
+        <v>63</v>
       </c>
       <c r="D50" s="12"/>
       <c r="E50" s="12"/>
-      <c r="F50" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="G50" s="12"/>
+      <c r="F50" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="G50" s="14"/>
       <c r="H50" s="12" t="s">
-        <v>21</v>
+        <v>75</v>
       </c>
       <c r="I50" s="12" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="J50" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="K50" s="12" t="s">
-        <v>32</v>
+      <c r="K50" s="18" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="51" spans="1:11">
       <c r="A51" s="12" t="s">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="B51" s="12" t="s">
         <v>17</v>
       </c>
       <c r="C51" s="12" t="s">
-        <v>23</v>
+        <v>63</v>
       </c>
       <c r="D51" s="12"/>
       <c r="E51" s="12"/>
       <c r="F51" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="G51" s="14"/>
+        <v>121</v>
+      </c>
+      <c r="G51" s="12"/>
       <c r="H51" s="12" t="s">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="I51" s="12" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="J51" s="12" t="s">
         <v>20</v>
       </c>
       <c r="K51" s="12" t="s">
-        <v>33</v>
+        <v>121</v>
       </c>
     </row>
     <row r="52" spans="1:11">
       <c r="A52" s="12" t="s">
-        <v>21</v>
+        <v>133</v>
       </c>
       <c r="B52" s="12" t="s">
         <v>17</v>
       </c>
       <c r="C52" s="12" t="s">
-        <v>23</v>
+        <v>63</v>
       </c>
       <c r="D52" s="12"/>
       <c r="E52" s="12"/>
       <c r="F52" s="12" t="s">
-        <v>34</v>
+        <v>133</v>
       </c>
       <c r="G52" s="14"/>
       <c r="H52" s="12" t="s">
-        <v>21</v>
+        <v>133</v>
       </c>
       <c r="I52" s="12" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="J52" s="12" t="s">
         <v>20</v>
       </c>
       <c r="K52" s="12" t="s">
-        <v>34</v>
+        <v>133</v>
       </c>
     </row>
     <row r="53" spans="1:11">
       <c r="A53" s="12" t="s">
-        <v>21</v>
+        <v>150</v>
       </c>
       <c r="B53" s="12" t="s">
-        <v>17</v>
+        <v>151</v>
       </c>
       <c r="C53" s="12" t="s">
-        <v>23</v>
+        <v>63</v>
       </c>
       <c r="D53" s="12"/>
       <c r="E53" s="12"/>
-      <c r="F53" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="G53" s="14"/>
-      <c r="H53" s="12" t="s">
-        <v>21</v>
-      </c>
+      <c r="F53" s="18"/>
+      <c r="G53" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="H53" s="12"/>
       <c r="I53" s="12" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="J53" s="12" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="K53" s="12" t="s">
-        <v>35</v>
+        <v>152</v>
       </c>
     </row>
     <row r="54" spans="1:11">
       <c r="A54" s="12" t="s">
-        <v>36</v>
+        <v>150</v>
       </c>
       <c r="B54" s="12" t="s">
-        <v>17</v>
+        <v>151</v>
       </c>
       <c r="C54" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="D54" s="12"/>
+        <v>63</v>
+      </c>
+      <c r="D54" s="12" t="s">
+        <v>160</v>
+      </c>
       <c r="E54" s="12"/>
-      <c r="F54" s="12" t="s">
-        <v>38</v>
-      </c>
+      <c r="F54" s="12"/>
       <c r="G54" s="12"/>
-      <c r="H54" s="12" t="s">
-        <v>36</v>
-      </c>
+      <c r="H54" s="12"/>
       <c r="I54" s="12" t="s">
         <v>39</v>
       </c>
       <c r="J54" s="12" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="K54" s="12" t="s">
-        <v>38</v>
+        <v>160</v>
       </c>
     </row>
     <row r="55" spans="1:11">
       <c r="A55" s="12" t="s">
-        <v>40</v>
+        <v>150</v>
       </c>
       <c r="B55" s="12" t="s">
-        <v>17</v>
+        <v>151</v>
       </c>
       <c r="C55" s="12" t="s">
-        <v>18</v>
+        <v>63</v>
       </c>
       <c r="D55" s="12"/>
       <c r="E55" s="12"/>
-      <c r="F55" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="G55" s="14"/>
-      <c r="H55" s="12" t="s">
-        <v>40</v>
-      </c>
+      <c r="F55" s="12"/>
+      <c r="G55" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="H55" s="12"/>
       <c r="I55" s="12" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="J55" s="12" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="K55" s="12" t="s">
-        <v>41</v>
+        <v>153</v>
       </c>
     </row>
     <row r="56" spans="1:11">
       <c r="A56" s="12" t="s">
-        <v>40</v>
+        <v>150</v>
       </c>
       <c r="B56" s="12" t="s">
-        <v>17</v>
+        <v>151</v>
       </c>
       <c r="C56" s="12" t="s">
-        <v>18</v>
+        <v>63</v>
       </c>
       <c r="D56" s="12"/>
       <c r="E56" s="12"/>
-      <c r="F56" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="G56" s="12"/>
-      <c r="H56" s="12" t="s">
-        <v>40</v>
-      </c>
+      <c r="F56" s="12"/>
+      <c r="G56" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="H56" s="12"/>
       <c r="I56" s="12" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="J56" s="12" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="K56" s="12" t="s">
-        <v>42</v>
+        <v>154</v>
       </c>
     </row>
     <row r="57" spans="1:11">
       <c r="A57" s="12" t="s">
-        <v>40</v>
+        <v>150</v>
       </c>
       <c r="B57" s="12" t="s">
-        <v>17</v>
+        <v>151</v>
       </c>
       <c r="C57" s="12" t="s">
-        <v>18</v>
+        <v>63</v>
       </c>
       <c r="D57" s="12"/>
       <c r="E57" s="12"/>
-      <c r="F57" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="G57" s="12"/>
-      <c r="H57" s="12" t="s">
-        <v>40</v>
-      </c>
+      <c r="F57" s="12"/>
+      <c r="G57" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="H57" s="12"/>
       <c r="I57" s="12" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="J57" s="12" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="K57" s="12" t="s">
-        <v>43</v>
+        <v>155</v>
       </c>
     </row>
     <row r="58" spans="1:11">
       <c r="A58" s="12" t="s">
-        <v>40</v>
+        <v>121</v>
       </c>
       <c r="B58" s="12" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="C58" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D58" s="18"/>
+        <v>63</v>
+      </c>
+      <c r="D58" s="12"/>
       <c r="E58" s="12"/>
       <c r="F58" s="12" t="s">
-        <v>44</v>
+        <v>121</v>
       </c>
       <c r="G58" s="12"/>
       <c r="H58" s="12" t="s">
-        <v>40</v>
+        <v>121</v>
       </c>
       <c r="I58" s="12" t="s">
         <v>19</v>
@@ -5145,28 +5191,28 @@
       <c r="J58" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="K58" s="18" t="s">
-        <v>44</v>
+      <c r="K58" s="12" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="59" spans="1:11">
       <c r="A59" s="12" t="s">
-        <v>40</v>
+        <v>121</v>
       </c>
       <c r="B59" s="12" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="C59" s="12" t="s">
-        <v>18</v>
+        <v>63</v>
       </c>
       <c r="D59" s="12"/>
       <c r="E59" s="12"/>
       <c r="F59" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="G59" s="14"/>
+        <v>122</v>
+      </c>
+      <c r="G59" s="12"/>
       <c r="H59" s="12" t="s">
-        <v>40</v>
+        <v>121</v>
       </c>
       <c r="I59" s="12" t="s">
         <v>19</v>
@@ -5175,27 +5221,27 @@
         <v>20</v>
       </c>
       <c r="K59" s="12" t="s">
-        <v>47</v>
+        <v>122</v>
       </c>
     </row>
     <row r="60" spans="1:11">
       <c r="A60" s="12" t="s">
-        <v>40</v>
+        <v>133</v>
       </c>
       <c r="B60" s="12" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="C60" s="12" t="s">
-        <v>18</v>
+        <v>63</v>
       </c>
       <c r="D60" s="12"/>
       <c r="E60" s="12"/>
       <c r="F60" s="12" t="s">
-        <v>49</v>
+        <v>134</v>
       </c>
       <c r="G60" s="12"/>
       <c r="H60" s="12" t="s">
-        <v>40</v>
+        <v>133</v>
       </c>
       <c r="I60" s="12" t="s">
         <v>19</v>
@@ -5204,297 +5250,285 @@
         <v>20</v>
       </c>
       <c r="K60" s="12" t="s">
-        <v>49</v>
+        <v>134</v>
       </c>
     </row>
     <row r="61" spans="1:11">
       <c r="A61" s="12" t="s">
-        <v>40</v>
+        <v>76</v>
       </c>
       <c r="B61" s="12" t="s">
-        <v>17</v>
+        <v>77</v>
       </c>
       <c r="C61" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D61" s="12"/>
+        <v>70</v>
+      </c>
+      <c r="D61" s="12" t="s">
+        <v>88</v>
+      </c>
       <c r="E61" s="12"/>
-      <c r="F61" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="G61" s="12"/>
-      <c r="H61" s="12" t="s">
-        <v>40</v>
-      </c>
+      <c r="F61" s="12"/>
+      <c r="G61" s="14"/>
+      <c r="H61" s="12"/>
       <c r="I61" s="12" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
       <c r="J61" s="12" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="K61" s="12" t="s">
-        <v>51</v>
+        <v>88</v>
       </c>
     </row>
     <row r="62" spans="1:11">
       <c r="A62" s="12" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="B62" s="12" t="s">
-        <v>17</v>
+        <v>77</v>
       </c>
       <c r="C62" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D62" s="12"/>
+        <v>70</v>
+      </c>
+      <c r="D62" s="12" t="s">
+        <v>90</v>
+      </c>
       <c r="E62" s="12"/>
-      <c r="F62" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="G62" s="12"/>
-      <c r="H62" s="12" t="s">
-        <v>53</v>
-      </c>
+      <c r="F62" s="12"/>
+      <c r="G62" s="14"/>
+      <c r="H62" s="12"/>
       <c r="I62" s="12" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
       <c r="J62" s="12" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="K62" s="12" t="s">
-        <v>53</v>
+        <v>90</v>
       </c>
     </row>
     <row r="63" spans="1:11">
       <c r="A63" s="12" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
       <c r="B63" s="12" t="s">
-        <v>17</v>
+        <v>77</v>
       </c>
       <c r="C63" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D63" s="12"/>
+        <v>70</v>
+      </c>
+      <c r="D63" s="12" t="s">
+        <v>91</v>
+      </c>
       <c r="E63" s="12"/>
-      <c r="F63" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="G63" s="12"/>
-      <c r="H63" s="12" t="s">
-        <v>56</v>
-      </c>
+      <c r="F63" s="12"/>
+      <c r="G63" s="14"/>
+      <c r="H63" s="12"/>
       <c r="I63" s="12" t="s">
-        <v>39</v>
+        <v>72</v>
       </c>
       <c r="J63" s="12" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="K63" s="12" t="s">
-        <v>57</v>
+        <v>91</v>
       </c>
     </row>
     <row r="64" spans="1:11">
       <c r="A64" s="12" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="B64" s="12" t="s">
-        <v>17</v>
+        <v>77</v>
       </c>
       <c r="C64" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="D64" s="16"/>
+        <v>70</v>
+      </c>
+      <c r="D64" s="16" t="s">
+        <v>93</v>
+      </c>
       <c r="E64" s="12"/>
-      <c r="F64" s="18" t="s">
-        <v>58</v>
-      </c>
+      <c r="F64" s="18"/>
       <c r="G64" s="12"/>
       <c r="H64" s="12" t="s">
-        <v>58</v>
+        <v>94</v>
       </c>
       <c r="I64" s="12" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="J64" s="12" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="K64" s="16" t="s">
-        <v>58</v>
+        <v>93</v>
       </c>
     </row>
     <row r="65" spans="1:11">
       <c r="A65" s="12" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="B65" s="12" t="s">
-        <v>17</v>
+        <v>77</v>
       </c>
       <c r="C65" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="D65" s="12"/>
+        <v>70</v>
+      </c>
+      <c r="D65" s="12" t="s">
+        <v>206</v>
+      </c>
       <c r="E65" s="12"/>
-      <c r="F65" s="18" t="s">
-        <v>62</v>
-      </c>
+      <c r="F65" s="12"/>
       <c r="G65" s="12"/>
-      <c r="H65" s="12" t="s">
-        <v>62</v>
-      </c>
+      <c r="H65" s="12"/>
       <c r="I65" s="12" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
       <c r="J65" s="12" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="K65" s="12" t="s">
-        <v>62</v>
+        <v>206</v>
       </c>
     </row>
     <row r="66" spans="1:11">
       <c r="A66" s="12" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="B66" s="12" t="s">
-        <v>17</v>
+        <v>77</v>
       </c>
       <c r="C66" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="D66" s="12"/>
+        <v>70</v>
+      </c>
+      <c r="D66" s="18" t="s">
+        <v>70</v>
+      </c>
       <c r="E66" s="12"/>
-      <c r="F66" s="12" t="s">
-        <v>66</v>
-      </c>
+      <c r="F66" s="12"/>
       <c r="G66" s="12"/>
-      <c r="H66" s="12" t="s">
-        <v>64</v>
-      </c>
+      <c r="H66" s="12"/>
       <c r="I66" s="12" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="J66" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="K66" s="12" t="s">
-        <v>66</v>
+        <v>73</v>
+      </c>
+      <c r="K66" s="18" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="67" spans="1:11">
       <c r="A67" s="12" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="B67" s="12" t="s">
-        <v>17</v>
+        <v>77</v>
       </c>
       <c r="C67" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="D67" s="12"/>
+        <v>70</v>
+      </c>
+      <c r="D67" s="12" t="s">
+        <v>104</v>
+      </c>
       <c r="E67" s="12"/>
-      <c r="F67" s="12" t="s">
-        <v>67</v>
-      </c>
+      <c r="F67" s="12"/>
       <c r="G67" s="12"/>
       <c r="H67" s="12" t="s">
-        <v>64</v>
+        <v>94</v>
       </c>
       <c r="I67" s="12" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="J67" s="12" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="K67" s="12" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
     </row>
     <row r="68" spans="1:11">
       <c r="A68" s="12" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B68" s="12" t="s">
-        <v>17</v>
+        <v>77</v>
       </c>
       <c r="C68" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="D68" s="12"/>
+        <v>70</v>
+      </c>
+      <c r="D68" s="12" t="s">
+        <v>105</v>
+      </c>
       <c r="E68" s="12"/>
-      <c r="F68" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="G68" s="14"/>
+      <c r="F68" s="12"/>
+      <c r="G68" s="12"/>
       <c r="H68" s="12" t="s">
-        <v>75</v>
+        <v>94</v>
       </c>
       <c r="I68" s="12" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
       <c r="J68" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="K68" s="18" t="s">
-        <v>75</v>
+        <v>73</v>
+      </c>
+      <c r="K68" s="12" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="69" spans="1:11">
       <c r="A69" s="12" t="s">
-        <v>119</v>
+        <v>76</v>
       </c>
       <c r="B69" s="12" t="s">
-        <v>17</v>
+        <v>77</v>
       </c>
       <c r="C69" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D69" s="12"/>
+        <v>70</v>
+      </c>
+      <c r="D69" s="12" t="s">
+        <v>107</v>
+      </c>
       <c r="E69" s="12"/>
-      <c r="F69" s="12" t="s">
-        <v>120</v>
-      </c>
+      <c r="F69" s="12"/>
       <c r="G69" s="12"/>
-      <c r="H69" s="12" t="s">
-        <v>119</v>
-      </c>
+      <c r="H69" s="12"/>
       <c r="I69" s="12" t="s">
         <v>39</v>
       </c>
       <c r="J69" s="12" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="K69" s="12" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
     </row>
     <row r="70" spans="1:11">
       <c r="A70" s="12" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="B70" s="12" t="s">
         <v>17</v>
       </c>
       <c r="C70" s="12" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="D70" s="12"/>
       <c r="E70" s="12"/>
-      <c r="F70" s="12" t="s">
-        <v>121</v>
+      <c r="F70" s="18" t="s">
+        <v>128</v>
       </c>
       <c r="G70" s="12"/>
       <c r="H70" s="12" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="I70" s="12" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
       <c r="J70" s="12" t="s">
         <v>20</v>
       </c>
       <c r="K70" s="12" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
     </row>
     <row r="71" spans="1:11">
@@ -5509,8 +5543,8 @@
       </c>
       <c r="D71" s="12"/>
       <c r="E71" s="12"/>
-      <c r="F71" s="18" t="s">
-        <v>128</v>
+      <c r="F71" s="12" t="s">
+        <v>129</v>
       </c>
       <c r="G71" s="12"/>
       <c r="H71" s="12" t="s">
@@ -5523,7 +5557,7 @@
         <v>20</v>
       </c>
       <c r="K71" s="12" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="72" spans="1:11">
@@ -5539,7 +5573,7 @@
       <c r="D72" s="12"/>
       <c r="E72" s="12"/>
       <c r="F72" s="12" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="G72" s="12"/>
       <c r="H72" s="12" t="s">
@@ -5552,7 +5586,7 @@
         <v>20</v>
       </c>
       <c r="K72" s="12" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="73" spans="1:11">
@@ -5568,7 +5602,7 @@
       <c r="D73" s="12"/>
       <c r="E73" s="12"/>
       <c r="F73" s="12" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="G73" s="12"/>
       <c r="H73" s="12" t="s">
@@ -5581,12 +5615,12 @@
         <v>20</v>
       </c>
       <c r="K73" s="12" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="74" spans="1:11">
       <c r="A74" s="12" t="s">
-        <v>127</v>
+        <v>204</v>
       </c>
       <c r="B74" s="12" t="s">
         <v>17</v>
@@ -5596,12 +5630,12 @@
       </c>
       <c r="D74" s="12"/>
       <c r="E74" s="12"/>
-      <c r="F74" s="12" t="s">
-        <v>132</v>
+      <c r="F74" s="18" t="s">
+        <v>140</v>
       </c>
       <c r="G74" s="12"/>
       <c r="H74" s="12" t="s">
-        <v>127</v>
+        <v>138</v>
       </c>
       <c r="I74" s="12" t="s">
         <v>72</v>
@@ -5610,41 +5644,41 @@
         <v>20</v>
       </c>
       <c r="K74" s="12" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
     </row>
     <row r="75" spans="1:11">
       <c r="A75" s="12" t="s">
-        <v>133</v>
+        <v>162</v>
       </c>
       <c r="B75" s="12" t="s">
         <v>17</v>
       </c>
       <c r="C75" s="12" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="D75" s="12"/>
       <c r="E75" s="12"/>
       <c r="F75" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="G75" s="14"/>
+        <v>163</v>
+      </c>
+      <c r="G75" s="12"/>
       <c r="H75" s="12" t="s">
-        <v>133</v>
+        <v>162</v>
       </c>
       <c r="I75" s="12" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
       <c r="J75" s="12" t="s">
         <v>20</v>
       </c>
       <c r="K75" s="12" t="s">
-        <v>133</v>
+        <v>163</v>
       </c>
     </row>
     <row r="76" spans="1:11">
       <c r="A76" s="12" t="s">
-        <v>204</v>
+        <v>162</v>
       </c>
       <c r="B76" s="12" t="s">
         <v>17</v>
@@ -5654,12 +5688,12 @@
       </c>
       <c r="D76" s="12"/>
       <c r="E76" s="12"/>
-      <c r="F76" s="18" t="s">
-        <v>140</v>
+      <c r="F76" s="12" t="s">
+        <v>164</v>
       </c>
       <c r="G76" s="12"/>
       <c r="H76" s="12" t="s">
-        <v>138</v>
+        <v>162</v>
       </c>
       <c r="I76" s="12" t="s">
         <v>72</v>
@@ -5668,36 +5702,36 @@
         <v>20</v>
       </c>
       <c r="K76" s="12" t="s">
-        <v>140</v>
+        <v>164</v>
       </c>
     </row>
     <row r="77" spans="1:11">
       <c r="A77" s="12" t="s">
-        <v>142</v>
+        <v>162</v>
       </c>
       <c r="B77" s="12" t="s">
         <v>17</v>
       </c>
       <c r="C77" s="12" t="s">
-        <v>18</v>
+        <v>70</v>
       </c>
       <c r="D77" s="12"/>
       <c r="E77" s="12"/>
       <c r="F77" s="12" t="s">
-        <v>142</v>
+        <v>165</v>
       </c>
       <c r="G77" s="12"/>
       <c r="H77" s="12" t="s">
-        <v>142</v>
+        <v>162</v>
       </c>
       <c r="I77" s="12" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
       <c r="J77" s="12" t="s">
         <v>20</v>
       </c>
       <c r="K77" s="12" t="s">
-        <v>142</v>
+        <v>165</v>
       </c>
     </row>
     <row r="78" spans="1:11">
@@ -5713,7 +5747,7 @@
       <c r="D78" s="12"/>
       <c r="E78" s="12"/>
       <c r="F78" s="12" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="G78" s="12"/>
       <c r="H78" s="12" t="s">
@@ -5726,73 +5760,69 @@
         <v>20</v>
       </c>
       <c r="K78" s="12" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
     </row>
     <row r="79" spans="1:11">
       <c r="A79" s="12" t="s">
-        <v>162</v>
+        <v>68</v>
       </c>
       <c r="B79" s="12" t="s">
-        <v>17</v>
+        <v>69</v>
       </c>
       <c r="C79" s="12" t="s">
         <v>70</v>
       </c>
       <c r="D79" s="12"/>
       <c r="E79" s="12"/>
-      <c r="F79" s="12" t="s">
-        <v>164</v>
+      <c r="F79" s="18" t="s">
+        <v>71</v>
       </c>
       <c r="G79" s="12"/>
-      <c r="H79" s="12" t="s">
-        <v>162</v>
-      </c>
+      <c r="H79" s="12"/>
       <c r="I79" s="12" t="s">
         <v>72</v>
       </c>
       <c r="J79" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="K79" s="12" t="s">
-        <v>164</v>
+        <v>73</v>
+      </c>
+      <c r="K79" s="18" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="80" spans="1:11">
       <c r="A80" s="12" t="s">
-        <v>162</v>
+        <v>68</v>
       </c>
       <c r="B80" s="12" t="s">
-        <v>17</v>
+        <v>69</v>
       </c>
       <c r="C80" s="12" t="s">
         <v>70</v>
       </c>
       <c r="D80" s="12"/>
       <c r="E80" s="12"/>
-      <c r="F80" s="12" t="s">
-        <v>165</v>
+      <c r="F80" s="18" t="s">
+        <v>74</v>
       </c>
       <c r="G80" s="12"/>
-      <c r="H80" s="12" t="s">
-        <v>162</v>
-      </c>
+      <c r="H80" s="12"/>
       <c r="I80" s="12" t="s">
         <v>72</v>
       </c>
       <c r="J80" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="K80" s="12" t="s">
-        <v>165</v>
+        <v>73</v>
+      </c>
+      <c r="K80" s="18" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="81" spans="1:11">
       <c r="A81" s="12" t="s">
-        <v>162</v>
+        <v>107</v>
       </c>
       <c r="B81" s="12" t="s">
-        <v>17</v>
+        <v>123</v>
       </c>
       <c r="C81" s="12" t="s">
         <v>70</v>
@@ -5800,36 +5830,34 @@
       <c r="D81" s="12"/>
       <c r="E81" s="12"/>
       <c r="F81" s="12" t="s">
-        <v>166</v>
+        <v>124</v>
       </c>
       <c r="G81" s="12"/>
-      <c r="H81" s="12" t="s">
-        <v>162</v>
-      </c>
+      <c r="H81" s="12"/>
       <c r="I81" s="12" t="s">
         <v>72</v>
       </c>
       <c r="J81" s="12" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="K81" s="12" t="s">
-        <v>166</v>
+        <v>124</v>
       </c>
     </row>
     <row r="82" spans="1:11">
       <c r="A82" s="12" t="s">
-        <v>68</v>
+        <v>107</v>
       </c>
       <c r="B82" s="12" t="s">
-        <v>69</v>
+        <v>123</v>
       </c>
       <c r="C82" s="12" t="s">
         <v>70</v>
       </c>
       <c r="D82" s="12"/>
       <c r="E82" s="12"/>
-      <c r="F82" s="18" t="s">
-        <v>71</v>
+      <c r="F82" s="12" t="s">
+        <v>125</v>
       </c>
       <c r="G82" s="12"/>
       <c r="H82" s="12"/>
@@ -5839,24 +5867,24 @@
       <c r="J82" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="K82" s="18" t="s">
-        <v>71</v>
+      <c r="K82" s="12" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="83" spans="1:11">
       <c r="A83" s="12" t="s">
-        <v>68</v>
+        <v>107</v>
       </c>
       <c r="B83" s="12" t="s">
-        <v>69</v>
+        <v>123</v>
       </c>
       <c r="C83" s="12" t="s">
         <v>70</v>
       </c>
       <c r="D83" s="12"/>
       <c r="E83" s="12"/>
-      <c r="F83" s="18" t="s">
-        <v>74</v>
+      <c r="F83" s="12" t="s">
+        <v>126</v>
       </c>
       <c r="G83" s="12"/>
       <c r="H83" s="12"/>
@@ -5866,16 +5894,16 @@
       <c r="J83" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="K83" s="18" t="s">
-        <v>74</v>
+      <c r="K83" s="12" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="84" spans="1:11">
       <c r="A84" s="12" t="s">
-        <v>107</v>
+        <v>204</v>
       </c>
       <c r="B84" s="12" t="s">
-        <v>123</v>
+        <v>30</v>
       </c>
       <c r="C84" s="12" t="s">
         <v>70</v>
@@ -5883,26 +5911,28 @@
       <c r="D84" s="12"/>
       <c r="E84" s="12"/>
       <c r="F84" s="12" t="s">
-        <v>124</v>
+        <v>139</v>
       </c>
       <c r="G84" s="12"/>
-      <c r="H84" s="12"/>
+      <c r="H84" s="12" t="s">
+        <v>138</v>
+      </c>
       <c r="I84" s="12" t="s">
         <v>72</v>
       </c>
       <c r="J84" s="12" t="s">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="K84" s="12" t="s">
-        <v>124</v>
+        <v>139</v>
       </c>
     </row>
     <row r="85" spans="1:11">
       <c r="A85" s="12" t="s">
-        <v>107</v>
+        <v>204</v>
       </c>
       <c r="B85" s="12" t="s">
-        <v>123</v>
+        <v>30</v>
       </c>
       <c r="C85" s="12" t="s">
         <v>70</v>
@@ -5910,26 +5940,28 @@
       <c r="D85" s="12"/>
       <c r="E85" s="12"/>
       <c r="F85" s="12" t="s">
-        <v>125</v>
+        <v>141</v>
       </c>
       <c r="G85" s="12"/>
-      <c r="H85" s="12"/>
+      <c r="H85" s="12" t="s">
+        <v>138</v>
+      </c>
       <c r="I85" s="12" t="s">
         <v>72</v>
       </c>
       <c r="J85" s="12" t="s">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="K85" s="12" t="s">
-        <v>125</v>
+        <v>141</v>
       </c>
     </row>
     <row r="86" spans="1:11">
       <c r="A86" s="12" t="s">
-        <v>107</v>
+        <v>127</v>
       </c>
       <c r="B86" s="12" t="s">
-        <v>123</v>
+        <v>45</v>
       </c>
       <c r="C86" s="12" t="s">
         <v>70</v>
@@ -5937,36 +5969,38 @@
       <c r="D86" s="12"/>
       <c r="E86" s="12"/>
       <c r="F86" s="12" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="G86" s="12"/>
-      <c r="H86" s="12"/>
+      <c r="H86" s="12" t="s">
+        <v>127</v>
+      </c>
       <c r="I86" s="12" t="s">
         <v>72</v>
       </c>
       <c r="J86" s="12" t="s">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="K86" s="12" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
     </row>
     <row r="87" spans="1:11">
       <c r="A87" s="12" t="s">
-        <v>150</v>
+        <v>76</v>
       </c>
       <c r="B87" s="12" t="s">
-        <v>151</v>
+        <v>77</v>
       </c>
       <c r="C87" s="12" t="s">
         <v>37</v>
       </c>
       <c r="D87" s="12" t="s">
-        <v>156</v>
+        <v>92</v>
       </c>
       <c r="E87" s="12"/>
       <c r="F87" s="12"/>
-      <c r="G87" s="12"/>
+      <c r="G87" s="14"/>
       <c r="H87" s="12"/>
       <c r="I87" s="12" t="s">
         <v>39</v>
@@ -5975,21 +6009,21 @@
         <v>73</v>
       </c>
       <c r="K87" s="12" t="s">
-        <v>156</v>
+        <v>92</v>
       </c>
     </row>
     <row r="88" spans="1:11">
       <c r="A88" s="12" t="s">
-        <v>150</v>
+        <v>76</v>
       </c>
       <c r="B88" s="12" t="s">
-        <v>151</v>
+        <v>77</v>
       </c>
       <c r="C88" s="12" t="s">
         <v>37</v>
       </c>
       <c r="D88" s="12" t="s">
-        <v>157</v>
+        <v>106</v>
       </c>
       <c r="E88" s="12"/>
       <c r="F88" s="12"/>
@@ -6002,34 +6036,36 @@
         <v>73</v>
       </c>
       <c r="K88" s="12" t="s">
-        <v>157</v>
+        <v>106</v>
       </c>
     </row>
     <row r="89" spans="1:11">
       <c r="A89" s="12" t="s">
-        <v>150</v>
+        <v>36</v>
       </c>
       <c r="B89" s="12" t="s">
-        <v>151</v>
+        <v>17</v>
       </c>
       <c r="C89" s="12" t="s">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="D89" s="12"/>
       <c r="E89" s="12"/>
-      <c r="F89" s="18"/>
-      <c r="G89" s="12" t="s">
-        <v>152</v>
-      </c>
-      <c r="H89" s="12"/>
+      <c r="F89" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="G89" s="12"/>
+      <c r="H89" s="12" t="s">
+        <v>36</v>
+      </c>
       <c r="I89" s="12" t="s">
         <v>39</v>
       </c>
       <c r="J89" s="12" t="s">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="K89" s="12" t="s">
-        <v>152</v>
+        <v>38</v>
       </c>
     </row>
     <row r="90" spans="1:11">
@@ -6043,7 +6079,7 @@
         <v>37</v>
       </c>
       <c r="D90" s="12" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E90" s="12"/>
       <c r="F90" s="12"/>
@@ -6056,7 +6092,7 @@
         <v>73</v>
       </c>
       <c r="K90" s="12" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="91" spans="1:11">
@@ -6070,7 +6106,7 @@
         <v>37</v>
       </c>
       <c r="D91" s="12" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E91" s="12"/>
       <c r="F91" s="12"/>
@@ -6083,7 +6119,7 @@
         <v>73</v>
       </c>
       <c r="K91" s="12" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="92" spans="1:11">
@@ -6094,10 +6130,10 @@
         <v>151</v>
       </c>
       <c r="C92" s="12" t="s">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="D92" s="12" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E92" s="12"/>
       <c r="F92" s="12"/>
@@ -6110,7 +6146,7 @@
         <v>73</v>
       </c>
       <c r="K92" s="12" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="93" spans="1:11">
@@ -6121,14 +6157,14 @@
         <v>151</v>
       </c>
       <c r="C93" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="D93" s="12"/>
+        <v>37</v>
+      </c>
+      <c r="D93" s="12" t="s">
+        <v>159</v>
+      </c>
       <c r="E93" s="12"/>
       <c r="F93" s="12"/>
-      <c r="G93" s="12" t="s">
-        <v>153</v>
-      </c>
+      <c r="G93" s="12"/>
       <c r="H93" s="12"/>
       <c r="I93" s="12" t="s">
         <v>39</v>
@@ -6137,7 +6173,7 @@
         <v>73</v>
       </c>
       <c r="K93" s="12" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
     </row>
     <row r="94" spans="1:11">
@@ -6169,20 +6205,20 @@
     </row>
     <row r="95" spans="1:11">
       <c r="A95" s="12" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="B95" s="12" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="C95" s="12" t="s">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="D95" s="12"/>
-      <c r="E95" s="12"/>
+      <c r="E95" s="12" t="s">
+        <v>147</v>
+      </c>
       <c r="F95" s="12"/>
-      <c r="G95" s="12" t="s">
-        <v>154</v>
-      </c>
+      <c r="G95" s="12"/>
       <c r="H95" s="12"/>
       <c r="I95" s="12" t="s">
         <v>39</v>
@@ -6191,25 +6227,25 @@
         <v>73</v>
       </c>
       <c r="K95" s="12" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
     </row>
     <row r="96" spans="1:11">
       <c r="A96" s="12" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="B96" s="12" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="C96" s="12" t="s">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="D96" s="12"/>
-      <c r="E96" s="12"/>
+      <c r="E96" s="12" t="s">
+        <v>148</v>
+      </c>
       <c r="F96" s="12"/>
-      <c r="G96" s="12" t="s">
-        <v>155</v>
-      </c>
+      <c r="G96" s="12"/>
       <c r="H96" s="12"/>
       <c r="I96" s="12" t="s">
         <v>39</v>
@@ -6218,7 +6254,7 @@
         <v>73</v>
       </c>
       <c r="K96" s="12" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
     </row>
     <row r="97" spans="1:11">
@@ -6233,7 +6269,7 @@
       </c>
       <c r="D97" s="12"/>
       <c r="E97" s="12" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F97" s="12"/>
       <c r="G97" s="12"/>
@@ -6245,7 +6281,7 @@
         <v>73</v>
       </c>
       <c r="K97" s="12" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="98" spans="1:11">
@@ -6258,10 +6294,10 @@
       <c r="C98" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D98" s="12"/>
-      <c r="E98" s="12" t="s">
-        <v>148</v>
-      </c>
+      <c r="D98" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="E98" s="12"/>
       <c r="F98" s="12"/>
       <c r="G98" s="12"/>
       <c r="H98" s="12"/>
@@ -6272,7 +6308,7 @@
         <v>73</v>
       </c>
       <c r="K98" s="12" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="99" spans="1:11">
@@ -6285,10 +6321,10 @@
       <c r="C99" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D99" s="12"/>
-      <c r="E99" s="12" t="s">
-        <v>149</v>
-      </c>
+      <c r="D99" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="E99" s="12"/>
       <c r="F99" s="12"/>
       <c r="G99" s="12"/>
       <c r="H99" s="12"/>
@@ -6299,670 +6335,634 @@
         <v>73</v>
       </c>
       <c r="K99" s="12" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="100" spans="1:11">
       <c r="A100" s="12" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="B100" s="12" t="s">
-        <v>144</v>
+        <v>22</v>
       </c>
       <c r="C100" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D100" s="12" t="s">
-        <v>145</v>
-      </c>
+      <c r="D100" s="12"/>
       <c r="E100" s="12"/>
-      <c r="F100" s="12"/>
+      <c r="F100" s="12" t="s">
+        <v>38</v>
+      </c>
       <c r="G100" s="12"/>
-      <c r="H100" s="12"/>
+      <c r="H100" s="12" t="s">
+        <v>36</v>
+      </c>
       <c r="I100" s="12" t="s">
         <v>39</v>
       </c>
       <c r="J100" s="12" t="s">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="K100" s="12" t="s">
-        <v>145</v>
+        <v>38</v>
       </c>
     </row>
     <row r="101" spans="1:11">
       <c r="A101" s="12" t="s">
-        <v>143</v>
+        <v>76</v>
       </c>
       <c r="B101" s="12" t="s">
-        <v>144</v>
+        <v>77</v>
       </c>
       <c r="C101" s="12" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="D101" s="12" t="s">
-        <v>146</v>
+        <v>83</v>
       </c>
       <c r="E101" s="12"/>
-      <c r="F101" s="12"/>
-      <c r="G101" s="12"/>
+      <c r="F101" s="18"/>
+      <c r="G101" s="14"/>
       <c r="H101" s="12"/>
-      <c r="I101" s="12" t="s">
-        <v>39</v>
+      <c r="I101" s="13" t="s">
+        <v>61</v>
       </c>
       <c r="J101" s="12" t="s">
         <v>73</v>
       </c>
       <c r="K101" s="12" t="s">
-        <v>146</v>
+        <v>83</v>
       </c>
     </row>
     <row r="102" spans="1:11">
       <c r="A102" s="12" t="s">
-        <v>21</v>
+        <v>76</v>
       </c>
       <c r="B102" s="12" t="s">
-        <v>22</v>
+        <v>77</v>
       </c>
       <c r="C102" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D102" s="12"/>
+        <v>59</v>
+      </c>
+      <c r="D102" s="12" t="s">
+        <v>84</v>
+      </c>
       <c r="E102" s="12"/>
-      <c r="F102" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="G102" s="12"/>
-      <c r="H102" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="I102" s="12" t="s">
-        <v>25</v>
+      <c r="F102" s="18"/>
+      <c r="G102" s="14"/>
+      <c r="H102" s="12"/>
+      <c r="I102" s="13" t="s">
+        <v>61</v>
       </c>
       <c r="J102" s="12" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="K102" s="12" t="s">
-        <v>24</v>
+        <v>84</v>
       </c>
     </row>
     <row r="103" spans="1:11">
       <c r="A103" s="12" t="s">
-        <v>21</v>
+        <v>76</v>
       </c>
       <c r="B103" s="12" t="s">
-        <v>22</v>
+        <v>77</v>
       </c>
       <c r="C103" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D103" s="12"/>
+        <v>59</v>
+      </c>
+      <c r="D103" s="12" t="s">
+        <v>85</v>
+      </c>
       <c r="E103" s="12"/>
-      <c r="F103" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="G103" s="12"/>
-      <c r="H103" s="12" t="s">
-        <v>21</v>
-      </c>
+      <c r="F103" s="18"/>
+      <c r="G103" s="14"/>
+      <c r="H103" s="12"/>
       <c r="I103" s="12" t="s">
-        <v>25</v>
+        <v>61</v>
       </c>
       <c r="J103" s="12" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="K103" s="12" t="s">
-        <v>26</v>
+        <v>85</v>
       </c>
     </row>
     <row r="104" spans="1:11">
       <c r="A104" s="12" t="s">
-        <v>21</v>
+        <v>76</v>
       </c>
       <c r="B104" s="12" t="s">
-        <v>22</v>
+        <v>77</v>
       </c>
       <c r="C104" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D104" s="12"/>
+        <v>59</v>
+      </c>
+      <c r="D104" s="12" t="s">
+        <v>86</v>
+      </c>
       <c r="E104" s="12"/>
-      <c r="F104" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="G104" s="12"/>
-      <c r="H104" s="12" t="s">
-        <v>21</v>
-      </c>
+      <c r="F104" s="18"/>
+      <c r="G104" s="14"/>
+      <c r="H104" s="12"/>
       <c r="I104" s="12" t="s">
-        <v>25</v>
+        <v>61</v>
       </c>
       <c r="J104" s="12" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="K104" s="12" t="s">
-        <v>27</v>
+        <v>86</v>
       </c>
     </row>
     <row r="105" spans="1:11">
       <c r="A105" s="12" t="s">
-        <v>21</v>
+        <v>76</v>
       </c>
       <c r="B105" s="12" t="s">
-        <v>22</v>
+        <v>77</v>
       </c>
       <c r="C105" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D105" s="12"/>
+        <v>59</v>
+      </c>
+      <c r="D105" s="12" t="s">
+        <v>89</v>
+      </c>
       <c r="E105" s="12"/>
-      <c r="F105" s="12" t="s">
-        <v>28</v>
-      </c>
+      <c r="F105" s="12"/>
       <c r="G105" s="12"/>
-      <c r="H105" s="12" t="s">
-        <v>21</v>
-      </c>
+      <c r="H105" s="12"/>
       <c r="I105" s="12" t="s">
-        <v>25</v>
+        <v>61</v>
       </c>
       <c r="J105" s="12" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="K105" s="12" t="s">
-        <v>28</v>
+        <v>89</v>
       </c>
     </row>
     <row r="106" spans="1:11">
       <c r="A106" s="12" t="s">
-        <v>36</v>
+        <v>76</v>
       </c>
       <c r="B106" s="12" t="s">
-        <v>22</v>
+        <v>77</v>
       </c>
       <c r="C106" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="D106" s="12"/>
+        <v>59</v>
+      </c>
+      <c r="D106" s="12" t="s">
+        <v>58</v>
+      </c>
       <c r="E106" s="12"/>
-      <c r="F106" s="12" t="s">
-        <v>38</v>
-      </c>
+      <c r="F106" s="18"/>
       <c r="G106" s="12"/>
-      <c r="H106" s="12" t="s">
-        <v>36</v>
-      </c>
+      <c r="H106" s="12"/>
       <c r="I106" s="12" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="J106" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="K106" s="12" t="s">
-        <v>38</v>
+        <v>73</v>
+      </c>
+      <c r="K106" s="18" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="107" spans="1:11">
       <c r="A107" s="12" t="s">
-        <v>40</v>
+        <v>76</v>
       </c>
       <c r="B107" s="12" t="s">
-        <v>22</v>
+        <v>77</v>
       </c>
       <c r="C107" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D107" s="12"/>
+        <v>59</v>
+      </c>
+      <c r="D107" s="12" t="s">
+        <v>95</v>
+      </c>
       <c r="E107" s="12"/>
-      <c r="F107" s="12" t="s">
-        <v>50</v>
-      </c>
+      <c r="F107" s="12"/>
       <c r="G107" s="12"/>
-      <c r="H107" s="12" t="s">
-        <v>40</v>
-      </c>
+      <c r="H107" s="12"/>
       <c r="I107" s="12" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="J107" s="12" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="K107" s="12" t="s">
-        <v>50</v>
+        <v>95</v>
       </c>
     </row>
     <row r="108" spans="1:11">
       <c r="A108" s="12" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="B108" s="12" t="s">
-        <v>22</v>
+        <v>77</v>
       </c>
       <c r="C108" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D108" s="12"/>
+        <v>59</v>
+      </c>
+      <c r="D108" s="12" t="s">
+        <v>97</v>
+      </c>
       <c r="E108" s="12"/>
-      <c r="F108" s="12" t="s">
-        <v>53</v>
-      </c>
+      <c r="F108" s="12"/>
       <c r="G108" s="12"/>
-      <c r="H108" s="12" t="s">
-        <v>53</v>
-      </c>
+      <c r="H108" s="12"/>
       <c r="I108" s="12" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="J108" s="12" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="K108" s="12" t="s">
-        <v>53</v>
+        <v>97</v>
       </c>
     </row>
     <row r="109" spans="1:11">
       <c r="A109" s="12" t="s">
-        <v>21</v>
+        <v>76</v>
       </c>
       <c r="B109" s="12" t="s">
-        <v>30</v>
+        <v>77</v>
       </c>
       <c r="C109" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D109" s="12"/>
+        <v>59</v>
+      </c>
+      <c r="D109" s="12" t="s">
+        <v>98</v>
+      </c>
       <c r="E109" s="12"/>
-      <c r="F109" s="12" t="s">
-        <v>31</v>
-      </c>
+      <c r="F109" s="12"/>
       <c r="G109" s="12"/>
-      <c r="H109" s="12" t="s">
-        <v>21</v>
-      </c>
+      <c r="H109" s="12"/>
       <c r="I109" s="12" t="s">
-        <v>25</v>
+        <v>61</v>
       </c>
       <c r="J109" s="12" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="K109" s="12" t="s">
-        <v>31</v>
+        <v>98</v>
       </c>
     </row>
     <row r="110" spans="1:11">
       <c r="A110" s="12" t="s">
-        <v>121</v>
+        <v>76</v>
       </c>
       <c r="B110" s="12" t="s">
-        <v>30</v>
+        <v>77</v>
       </c>
       <c r="C110" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="D110" s="12"/>
+        <v>59</v>
+      </c>
+      <c r="D110" s="18" t="s">
+        <v>99</v>
+      </c>
       <c r="E110" s="12"/>
-      <c r="F110" s="12" t="s">
-        <v>121</v>
-      </c>
+      <c r="F110" s="12"/>
       <c r="G110" s="12"/>
-      <c r="H110" s="12" t="s">
-        <v>121</v>
-      </c>
+      <c r="H110" s="12"/>
       <c r="I110" s="12" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="J110" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="K110" s="12" t="s">
-        <v>121</v>
+        <v>73</v>
+      </c>
+      <c r="K110" s="18" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="111" spans="1:11">
       <c r="A111" s="12" t="s">
-        <v>204</v>
+        <v>76</v>
       </c>
       <c r="B111" s="12" t="s">
-        <v>30</v>
+        <v>77</v>
       </c>
       <c r="C111" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="D111" s="12"/>
+        <v>59</v>
+      </c>
+      <c r="D111" s="12" t="s">
+        <v>101</v>
+      </c>
       <c r="E111" s="12"/>
-      <c r="F111" s="12" t="s">
-        <v>139</v>
-      </c>
+      <c r="F111" s="12"/>
       <c r="G111" s="12"/>
-      <c r="H111" s="12" t="s">
-        <v>138</v>
-      </c>
+      <c r="H111" s="12"/>
       <c r="I111" s="12" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="J111" s="12" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="K111" s="12" t="s">
-        <v>139</v>
+        <v>101</v>
       </c>
     </row>
     <row r="112" spans="1:11">
       <c r="A112" s="12" t="s">
-        <v>204</v>
+        <v>76</v>
       </c>
       <c r="B112" s="12" t="s">
-        <v>30</v>
+        <v>77</v>
       </c>
       <c r="C112" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="D112" s="12"/>
+        <v>59</v>
+      </c>
+      <c r="D112" s="12" t="s">
+        <v>102</v>
+      </c>
       <c r="E112" s="12"/>
-      <c r="F112" s="12" t="s">
-        <v>141</v>
-      </c>
+      <c r="F112" s="12"/>
       <c r="G112" s="12"/>
-      <c r="H112" s="12" t="s">
-        <v>138</v>
-      </c>
+      <c r="H112" s="12"/>
       <c r="I112" s="12" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="J112" s="12" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="K112" s="12" t="s">
-        <v>141</v>
+        <v>102</v>
       </c>
     </row>
     <row r="113" spans="1:11">
       <c r="A113" s="12" t="s">
-        <v>40</v>
+        <v>76</v>
       </c>
       <c r="B113" s="12" t="s">
-        <v>45</v>
+        <v>77</v>
       </c>
       <c r="C113" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D113" s="12"/>
+        <v>59</v>
+      </c>
+      <c r="D113" s="12" t="s">
+        <v>103</v>
+      </c>
       <c r="E113" s="12"/>
-      <c r="F113" s="12" t="s">
-        <v>46</v>
-      </c>
+      <c r="F113" s="12"/>
       <c r="G113" s="12"/>
-      <c r="H113" s="12" t="s">
-        <v>40</v>
-      </c>
+      <c r="H113" s="12"/>
       <c r="I113" s="12" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="J113" s="12" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="K113" s="12" t="s">
-        <v>46</v>
+        <v>103</v>
       </c>
     </row>
     <row r="114" spans="1:11">
       <c r="A114" s="12" t="s">
-        <v>40</v>
+        <v>76</v>
       </c>
       <c r="B114" s="12" t="s">
-        <v>45</v>
+        <v>77</v>
       </c>
       <c r="C114" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D114" s="12"/>
+        <v>59</v>
+      </c>
+      <c r="D114" s="12" t="s">
+        <v>109</v>
+      </c>
       <c r="E114" s="12"/>
-      <c r="F114" s="12" t="s">
-        <v>48</v>
-      </c>
+      <c r="F114" s="12"/>
       <c r="G114" s="12"/>
-      <c r="H114" s="12" t="s">
-        <v>40</v>
-      </c>
+      <c r="H114" s="12"/>
       <c r="I114" s="12" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="J114" s="12" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="K114" s="12" t="s">
-        <v>48</v>
+        <v>109</v>
       </c>
     </row>
     <row r="115" spans="1:11">
       <c r="A115" s="12" t="s">
-        <v>40</v>
+        <v>76</v>
       </c>
       <c r="B115" s="12" t="s">
-        <v>45</v>
+        <v>77</v>
       </c>
       <c r="C115" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D115" s="12"/>
+        <v>59</v>
+      </c>
+      <c r="D115" s="12" t="s">
+        <v>110</v>
+      </c>
       <c r="E115" s="12"/>
-      <c r="F115" s="12" t="s">
-        <v>52</v>
-      </c>
+      <c r="F115" s="18"/>
       <c r="G115" s="12"/>
-      <c r="H115" s="12" t="s">
-        <v>40</v>
-      </c>
+      <c r="H115" s="12"/>
       <c r="I115" s="12" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="J115" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="K115" s="12" t="s">
-        <v>52</v>
+        <v>73</v>
+      </c>
+      <c r="K115" s="18" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="116" spans="1:11">
       <c r="A116" s="12" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="B116" s="12" t="s">
-        <v>45</v>
+        <v>77</v>
       </c>
       <c r="C116" s="12" t="s">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="D116" s="12"/>
       <c r="E116" s="12"/>
-      <c r="F116" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="G116" s="12"/>
-      <c r="H116" s="12" t="s">
-        <v>53</v>
-      </c>
+      <c r="F116" s="18"/>
+      <c r="G116" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="H116" s="12"/>
       <c r="I116" s="12" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="J116" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="K116" s="12" t="s">
-        <v>53</v>
+        <v>73</v>
+      </c>
+      <c r="K116" s="18" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="117" spans="1:11">
       <c r="A117" s="12" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="B117" s="12" t="s">
-        <v>45</v>
+        <v>77</v>
       </c>
       <c r="C117" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D117" s="12"/>
+        <v>59</v>
+      </c>
+      <c r="D117" s="12" t="s">
+        <v>111</v>
+      </c>
       <c r="E117" s="12"/>
-      <c r="F117" s="12" t="s">
-        <v>54</v>
-      </c>
+      <c r="F117" s="18"/>
       <c r="G117" s="12"/>
-      <c r="H117" s="12" t="s">
-        <v>53</v>
-      </c>
+      <c r="H117" s="12"/>
       <c r="I117" s="12" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="J117" s="12" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="K117" s="12" t="s">
-        <v>54</v>
+        <v>111</v>
       </c>
     </row>
     <row r="118" spans="1:11">
       <c r="A118" s="12" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="B118" s="12" t="s">
-        <v>45</v>
+        <v>77</v>
       </c>
       <c r="C118" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D118" s="12"/>
+        <v>59</v>
+      </c>
+      <c r="D118" s="12" t="s">
+        <v>114</v>
+      </c>
       <c r="E118" s="12"/>
-      <c r="F118" s="12" t="s">
-        <v>55</v>
-      </c>
+      <c r="F118" s="18"/>
       <c r="G118" s="12"/>
-      <c r="H118" s="12" t="s">
-        <v>53</v>
-      </c>
+      <c r="H118" s="12"/>
       <c r="I118" s="12" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="J118" s="12" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="K118" s="12" t="s">
-        <v>55</v>
+        <v>114</v>
       </c>
     </row>
     <row r="119" spans="1:11">
       <c r="A119" s="12" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="B119" s="12" t="s">
-        <v>45</v>
+        <v>77</v>
       </c>
       <c r="C119" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="D119" s="12"/>
+      <c r="D119" s="12" t="s">
+        <v>115</v>
+      </c>
       <c r="E119" s="12"/>
-      <c r="F119" s="12" t="s">
-        <v>60</v>
-      </c>
+      <c r="F119" s="12"/>
       <c r="G119" s="12"/>
-      <c r="H119" s="12" t="s">
-        <v>58</v>
-      </c>
+      <c r="H119" s="12"/>
       <c r="I119" s="12" t="s">
         <v>61</v>
       </c>
       <c r="J119" s="12" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="K119" s="12" t="s">
-        <v>60</v>
+        <v>115</v>
       </c>
     </row>
     <row r="120" spans="1:11">
       <c r="A120" s="12" t="s">
-        <v>121</v>
+        <v>76</v>
       </c>
       <c r="B120" s="12" t="s">
-        <v>45</v>
+        <v>77</v>
       </c>
       <c r="C120" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="D120" s="12"/>
+        <v>59</v>
+      </c>
+      <c r="D120" s="12" t="s">
+        <v>116</v>
+      </c>
       <c r="E120" s="12"/>
-      <c r="F120" s="12" t="s">
-        <v>122</v>
-      </c>
+      <c r="F120" s="12"/>
       <c r="G120" s="12"/>
-      <c r="H120" s="12" t="s">
-        <v>121</v>
-      </c>
+      <c r="H120" s="12"/>
       <c r="I120" s="12" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="J120" s="12" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="K120" s="12" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="121" spans="1:11">
       <c r="A121" s="12" t="s">
-        <v>127</v>
+        <v>58</v>
       </c>
       <c r="B121" s="12" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="C121" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="D121" s="12"/>
+        <v>59</v>
+      </c>
+      <c r="D121" s="18"/>
       <c r="E121" s="12"/>
-      <c r="F121" s="12" t="s">
-        <v>130</v>
+      <c r="F121" s="18" t="s">
+        <v>58</v>
       </c>
       <c r="G121" s="12"/>
       <c r="H121" s="12" t="s">
-        <v>127</v>
+        <v>58</v>
       </c>
       <c r="I121" s="12" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="J121" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="K121" s="12" t="s">
-        <v>130</v>
+      <c r="K121" s="18" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="122" spans="1:11">
       <c r="A122" s="12" t="s">
-        <v>133</v>
+        <v>58</v>
       </c>
       <c r="B122" s="12" t="s">
         <v>45</v>
       </c>
       <c r="C122" s="12" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D122" s="12"/>
       <c r="E122" s="12"/>
       <c r="F122" s="12" t="s">
-        <v>134</v>
+        <v>60</v>
       </c>
       <c r="G122" s="12"/>
       <c r="H122" s="12" t="s">
-        <v>133</v>
+        <v>58</v>
       </c>
       <c r="I122" s="12" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="J122" s="12" t="s">
         <v>20</v>
       </c>
       <c r="K122" s="12" t="s">
-        <v>134</v>
+        <v>60</v>
       </c>
     </row>
     <row r="123" spans="1:11">
@@ -7026,7 +7026,7 @@
   </sheetData>
   <autoFilter ref="A1:K1">
     <sortState ref="A2:K124">
-      <sortCondition ref="B1:B124"/>
+      <sortCondition ref="C1:C124"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Change .js variable names, resize search input box
</commit_message>
<xml_diff>
--- a/_data/_data.xlsx
+++ b/_data/_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26330"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="0" windowWidth="30260" windowHeight="18980" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="600" yWindow="0" windowWidth="36320" windowHeight="19580" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="navigation" sheetId="4" r:id="rId1"/>
@@ -13,7 +13,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">navigation!$A$1:$F$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'planning-guides'!$A$1:$K$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'planning-guides'!$A$1:$L$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">programs!$A$1:$L$124</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1188" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1195" uniqueCount="215">
   <si>
     <t>label</t>
   </si>
@@ -650,6 +650,27 @@
   </si>
   <si>
     <t>exercise science and kinesiology</t>
+  </si>
+  <si>
+    <t>url</t>
+  </si>
+  <si>
+    <t>http://www.shoreline.edu/areas-of-study/planning-guides/2015-2016/prof-tech-planning-guides/accounting-aaas-cp.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/AUTO-General-Motors-ASEP-AAAS.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/AUTO-GST-CP.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/AUTO-Honda-PACT-AAAS.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/AUTO-MoparCAP-AAAS.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/AUTO-Toyota-T-TEN-AAAS.pdf</t>
   </si>
 </sst>
 </file>
@@ -3527,11 +3548,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K124"/>
+  <dimension ref="A1:L124"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K5" sqref="K5"/>
+      <selection pane="bottomLeft" activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3544,10 +3565,11 @@
     <col min="9" max="9" width="18" style="8" customWidth="1"/>
     <col min="10" max="10" width="12" style="8" customWidth="1"/>
     <col min="11" max="11" width="30" style="8" customWidth="1"/>
-    <col min="12" max="16384" width="10.83203125" style="8"/>
+    <col min="12" max="12" width="32.5" style="8" customWidth="1"/>
+    <col min="13" max="16384" width="10.83203125" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="9" customFormat="1">
+    <row r="1" spans="1:12" s="9" customFormat="1">
       <c r="A1" s="10" t="s">
         <v>5</v>
       </c>
@@ -3581,8 +3603,11 @@
       <c r="K1" s="11" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="L1" s="9" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" s="12" t="s">
         <v>16</v>
       </c>
@@ -3610,8 +3635,11 @@
       <c r="K2" s="12" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:11">
+      <c r="L2" s="8" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" s="12" t="s">
         <v>21</v>
       </c>
@@ -3639,8 +3667,11 @@
       <c r="K3" s="12" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="4" spans="1:11">
+      <c r="L3" s="8" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" s="12" t="s">
         <v>21</v>
       </c>
@@ -3669,7 +3700,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:12">
       <c r="A5" s="12" t="s">
         <v>21</v>
       </c>
@@ -3697,8 +3728,11 @@
       <c r="K5" s="12" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="6" spans="1:11">
+      <c r="L5" s="8" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" s="12" t="s">
         <v>21</v>
       </c>
@@ -3726,8 +3760,11 @@
       <c r="K6" s="12" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="7" spans="1:11">
+      <c r="L6" s="8" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" s="12" t="s">
         <v>21</v>
       </c>
@@ -3755,8 +3792,11 @@
       <c r="K7" s="12" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="8" spans="1:11">
+      <c r="L7" s="8" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" s="12" t="s">
         <v>21</v>
       </c>
@@ -3785,7 +3825,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:12">
       <c r="A9" s="12" t="s">
         <v>21</v>
       </c>
@@ -3814,7 +3854,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:12">
       <c r="A10" s="12" t="s">
         <v>21</v>
       </c>
@@ -3843,7 +3883,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:12">
       <c r="A11" s="12" t="s">
         <v>21</v>
       </c>
@@ -3872,7 +3912,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:12">
       <c r="A12" s="12" t="s">
         <v>21</v>
       </c>
@@ -3900,8 +3940,11 @@
       <c r="K12" s="12" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="13" spans="1:11">
+      <c r="L12" s="8" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" s="12" t="s">
         <v>36</v>
       </c>
@@ -3930,7 +3973,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:12">
       <c r="A14" s="12" t="s">
         <v>36</v>
       </c>
@@ -3959,7 +4002,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:12">
       <c r="A15" s="12" t="s">
         <v>40</v>
       </c>
@@ -3988,7 +4031,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:12">
       <c r="A16" s="12" t="s">
         <v>40</v>
       </c>
@@ -7024,11 +7067,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K1">
-    <sortState ref="A2:K124">
-      <sortCondition ref="A1:A124"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:L1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>

<commit_message>
Add University Transfer page
</commit_message>
<xml_diff>
--- a/_data/_data.xlsx
+++ b/_data/_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26330"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="0" windowWidth="36320" windowHeight="19580" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="-460" windowWidth="38400" windowHeight="21600" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="navigation" sheetId="4" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1195" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1309" uniqueCount="326">
   <si>
     <t>label</t>
   </si>
@@ -671,6 +671,339 @@
   </si>
   <si>
     <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/AUTO-Toyota-T-TEN-AAAS.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/AUTO-Brakes-Specialist.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/AUTO-Electrical-Specialist-CC.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/AUTO-Engine-Specialist-CC.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/BIOTECH-Biotechnology-Lab-Specialist-CC.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/BIOTECH-Biotechnology-Lab-Specialist-AAAS-AAST.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/BUS-Business-Technology-AAA-CP.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/BUS-Entrepreneurship-AAAS-CP.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/BUS-Fashion-Merchandising-AAAS-CP.pdf</t>
+  </si>
+  <si>
+    <t>http://www.shoreline.edu/areas-of-study/planning-guides/2015-2016/prof-tech-planning-guides/general-business-administration-aaas-cp.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/BUS-Marketing-AAAS-CP.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/BUS-Retail-Management-CC.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/BUS-Sports-and-Event-Marketing-AAAS-CP.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/BUS-Social-Media-Marketing-CC.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/BUS-International-Trade-CC.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/BUS-Project-Management-CC.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/BUS-Sustainable-Business-Leadership-CC.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/BUS-Microsoft-Software-Applications-CC.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/BUS-Office-Assistant-Receptionist-CC.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/CNRG-Clean-Energy-Technology-and-Entrpn-AAAS.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/CJ-Criminal-Justice-AAAS.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/CJ-CAST-CC.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/DENHY-Dental-Hygiene-AAAS-AAST.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/EDUC-Early-Childhood-Educator-Paraeducator-AAAS.pdf</t>
+  </si>
+  <si>
+    <t>http://www.shoreline.edu/areas-of-study/planning-guides/2015-2016/prof-tech-planning-guides/education-special-ed-aaas.pdf</t>
+  </si>
+  <si>
+    <t>http://www.shoreline.edu/areas-of-study/planning-guides/2015-2016/u-transfer-planning-guides/foundation-studio-art.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/Spec-AFA-Photography.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MPS-AA-Health-Informatics.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MPS-AA-Architectural-Studies.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/AA-DTA-Construction-Management-MRP.pdf</t>
+  </si>
+  <si>
+    <t>http://www.shoreline.edu/areas-of-study/planning-guides/2015-2016/u-transfer-planning-guides/business.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MPS-AA-Elementary-Education.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MPS-AA-Secondary-Education.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MPS-AA-Diagnostic-Ultrasound.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MPS-AA-Exercise-Science-Kinesiology.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MPS-AA-Nutrition-and-Food-Science.pdf</t>
+  </si>
+  <si>
+    <t>http://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MPS-AA-Occupational-Therapy.pdf</t>
+  </si>
+  <si>
+    <t>http://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MPS-AA-Physical-Therapy.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MPS-AA-Physician-Assistant.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/AA-Pre-Nursing-MRP.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MPS-AA-Public-and-Community-Health.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MPS-AA-Speech-and-Hearing-Sciences.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MPS-AA-Art-History.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MPS-AA-Cinema-Film-and-Media-Studies.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MPS-AA-Communication-Studies.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MPS-AA-Creative-Writing.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MPS-AA-Drama-Theatre%20Arts.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MPS-AA-Humanities.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MPS-AA-Journalism.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MPS-AA-English-Language-and-Literature.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MPS-AA-Music.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MPS-AA-ComputerScience.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MPS-AA-Mathematics-Applied-Math-Statistics.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MPS-AA-African-Studies.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MPS-AA-American-Ethnic-Studies.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MPS-AA-American-Studies.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MPS-AA-Anthropology.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MPS-AA-East-Asian-Studies.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/planning-guides/2015-2016/u-transfer-planning-guides/criminal-justice.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MPS-AA-Economics.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MPS-AA-Environmental-Studies.pdf</t>
+  </si>
+  <si>
+    <t>http://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MPS-AA-Gender-and-Womens-Studies.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MPS-AA-Geography.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MPS-AA-History.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MPS-AA-Informatics.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MPS-AA-International-Global-Studies.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MPS-AA-Philosophy.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MPS-AA-Political-Science.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MPS-AA-Pre-Law.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MPS-AA-Psychology.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MPS-AA-Social-Work-and-Human-Services.pdf</t>
+  </si>
+  <si>
+    <t>http://www.shoreline.edu/areas-of-study/planning-guides/2015-2016/u-transfer-planning-guides/sociology.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MPS-AA-World-Languages.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MFGT-Machinist-Technology-AAAS-CP.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MLT-Medical-Laboratory-Technology-AAAS-CP.pdf</t>
+  </si>
+  <si>
+    <t>http://www.shoreline.edu/areas-of-study/planning-guides/2015-2016/prof-tech-planning-guides/phlebotomy-cc.pdf</t>
+  </si>
+  <si>
+    <t>phlebotomy</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/DegreePlanningGuides/AM-IP%20Classical%20Piano.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/DegreePlanningGuides/AM-IP%20Classical%20Voice.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/DegreePlanningGuides/AM-IP%20Instrumental%20Music.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MUSTC-Digital-Audio-Engineering-AAAS.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MUSTC-Electronic-MIDI-Music-Production-AAAS.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MUSTC-Merchandising-AAAS.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MUSTC-Performance-AAAS.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MUSTC-Foundations-of-Electronic-Music-CC.pdf</t>
+  </si>
+  <si>
+    <t>http://www.shoreline.edu/areas-of-study/planning-guides/2015-2016/prof-tech-planning-guides/nursing-aaas-6-quarter.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/NAC-Nursing-Assistant-Certified-IBEST-CC.pdf</t>
+  </si>
+  <si>
+    <t>http://www.shoreline.edu/areas-of-study/planning-guides/2015-2016/prof-tech-planning-guides/parent-education-leadership-skills-cc.pdf</t>
+  </si>
+  <si>
+    <t>http://www.shoreline.edu/areas-of-study/planning-guides/2015-2016/prof-tech-planning-guides/parenting-education-parenting-skills-cc.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/PERF-Digital-Film-Production-AAAS.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/PERF-Acting-for-Stage-and-Camera-CP.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/PERF-Writing-and-Directing-for-Camera-CP.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/BUS-Purchasing-and-Supply-Chain-Management-AAAS-CP.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/AST2-Aero-Engineering-MRP.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/AST2-BioEngineering-MRP.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/AST2-Computer-and-Electrical-Engineering-MRP.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MPS-AST2-Engineering-General.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MPS-AST2-Physics.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MPS-AST1-Dentistry-Pathway.pdf</t>
+  </si>
+  <si>
+    <t>http://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MPS-AST1-Medical-Laboratory-Science-Pathway.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MPS-AST1-Medicine-Pathway.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MPS-AST1-Pharmacy-Pathway.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MPS-AST1-Veterinary-Medicine-Pathway.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MPS-AST1-Biological-Science.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MPS-AST1-Chemistry-Biochemistry.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MPS-AST1-Environmental-Sciences.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/DegreePlanningGuides/AST1-Degree-Planning-Guide.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MPS-AST1-Oceanography-and-Marine-Sciences.pdf</t>
+  </si>
+  <si>
+    <t>http://www.shoreline.edu/areas-of-study/planning-guides/2015-2016/prof-tech-planning-guides/animation-video-for-multimedia.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/VCT-Creative-Project-Management-AAAS-AAST.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/VCT-Game-Art-and-Design-AAAS-AAST.pdf</t>
+  </si>
+  <si>
+    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/VCT-Graphic-Design-AAAS-AAST.pdf</t>
   </si>
 </sst>
 </file>
@@ -782,7 +1115,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="63">
+  <cellStyleXfs count="283">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -845,6 +1178,226 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="20">
@@ -903,7 +1456,7 @@
       <alignment horizontal="right" vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="63">
+  <cellStyles count="283">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -944,6 +1497,116 @@
     <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="236" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="240" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="244" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="246" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="250" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="252" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="256" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="258" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="260" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="262" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="264" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="266" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="268" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="270" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="272" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="274" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="276" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="278" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="280" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="282" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -966,6 +1629,116 @@
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="225" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="227" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="235" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="237" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="239" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="241" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="243" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="245" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="247" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="249" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="251" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="253" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="255" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="257" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="259" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="261" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="263" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="265" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="267" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="269" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="271" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="273" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="275" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="277" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="279" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="281" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1233,7 +2006,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3550,9 +4323,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L124"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L20" sqref="L20"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L124" sqref="L124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3824,6 +4597,9 @@
       <c r="K8" s="12" t="s">
         <v>24</v>
       </c>
+      <c r="L8" s="8" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="12" t="s">
@@ -3882,6 +4658,9 @@
       <c r="K10" s="12" t="s">
         <v>27</v>
       </c>
+      <c r="L10" s="8" t="s">
+        <v>216</v>
+      </c>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="12" t="s">
@@ -3911,6 +4690,9 @@
       <c r="K11" s="12" t="s">
         <v>28</v>
       </c>
+      <c r="L11" s="8" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="12" t="s">
@@ -3972,6 +4754,9 @@
       <c r="K13" s="12" t="s">
         <v>38</v>
       </c>
+      <c r="L13" s="8" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="12" t="s">
@@ -4001,6 +4786,9 @@
       <c r="K14" s="12" t="s">
         <v>38</v>
       </c>
+      <c r="L14" s="8" t="s">
+        <v>218</v>
+      </c>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="12" t="s">
@@ -4059,8 +4847,11 @@
       <c r="K16" s="12" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="17" spans="1:11">
+      <c r="L16" s="8" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
       <c r="A17" s="12" t="s">
         <v>40</v>
       </c>
@@ -4088,8 +4879,11 @@
       <c r="K17" s="12" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" s="7" customFormat="1">
+      <c r="L17" s="8" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" s="7" customFormat="1">
       <c r="A18" s="12" t="s">
         <v>40</v>
       </c>
@@ -4117,8 +4911,11 @@
       <c r="K18" s="18" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="19" spans="1:11">
+      <c r="L18" s="8" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
       <c r="A19" s="12" t="s">
         <v>40</v>
       </c>
@@ -4146,8 +4943,11 @@
       <c r="K19" s="12" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="20" spans="1:11">
+      <c r="L19" s="8" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
       <c r="A20" s="12" t="s">
         <v>40</v>
       </c>
@@ -4175,8 +4975,11 @@
       <c r="K20" s="12" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="21" spans="1:11">
+      <c r="L20" s="8" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
       <c r="A21" s="12" t="s">
         <v>40</v>
       </c>
@@ -4204,8 +5007,11 @@
       <c r="K21" s="12" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="22" spans="1:11">
+      <c r="L21" s="8" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
       <c r="A22" s="12" t="s">
         <v>40</v>
       </c>
@@ -4233,8 +5039,11 @@
       <c r="K22" s="12" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="23" spans="1:11">
+      <c r="L22" s="8" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
       <c r="A23" s="12" t="s">
         <v>40</v>
       </c>
@@ -4262,8 +5071,11 @@
       <c r="K23" s="12" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="24" spans="1:11">
+      <c r="L23" s="8" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
       <c r="A24" s="12" t="s">
         <v>40</v>
       </c>
@@ -4291,8 +5103,11 @@
       <c r="K24" s="12" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="25" spans="1:11">
+      <c r="L24" s="8" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
       <c r="A25" s="12" t="s">
         <v>40</v>
       </c>
@@ -4320,8 +5135,11 @@
       <c r="K25" s="12" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="26" spans="1:11">
+      <c r="L25" s="8" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
       <c r="A26" s="12" t="s">
         <v>53</v>
       </c>
@@ -4349,8 +5167,11 @@
       <c r="K26" s="12" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="27" spans="1:11">
+      <c r="L26" s="8" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
       <c r="A27" s="12" t="s">
         <v>53</v>
       </c>
@@ -4378,8 +5199,11 @@
       <c r="K27" s="12" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="28" spans="1:11">
+      <c r="L27" s="8" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
       <c r="A28" s="12" t="s">
         <v>53</v>
       </c>
@@ -4407,8 +5231,11 @@
       <c r="K28" s="12" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="29" spans="1:11">
+      <c r="L28" s="8" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
       <c r="A29" s="12" t="s">
         <v>53</v>
       </c>
@@ -4436,8 +5263,11 @@
       <c r="K29" s="12" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="30" spans="1:11">
+      <c r="L29" s="8" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
       <c r="A30" s="12" t="s">
         <v>53</v>
       </c>
@@ -4465,8 +5295,11 @@
       <c r="K30" s="12" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="31" spans="1:11">
+      <c r="L30" s="8" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
       <c r="A31" s="12" t="s">
         <v>56</v>
       </c>
@@ -4494,8 +5327,11 @@
       <c r="K31" s="12" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="32" spans="1:11">
+      <c r="L31" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
       <c r="A32" s="12" t="s">
         <v>58</v>
       </c>
@@ -4523,8 +5359,11 @@
       <c r="K32" s="18" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="33" spans="1:11">
+      <c r="L32" s="8" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
       <c r="A33" s="12" t="s">
         <v>58</v>
       </c>
@@ -4552,8 +5391,11 @@
       <c r="K33" s="12" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="34" spans="1:11">
+      <c r="L33" s="8" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12">
       <c r="A34" s="12" t="s">
         <v>62</v>
       </c>
@@ -4581,8 +5423,11 @@
       <c r="K34" s="12" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="35" spans="1:11">
+      <c r="L34" s="8" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12">
       <c r="A35" s="12" t="s">
         <v>64</v>
       </c>
@@ -4610,8 +5455,11 @@
       <c r="K35" s="18" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="36" spans="1:11">
+      <c r="L35" s="8" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
       <c r="A36" s="12" t="s">
         <v>64</v>
       </c>
@@ -4639,8 +5487,11 @@
       <c r="K36" s="18" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="37" spans="1:11">
+      <c r="L36" s="8" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12">
       <c r="A37" s="12" t="s">
         <v>68</v>
       </c>
@@ -4666,8 +5517,11 @@
       <c r="K37" s="15" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="38" spans="1:11">
+      <c r="L37" s="8" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12">
       <c r="A38" s="12" t="s">
         <v>68</v>
       </c>
@@ -4693,8 +5547,11 @@
       <c r="K38" s="15" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="39" spans="1:11">
+      <c r="L38" s="8" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
       <c r="A39" s="12" t="s">
         <v>75</v>
       </c>
@@ -4722,8 +5579,11 @@
       <c r="K39" s="15" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="40" spans="1:11">
+      <c r="L39" s="8" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12">
       <c r="A40" s="12" t="s">
         <v>76</v>
       </c>
@@ -4749,8 +5609,11 @@
       <c r="K40" s="12" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="41" spans="1:11">
+      <c r="L40" s="8" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12">
       <c r="A41" s="12" t="s">
         <v>76</v>
       </c>
@@ -4776,8 +5639,11 @@
       <c r="K41" s="12" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="42" spans="1:11">
+      <c r="L41" s="8" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12">
       <c r="A42" s="12" t="s">
         <v>76</v>
       </c>
@@ -4803,8 +5669,11 @@
       <c r="K42" s="12" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="43" spans="1:11">
+      <c r="L42" s="8" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12">
       <c r="A43" s="12" t="s">
         <v>76</v>
       </c>
@@ -4830,8 +5699,11 @@
       <c r="K43" s="12" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="44" spans="1:11">
+      <c r="L43" s="8" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12">
       <c r="A44" s="12" t="s">
         <v>76</v>
       </c>
@@ -4857,8 +5729,11 @@
       <c r="K44" s="12" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="45" spans="1:11">
+      <c r="L44" s="8" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12">
       <c r="A45" s="12" t="s">
         <v>76</v>
       </c>
@@ -4884,8 +5759,11 @@
       <c r="K45" s="18" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="46" spans="1:11">
+      <c r="L45" s="8" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12">
       <c r="A46" s="12" t="s">
         <v>76</v>
       </c>
@@ -4911,8 +5789,11 @@
       <c r="K46" s="12" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="47" spans="1:11">
+      <c r="L46" s="8" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12">
       <c r="A47" s="12" t="s">
         <v>76</v>
       </c>
@@ -4938,8 +5819,11 @@
       <c r="K47" s="12" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="48" spans="1:11">
+      <c r="L47" s="8" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12">
       <c r="A48" s="12" t="s">
         <v>76</v>
       </c>
@@ -4965,8 +5849,11 @@
       <c r="K48" s="12" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="49" spans="1:11">
+      <c r="L48" s="8" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12">
       <c r="A49" s="12" t="s">
         <v>76</v>
       </c>
@@ -4992,8 +5879,11 @@
       <c r="K49" s="12" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="50" spans="1:11">
+      <c r="L49" s="8" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12">
       <c r="A50" s="12" t="s">
         <v>76</v>
       </c>
@@ -5019,8 +5909,11 @@
       <c r="K50" s="12" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="51" spans="1:11">
+      <c r="L50" s="8" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12">
       <c r="A51" s="12" t="s">
         <v>76</v>
       </c>
@@ -5046,8 +5939,11 @@
       <c r="K51" s="18" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="52" spans="1:11">
+      <c r="L51" s="8" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12">
       <c r="A52" s="12" t="s">
         <v>76</v>
       </c>
@@ -5073,8 +5969,11 @@
       <c r="K52" s="12" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="53" spans="1:11">
+      <c r="L52" s="8" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12">
       <c r="A53" s="12" t="s">
         <v>76</v>
       </c>
@@ -5100,8 +5999,11 @@
       <c r="K53" s="12" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="54" spans="1:11">
+      <c r="L53" s="8" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12">
       <c r="A54" s="12" t="s">
         <v>76</v>
       </c>
@@ -5127,8 +6029,11 @@
       <c r="K54" s="12" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="55" spans="1:11">
+      <c r="L54" s="8" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12">
       <c r="A55" s="12" t="s">
         <v>76</v>
       </c>
@@ -5154,8 +6059,11 @@
       <c r="K55" s="12" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="56" spans="1:11">
+      <c r="L55" s="8" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12">
       <c r="A56" s="12" t="s">
         <v>76</v>
       </c>
@@ -5181,8 +6089,11 @@
       <c r="K56" s="12" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="57" spans="1:11">
+      <c r="L56" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12">
       <c r="A57" s="12" t="s">
         <v>76</v>
       </c>
@@ -5208,8 +6119,11 @@
       <c r="K57" s="12" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="58" spans="1:11">
+      <c r="L57" s="8" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12">
       <c r="A58" s="12" t="s">
         <v>76</v>
       </c>
@@ -5237,8 +6151,11 @@
       <c r="K58" s="18" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="59" spans="1:11">
+      <c r="L58" s="8" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12">
       <c r="A59" s="12" t="s">
         <v>76</v>
       </c>
@@ -5264,8 +6181,11 @@
       <c r="K59" s="12" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="60" spans="1:11">
+      <c r="L59" s="8" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12">
       <c r="A60" s="12" t="s">
         <v>76</v>
       </c>
@@ -5291,8 +6211,11 @@
       <c r="K60" s="18" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="61" spans="1:11">
+      <c r="L60" s="8" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12">
       <c r="A61" s="12" t="s">
         <v>76</v>
       </c>
@@ -5320,8 +6243,11 @@
       <c r="K61" s="12" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="62" spans="1:11">
+      <c r="L61" s="8" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12">
       <c r="A62" s="12" t="s">
         <v>76</v>
       </c>
@@ -5349,8 +6275,11 @@
       <c r="K62" s="12" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="63" spans="1:11">
+      <c r="L62" s="8" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12">
       <c r="A63" s="12" t="s">
         <v>76</v>
       </c>
@@ -5376,8 +6305,11 @@
       <c r="K63" s="12" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="64" spans="1:11">
+      <c r="L63" s="8" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12">
       <c r="A64" s="12" t="s">
         <v>76</v>
       </c>
@@ -5403,8 +6335,11 @@
       <c r="K64" s="16" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="65" spans="1:11">
+      <c r="L64" s="8" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12">
       <c r="A65" s="12" t="s">
         <v>76</v>
       </c>
@@ -5430,8 +6365,11 @@
       <c r="K65" s="12" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="66" spans="1:11">
+      <c r="L65" s="8" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12">
       <c r="A66" s="12" t="s">
         <v>76</v>
       </c>
@@ -5457,8 +6395,11 @@
       <c r="K66" s="12" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="67" spans="1:11">
+      <c r="L66" s="8" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12">
       <c r="A67" s="12" t="s">
         <v>76</v>
       </c>
@@ -5484,8 +6425,11 @@
       <c r="K67" s="12" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="68" spans="1:11">
+      <c r="L67" s="8" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12">
       <c r="A68" s="12" t="s">
         <v>76</v>
       </c>
@@ -5511,8 +6455,11 @@
       <c r="K68" s="12" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="69" spans="1:11">
+      <c r="L68" s="8" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12">
       <c r="A69" s="12" t="s">
         <v>76</v>
       </c>
@@ -5538,8 +6485,11 @@
       <c r="K69" s="12" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="70" spans="1:11">
+      <c r="L69" s="8" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12">
       <c r="A70" s="12" t="s">
         <v>76</v>
       </c>
@@ -5565,8 +6515,11 @@
       <c r="K70" s="12" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="71" spans="1:11">
+      <c r="L70" s="8" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12">
       <c r="A71" s="12" t="s">
         <v>76</v>
       </c>
@@ -5592,8 +6545,11 @@
       <c r="K71" s="18" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="72" spans="1:11">
+      <c r="L71" s="8" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12">
       <c r="A72" s="12" t="s">
         <v>76</v>
       </c>
@@ -5619,8 +6575,11 @@
       <c r="K72" s="12" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="73" spans="1:11">
+      <c r="L72" s="8" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12">
       <c r="A73" s="12" t="s">
         <v>76</v>
       </c>
@@ -5646,8 +6605,11 @@
       <c r="K73" s="12" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="74" spans="1:11">
+      <c r="L73" s="8" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12">
       <c r="A74" s="12" t="s">
         <v>76</v>
       </c>
@@ -5673,8 +6635,11 @@
       <c r="K74" s="12" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="75" spans="1:11">
+      <c r="L74" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12">
       <c r="A75" s="12" t="s">
         <v>76</v>
       </c>
@@ -5700,8 +6665,11 @@
       <c r="K75" s="18" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="76" spans="1:11">
+      <c r="L75" s="8" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12">
       <c r="A76" s="12" t="s">
         <v>76</v>
       </c>
@@ -5727,8 +6695,11 @@
       <c r="K76" s="12" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="77" spans="1:11">
+      <c r="L76" s="8" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12">
       <c r="A77" s="12" t="s">
         <v>76</v>
       </c>
@@ -5754,8 +6725,11 @@
       <c r="K77" s="12" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="78" spans="1:11">
+      <c r="L77" s="8" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12">
       <c r="A78" s="12" t="s">
         <v>76</v>
       </c>
@@ -5781,8 +6755,11 @@
       <c r="K78" s="12" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="79" spans="1:11">
+      <c r="L78" s="8" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12">
       <c r="A79" s="12" t="s">
         <v>76</v>
       </c>
@@ -5808,8 +6785,11 @@
       <c r="K79" s="12" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="80" spans="1:11">
+      <c r="L79" s="8" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12">
       <c r="A80" s="12" t="s">
         <v>76</v>
       </c>
@@ -5835,8 +6815,11 @@
       <c r="K80" s="18" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="81" spans="1:11">
+      <c r="L80" s="8" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12">
       <c r="A81" s="12" t="s">
         <v>76</v>
       </c>
@@ -5862,8 +6845,11 @@
       <c r="K81" s="18" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="82" spans="1:11">
+      <c r="L81" s="8" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12">
       <c r="A82" s="12" t="s">
         <v>76</v>
       </c>
@@ -5889,8 +6875,11 @@
       <c r="K82" s="12" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="83" spans="1:11">
+      <c r="L82" s="8" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12">
       <c r="A83" s="12" t="s">
         <v>76</v>
       </c>
@@ -5916,8 +6905,11 @@
       <c r="K83" s="12" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="84" spans="1:11">
+      <c r="L83" s="8" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12">
       <c r="A84" s="12" t="s">
         <v>76</v>
       </c>
@@ -5943,8 +6935,11 @@
       <c r="K84" s="12" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="85" spans="1:11">
+      <c r="L84" s="8" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12">
       <c r="A85" s="12" t="s">
         <v>76</v>
       </c>
@@ -5970,8 +6965,11 @@
       <c r="K85" s="12" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="86" spans="1:11">
+      <c r="L85" s="8" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12">
       <c r="A86" s="12" t="s">
         <v>119</v>
       </c>
@@ -5999,8 +6997,11 @@
       <c r="K86" s="12" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="87" spans="1:11">
+      <c r="L86" s="8" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12">
       <c r="A87" s="12" t="s">
         <v>121</v>
       </c>
@@ -6028,8 +7029,11 @@
       <c r="K87" s="12" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="88" spans="1:11">
+      <c r="L87" s="8" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12">
       <c r="A88" s="12" t="s">
         <v>121</v>
       </c>
@@ -6057,8 +7061,11 @@
       <c r="K88" s="12" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="89" spans="1:11">
+      <c r="L88" s="8" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12">
       <c r="A89" s="12" t="s">
         <v>121</v>
       </c>
@@ -6084,10 +7091,13 @@
         <v>20</v>
       </c>
       <c r="K89" s="12" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="90" spans="1:11">
+        <v>290</v>
+      </c>
+      <c r="L89" s="8" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12">
       <c r="A90" s="12" t="s">
         <v>107</v>
       </c>
@@ -6113,8 +7123,11 @@
       <c r="K90" s="12" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="91" spans="1:11">
+      <c r="L90" s="8" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12">
       <c r="A91" s="12" t="s">
         <v>107</v>
       </c>
@@ -6140,8 +7153,11 @@
       <c r="K91" s="12" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="92" spans="1:11">
+      <c r="L91" s="8" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12">
       <c r="A92" s="12" t="s">
         <v>107</v>
       </c>
@@ -6167,8 +7183,11 @@
       <c r="K92" s="12" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="93" spans="1:11">
+      <c r="L92" s="8" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12">
       <c r="A93" s="12" t="s">
         <v>127</v>
       </c>
@@ -6196,8 +7215,11 @@
       <c r="K93" s="12" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="94" spans="1:11">
+      <c r="L93" s="8" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12">
       <c r="A94" s="12" t="s">
         <v>127</v>
       </c>
@@ -6225,8 +7247,11 @@
       <c r="K94" s="12" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="95" spans="1:11">
+      <c r="L94" s="8" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12">
       <c r="A95" s="12" t="s">
         <v>127</v>
       </c>
@@ -6254,8 +7279,11 @@
       <c r="K95" s="12" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="96" spans="1:11">
+      <c r="L95" s="8" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12">
       <c r="A96" s="12" t="s">
         <v>127</v>
       </c>
@@ -6283,8 +7311,11 @@
       <c r="K96" s="12" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="97" spans="1:11">
+      <c r="L96" s="8" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12">
       <c r="A97" s="12" t="s">
         <v>127</v>
       </c>
@@ -6312,8 +7343,11 @@
       <c r="K97" s="12" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="98" spans="1:11">
+      <c r="L97" s="8" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12">
       <c r="A98" s="12" t="s">
         <v>133</v>
       </c>
@@ -6341,8 +7375,11 @@
       <c r="K98" s="12" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="99" spans="1:11">
+      <c r="L98" s="8" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12">
       <c r="A99" s="12" t="s">
         <v>133</v>
       </c>
@@ -6370,8 +7407,11 @@
       <c r="K99" s="12" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="100" spans="1:11">
+      <c r="L99" s="8" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12">
       <c r="A100" s="12" t="s">
         <v>135</v>
       </c>
@@ -6399,8 +7439,11 @@
       <c r="K100" s="12" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="101" spans="1:11">
+      <c r="L100" s="8" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12">
       <c r="A101" s="12" t="s">
         <v>135</v>
       </c>
@@ -6428,8 +7471,11 @@
       <c r="K101" s="12" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="102" spans="1:11">
+      <c r="L101" s="8" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12">
       <c r="A102" s="12" t="s">
         <v>204</v>
       </c>
@@ -6457,8 +7503,11 @@
       <c r="K102" s="12" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="103" spans="1:11">
+      <c r="L102" s="8" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12">
       <c r="A103" s="12" t="s">
         <v>204</v>
       </c>
@@ -6486,8 +7535,11 @@
       <c r="K103" s="12" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="104" spans="1:11">
+      <c r="L103" s="8" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12">
       <c r="A104" s="12" t="s">
         <v>204</v>
       </c>
@@ -6515,8 +7567,11 @@
       <c r="K104" s="12" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="105" spans="1:11">
+      <c r="L104" s="8" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12">
       <c r="A105" s="12" t="s">
         <v>142</v>
       </c>
@@ -6544,8 +7599,11 @@
       <c r="K105" s="12" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="106" spans="1:11">
+      <c r="L105" s="8" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12">
       <c r="A106" s="12" t="s">
         <v>143</v>
       </c>
@@ -6571,8 +7629,11 @@
       <c r="K106" s="12" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="107" spans="1:11">
+      <c r="L106" s="8" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12">
       <c r="A107" s="12" t="s">
         <v>143</v>
       </c>
@@ -6598,8 +7659,11 @@
       <c r="K107" s="12" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="108" spans="1:11">
+      <c r="L107" s="8" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="108" spans="1:12">
       <c r="A108" s="12" t="s">
         <v>143</v>
       </c>
@@ -6625,8 +7689,11 @@
       <c r="K108" s="12" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="109" spans="1:11">
+      <c r="L108" s="8" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12">
       <c r="A109" s="12" t="s">
         <v>143</v>
       </c>
@@ -6652,8 +7719,11 @@
       <c r="K109" s="12" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="110" spans="1:11">
+      <c r="L109" s="8" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="110" spans="1:12">
       <c r="A110" s="12" t="s">
         <v>143</v>
       </c>
@@ -6679,8 +7749,11 @@
       <c r="K110" s="12" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="111" spans="1:11">
+      <c r="L110" s="8" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="111" spans="1:12">
       <c r="A111" s="12" t="s">
         <v>150</v>
       </c>
@@ -6706,8 +7779,11 @@
       <c r="K111" s="12" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="112" spans="1:11">
+      <c r="L111" s="8" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12">
       <c r="A112" s="12" t="s">
         <v>150</v>
       </c>
@@ -6733,8 +7809,11 @@
       <c r="K112" s="12" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="113" spans="1:11">
+      <c r="L112" s="8" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12">
       <c r="A113" s="12" t="s">
         <v>150</v>
       </c>
@@ -6760,8 +7839,11 @@
       <c r="K113" s="12" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="114" spans="1:11">
+      <c r="L113" s="8" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="114" spans="1:12">
       <c r="A114" s="12" t="s">
         <v>150</v>
       </c>
@@ -6787,8 +7869,11 @@
       <c r="K114" s="12" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="115" spans="1:11">
+      <c r="L114" s="8" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="115" spans="1:12">
       <c r="A115" s="12" t="s">
         <v>150</v>
       </c>
@@ -6814,8 +7899,11 @@
       <c r="K115" s="12" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="116" spans="1:11">
+      <c r="L115" s="8" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12">
       <c r="A116" s="12" t="s">
         <v>150</v>
       </c>
@@ -6841,8 +7929,11 @@
       <c r="K116" s="12" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="117" spans="1:11">
+      <c r="L116" s="8" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="117" spans="1:12">
       <c r="A117" s="12" t="s">
         <v>150</v>
       </c>
@@ -6868,8 +7959,11 @@
       <c r="K117" s="12" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="118" spans="1:11">
+      <c r="L117" s="8" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="118" spans="1:12">
       <c r="A118" s="12" t="s">
         <v>150</v>
       </c>
@@ -6895,8 +7989,11 @@
       <c r="K118" s="12" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="119" spans="1:11">
+      <c r="L118" s="8" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="119" spans="1:12">
       <c r="A119" s="12" t="s">
         <v>150</v>
       </c>
@@ -6922,8 +8019,11 @@
       <c r="K119" s="12" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="120" spans="1:11">
+      <c r="L119" s="8" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="120" spans="1:12">
       <c r="A120" s="12" t="s">
         <v>150</v>
       </c>
@@ -6949,8 +8049,11 @@
       <c r="K120" s="12" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="121" spans="1:11">
+      <c r="L120" s="8" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="121" spans="1:12">
       <c r="A121" s="12" t="s">
         <v>162</v>
       </c>
@@ -6978,8 +8081,11 @@
       <c r="K121" s="12" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="122" spans="1:11">
+      <c r="L121" s="8" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="122" spans="1:12">
       <c r="A122" s="12" t="s">
         <v>162</v>
       </c>
@@ -7007,8 +8113,11 @@
       <c r="K122" s="12" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="123" spans="1:11">
+      <c r="L122" s="8" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="123" spans="1:12">
       <c r="A123" s="12" t="s">
         <v>162</v>
       </c>
@@ -7036,8 +8145,11 @@
       <c r="K123" s="12" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="124" spans="1:11">
+      <c r="L123" s="8" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="124" spans="1:12">
       <c r="A124" s="12" t="s">
         <v>162</v>
       </c>
@@ -7064,6 +8176,9 @@
       </c>
       <c r="K124" s="12" t="s">
         <v>166</v>
+      </c>
+      <c r="L124" s="8" t="s">
+        <v>325</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove Main Nav arrow; change Programs to Explore Programs
</commit_message>
<xml_diff>
--- a/_data/_data.xlsx
+++ b/_data/_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26330"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="navigation" sheetId="4" r:id="rId1"/>
@@ -532,9 +532,6 @@
     <t>About Shoreline</t>
   </si>
   <si>
-    <t>Programs</t>
-  </si>
-  <si>
     <t>Apply &amp; Aid</t>
   </si>
   <si>
@@ -1010,6 +1007,9 @@
   </si>
   <si>
     <t>https://www.shoreline.edu/about-shoreline/documents/catalog2010scc.pdf</t>
+  </si>
+  <si>
+    <t>Explore Programs</t>
   </si>
 </sst>
 </file>
@@ -2024,7 +2024,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2034,8 +2034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2059,10 +2059,10 @@
         <v>3</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>200</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>201</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>1</v>
@@ -2084,13 +2084,13 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="17" t="s">
-        <v>168</v>
+        <v>327</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -2098,10 +2098,10 @@
     <row r="4" spans="1:8">
       <c r="A4" s="17"/>
       <c r="D4" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>202</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -2127,7 +2127,7 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>4</v>
@@ -2138,7 +2138,7 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>4</v>
@@ -2149,7 +2149,7 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>4</v>
@@ -2171,7 +2171,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M124"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
     </sheetView>
@@ -2202,10 +2202,10 @@
         <v>14</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G1" s="11" t="s">
         <v>6</v>
@@ -2240,10 +2240,10 @@
         <v>20</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G2" s="12" t="s">
         <v>17</v>
@@ -2258,7 +2258,7 @@
       </c>
       <c r="L2" s="14"/>
       <c r="M2" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -2275,10 +2275,10 @@
         <v>20</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G3" s="12" t="s">
         <v>22</v>
@@ -2293,7 +2293,7 @@
       </c>
       <c r="L3" s="12"/>
       <c r="M3" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -2310,10 +2310,10 @@
         <v>20</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G4" s="12" t="s">
         <v>17</v>
@@ -2328,7 +2328,7 @@
       </c>
       <c r="L4" s="12"/>
       <c r="M4" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -2345,10 +2345,10 @@
         <v>20</v>
       </c>
       <c r="E5" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="F5" s="12" t="s">
         <v>175</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>176</v>
       </c>
       <c r="G5" s="12" t="s">
         <v>17</v>
@@ -2363,7 +2363,7 @@
       </c>
       <c r="L5" s="14"/>
       <c r="M5" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -2380,10 +2380,10 @@
         <v>20</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G6" s="12" t="s">
         <v>17</v>
@@ -2398,7 +2398,7 @@
       </c>
       <c r="L6" s="12"/>
       <c r="M6" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -2415,10 +2415,10 @@
         <v>20</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G7" s="12" t="s">
         <v>17</v>
@@ -2433,7 +2433,7 @@
       </c>
       <c r="L7" s="12"/>
       <c r="M7" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -2450,10 +2450,10 @@
         <v>20</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G8" s="12" t="s">
         <v>45</v>
@@ -2468,7 +2468,7 @@
       </c>
       <c r="L8" s="12"/>
       <c r="M8" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -2485,10 +2485,10 @@
         <v>20</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G9" s="12" t="s">
         <v>17</v>
@@ -2503,7 +2503,7 @@
       </c>
       <c r="L9" s="12"/>
       <c r="M9" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -2520,10 +2520,10 @@
         <v>20</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G10" s="12" t="s">
         <v>17</v>
@@ -2538,7 +2538,7 @@
       </c>
       <c r="L10" s="12"/>
       <c r="M10" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -2555,10 +2555,10 @@
         <v>73</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G11" s="12" t="s">
         <v>69</v>
@@ -2571,7 +2571,7 @@
       </c>
       <c r="L11" s="12"/>
       <c r="M11" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="12" spans="1:13">
@@ -2588,10 +2588,10 @@
         <v>20</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G12" s="12" t="s">
         <v>17</v>
@@ -2606,7 +2606,7 @@
       </c>
       <c r="L12" s="14"/>
       <c r="M12" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="13" spans="1:13">
@@ -2623,10 +2623,10 @@
         <v>73</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G13" s="12" t="s">
         <v>77</v>
@@ -2639,7 +2639,7 @@
         <v>78</v>
       </c>
       <c r="M13" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="14" spans="1:13">
@@ -2656,10 +2656,10 @@
         <v>20</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G14" s="12" t="s">
         <v>17</v>
@@ -2674,7 +2674,7 @@
       </c>
       <c r="L14" s="12"/>
       <c r="M14" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="15" spans="1:13">
@@ -2691,10 +2691,10 @@
         <v>20</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G15" s="12" t="s">
         <v>17</v>
@@ -2709,7 +2709,7 @@
       </c>
       <c r="L15" s="12"/>
       <c r="M15" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="16" spans="1:13">
@@ -2726,10 +2726,10 @@
         <v>73</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G16" s="12" t="s">
         <v>123</v>
@@ -2742,7 +2742,7 @@
       </c>
       <c r="L16" s="12"/>
       <c r="M16" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="17" spans="1:13">
@@ -2759,10 +2759,10 @@
         <v>20</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G17" s="12" t="s">
         <v>17</v>
@@ -2777,7 +2777,7 @@
       </c>
       <c r="L17" s="12"/>
       <c r="M17" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="18" spans="1:13" s="7" customFormat="1">
@@ -2794,10 +2794,10 @@
         <v>20</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G18" s="12" t="s">
         <v>17</v>
@@ -2812,7 +2812,7 @@
       </c>
       <c r="L18" s="14"/>
       <c r="M18" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="19" spans="1:13">
@@ -2829,10 +2829,10 @@
         <v>20</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G19" s="12" t="s">
         <v>45</v>
@@ -2847,12 +2847,12 @@
       </c>
       <c r="L19" s="12"/>
       <c r="M19" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="20" spans="1:13">
       <c r="A20" s="12" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B20" s="12" t="s">
         <v>70</v>
@@ -2864,10 +2864,10 @@
         <v>20</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G20" s="12" t="s">
         <v>30</v>
@@ -2882,7 +2882,7 @@
       </c>
       <c r="L20" s="12"/>
       <c r="M20" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="21" spans="1:13">
@@ -2899,10 +2899,10 @@
         <v>20</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G21" s="12" t="s">
         <v>17</v>
@@ -2917,7 +2917,7 @@
       </c>
       <c r="L21" s="12"/>
       <c r="M21" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="22" spans="1:13">
@@ -2934,10 +2934,10 @@
         <v>73</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G22" s="12" t="s">
         <v>144</v>
@@ -2950,7 +2950,7 @@
       <c r="K22" s="12"/>
       <c r="L22" s="12"/>
       <c r="M22" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="23" spans="1:13">
@@ -2967,10 +2967,10 @@
         <v>73</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G23" s="12" t="s">
         <v>151</v>
@@ -2983,7 +2983,7 @@
         <v>152</v>
       </c>
       <c r="M23" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="24" spans="1:13">
@@ -3000,10 +3000,10 @@
         <v>20</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G24" s="12" t="s">
         <v>17</v>
@@ -3018,7 +3018,7 @@
       </c>
       <c r="L24" s="12"/>
       <c r="M24" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="25" spans="1:13">
@@ -4395,7 +4395,7 @@
         <v>15</v>
       </c>
       <c r="L1" s="9" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -4427,7 +4427,7 @@
         <v>16</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -4459,7 +4459,7 @@
         <v>29</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -4491,7 +4491,7 @@
         <v>32</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -4523,7 +4523,7 @@
         <v>33</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -4555,7 +4555,7 @@
         <v>34</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -4587,7 +4587,7 @@
         <v>35</v>
       </c>
       <c r="L7" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -4619,7 +4619,7 @@
         <v>24</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -4651,7 +4651,7 @@
         <v>26</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -4683,7 +4683,7 @@
         <v>27</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -4715,7 +4715,7 @@
         <v>28</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -4747,7 +4747,7 @@
         <v>31</v>
       </c>
       <c r="L12" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -4779,7 +4779,7 @@
         <v>38</v>
       </c>
       <c r="L13" s="8" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -4811,7 +4811,7 @@
         <v>38</v>
       </c>
       <c r="L14" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -4843,7 +4843,7 @@
         <v>41</v>
       </c>
       <c r="L15" s="8" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -4875,7 +4875,7 @@
         <v>42</v>
       </c>
       <c r="L16" s="8" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -4907,7 +4907,7 @@
         <v>43</v>
       </c>
       <c r="L17" s="8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="18" spans="1:12" s="7" customFormat="1">
@@ -4939,7 +4939,7 @@
         <v>44</v>
       </c>
       <c r="L18" s="8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -4971,7 +4971,7 @@
         <v>47</v>
       </c>
       <c r="L19" s="8" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -5003,7 +5003,7 @@
         <v>49</v>
       </c>
       <c r="L20" s="8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -5035,7 +5035,7 @@
         <v>51</v>
       </c>
       <c r="L21" s="8" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="22" spans="1:12">
@@ -5067,7 +5067,7 @@
         <v>50</v>
       </c>
       <c r="L22" s="8" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="23" spans="1:12">
@@ -5099,7 +5099,7 @@
         <v>46</v>
       </c>
       <c r="L23" s="8" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -5131,7 +5131,7 @@
         <v>48</v>
       </c>
       <c r="L24" s="8" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="25" spans="1:12">
@@ -5163,7 +5163,7 @@
         <v>52</v>
       </c>
       <c r="L25" s="8" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="26" spans="1:12">
@@ -5195,7 +5195,7 @@
         <v>53</v>
       </c>
       <c r="L26" s="8" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -5227,7 +5227,7 @@
         <v>53</v>
       </c>
       <c r="L27" s="8" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="28" spans="1:12">
@@ -5259,7 +5259,7 @@
         <v>53</v>
       </c>
       <c r="L28" s="8" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="29" spans="1:12">
@@ -5291,7 +5291,7 @@
         <v>54</v>
       </c>
       <c r="L29" s="8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="30" spans="1:12">
@@ -5323,7 +5323,7 @@
         <v>55</v>
       </c>
       <c r="L30" s="8" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="31" spans="1:12">
@@ -5355,7 +5355,7 @@
         <v>57</v>
       </c>
       <c r="L31" s="8" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="32" spans="1:12">
@@ -5387,7 +5387,7 @@
         <v>58</v>
       </c>
       <c r="L32" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="33" spans="1:12">
@@ -5419,7 +5419,7 @@
         <v>60</v>
       </c>
       <c r="L33" s="8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="34" spans="1:12">
@@ -5451,7 +5451,7 @@
         <v>62</v>
       </c>
       <c r="L34" s="8" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="35" spans="1:12">
@@ -5483,7 +5483,7 @@
         <v>66</v>
       </c>
       <c r="L35" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="36" spans="1:12">
@@ -5515,7 +5515,7 @@
         <v>67</v>
       </c>
       <c r="L36" s="8" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="37" spans="1:12">
@@ -5545,7 +5545,7 @@
         <v>71</v>
       </c>
       <c r="L37" s="8" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="38" spans="1:12">
@@ -5575,7 +5575,7 @@
         <v>74</v>
       </c>
       <c r="L38" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="39" spans="1:12">
@@ -5607,7 +5607,7 @@
         <v>75</v>
       </c>
       <c r="L39" s="8" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="40" spans="1:12">
@@ -5637,7 +5637,7 @@
         <v>87</v>
       </c>
       <c r="L40" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="41" spans="1:12">
@@ -5667,7 +5667,7 @@
         <v>117</v>
       </c>
       <c r="L41" s="8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="42" spans="1:12">
@@ -5697,7 +5697,7 @@
         <v>18</v>
       </c>
       <c r="L42" s="8" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="43" spans="1:12">
@@ -5727,7 +5727,7 @@
         <v>96</v>
       </c>
       <c r="L43" s="8" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="44" spans="1:12">
@@ -5757,7 +5757,7 @@
         <v>113</v>
       </c>
       <c r="L44" s="8" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="45" spans="1:12">
@@ -5771,7 +5771,7 @@
         <v>63</v>
       </c>
       <c r="D45" s="12" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E45" s="12"/>
       <c r="F45" s="18"/>
@@ -5784,10 +5784,10 @@
         <v>73</v>
       </c>
       <c r="K45" s="18" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="L45" s="8" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="46" spans="1:12">
@@ -5801,7 +5801,7 @@
         <v>63</v>
       </c>
       <c r="D46" s="12" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E46" s="12"/>
       <c r="F46" s="18"/>
@@ -5814,10 +5814,10 @@
         <v>73</v>
       </c>
       <c r="K46" s="12" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L46" s="8" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="47" spans="1:12">
@@ -5847,7 +5847,7 @@
         <v>100</v>
       </c>
       <c r="L47" s="8" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="48" spans="1:12">
@@ -5877,7 +5877,7 @@
         <v>108</v>
       </c>
       <c r="L48" s="8" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="49" spans="1:12">
@@ -5907,7 +5907,7 @@
         <v>78</v>
       </c>
       <c r="L49" s="8" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="50" spans="1:12">
@@ -5937,7 +5937,7 @@
         <v>79</v>
       </c>
       <c r="L50" s="8" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="51" spans="1:12">
@@ -5967,7 +5967,7 @@
         <v>80</v>
       </c>
       <c r="L51" s="8" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="52" spans="1:12">
@@ -5997,7 +5997,7 @@
         <v>118</v>
       </c>
       <c r="L52" s="8" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="53" spans="1:12">
@@ -6027,7 +6027,7 @@
         <v>112</v>
       </c>
       <c r="L53" s="8" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="54" spans="1:12">
@@ -6057,7 +6057,7 @@
         <v>82</v>
       </c>
       <c r="L54" s="8" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="55" spans="1:12">
@@ -6087,7 +6087,7 @@
         <v>88</v>
       </c>
       <c r="L55" s="8" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="56" spans="1:12">
@@ -6117,7 +6117,7 @@
         <v>90</v>
       </c>
       <c r="L56" s="8" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="57" spans="1:12">
@@ -6147,7 +6147,7 @@
         <v>91</v>
       </c>
       <c r="L57" s="8" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="58" spans="1:12">
@@ -6179,7 +6179,7 @@
         <v>93</v>
       </c>
       <c r="L58" s="8" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="59" spans="1:12">
@@ -6193,7 +6193,7 @@
         <v>70</v>
       </c>
       <c r="D59" s="12" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E59" s="12"/>
       <c r="F59" s="12"/>
@@ -6206,10 +6206,10 @@
         <v>73</v>
       </c>
       <c r="K59" s="12" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L59" s="8" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="60" spans="1:12">
@@ -6239,7 +6239,7 @@
         <v>70</v>
       </c>
       <c r="L60" s="8" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="61" spans="1:12">
@@ -6271,7 +6271,7 @@
         <v>104</v>
       </c>
       <c r="L61" s="8" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="62" spans="1:12">
@@ -6303,7 +6303,7 @@
         <v>105</v>
       </c>
       <c r="L62" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="63" spans="1:12">
@@ -6333,7 +6333,7 @@
         <v>107</v>
       </c>
       <c r="L63" s="8" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="64" spans="1:12">
@@ -6363,7 +6363,7 @@
         <v>92</v>
       </c>
       <c r="L64" s="8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="65" spans="1:12">
@@ -6393,7 +6393,7 @@
         <v>106</v>
       </c>
       <c r="L65" s="8" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="66" spans="1:12">
@@ -6423,7 +6423,7 @@
         <v>83</v>
       </c>
       <c r="L66" s="8" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="67" spans="1:12">
@@ -6453,7 +6453,7 @@
         <v>84</v>
       </c>
       <c r="L67" s="8" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="68" spans="1:12">
@@ -6483,7 +6483,7 @@
         <v>85</v>
       </c>
       <c r="L68" s="8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="69" spans="1:12">
@@ -6513,7 +6513,7 @@
         <v>86</v>
       </c>
       <c r="L69" s="8" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="70" spans="1:12">
@@ -6543,7 +6543,7 @@
         <v>89</v>
       </c>
       <c r="L70" s="8" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="71" spans="1:12">
@@ -6573,7 +6573,7 @@
         <v>58</v>
       </c>
       <c r="L71" s="8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="72" spans="1:12">
@@ -6603,7 +6603,7 @@
         <v>95</v>
       </c>
       <c r="L72" s="8" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="73" spans="1:12">
@@ -6633,7 +6633,7 @@
         <v>97</v>
       </c>
       <c r="L73" s="8" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="74" spans="1:12">
@@ -6663,7 +6663,7 @@
         <v>98</v>
       </c>
       <c r="L74" s="8" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="75" spans="1:12">
@@ -6693,7 +6693,7 @@
         <v>99</v>
       </c>
       <c r="L75" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="76" spans="1:12">
@@ -6723,7 +6723,7 @@
         <v>101</v>
       </c>
       <c r="L76" s="8" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="77" spans="1:12">
@@ -6753,7 +6753,7 @@
         <v>102</v>
       </c>
       <c r="L77" s="8" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="78" spans="1:12">
@@ -6783,7 +6783,7 @@
         <v>103</v>
       </c>
       <c r="L78" s="8" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="79" spans="1:12">
@@ -6813,7 +6813,7 @@
         <v>109</v>
       </c>
       <c r="L79" s="8" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="80" spans="1:12">
@@ -6843,7 +6843,7 @@
         <v>110</v>
       </c>
       <c r="L80" s="8" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="81" spans="1:12">
@@ -6873,7 +6873,7 @@
         <v>81</v>
       </c>
       <c r="L81" s="8" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="82" spans="1:12">
@@ -6903,7 +6903,7 @@
         <v>111</v>
       </c>
       <c r="L82" s="8" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="83" spans="1:12">
@@ -6933,7 +6933,7 @@
         <v>114</v>
       </c>
       <c r="L83" s="8" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="84" spans="1:12">
@@ -6963,7 +6963,7 @@
         <v>115</v>
       </c>
       <c r="L84" s="8" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="85" spans="1:12">
@@ -6993,7 +6993,7 @@
         <v>116</v>
       </c>
       <c r="L85" s="8" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="86" spans="1:12">
@@ -7025,7 +7025,7 @@
         <v>120</v>
       </c>
       <c r="L86" s="8" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="87" spans="1:12">
@@ -7057,7 +7057,7 @@
         <v>121</v>
       </c>
       <c r="L87" s="8" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="88" spans="1:12">
@@ -7089,7 +7089,7 @@
         <v>121</v>
       </c>
       <c r="L88" s="8" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="89" spans="1:12">
@@ -7118,10 +7118,10 @@
         <v>20</v>
       </c>
       <c r="K89" s="12" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="L89" s="8" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="90" spans="1:12">
@@ -7151,7 +7151,7 @@
         <v>124</v>
       </c>
       <c r="L90" s="8" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="91" spans="1:12">
@@ -7181,7 +7181,7 @@
         <v>125</v>
       </c>
       <c r="L91" s="8" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="92" spans="1:12">
@@ -7211,7 +7211,7 @@
         <v>126</v>
       </c>
       <c r="L92" s="8" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="93" spans="1:12">
@@ -7243,7 +7243,7 @@
         <v>128</v>
       </c>
       <c r="L93" s="8" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="94" spans="1:12">
@@ -7275,7 +7275,7 @@
         <v>129</v>
       </c>
       <c r="L94" s="8" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="95" spans="1:12">
@@ -7307,7 +7307,7 @@
         <v>131</v>
       </c>
       <c r="L95" s="8" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="96" spans="1:12">
@@ -7339,7 +7339,7 @@
         <v>132</v>
       </c>
       <c r="L96" s="8" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="97" spans="1:12">
@@ -7371,7 +7371,7 @@
         <v>130</v>
       </c>
       <c r="L97" s="8" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="98" spans="1:12">
@@ -7403,7 +7403,7 @@
         <v>133</v>
       </c>
       <c r="L98" s="8" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="99" spans="1:12">
@@ -7435,7 +7435,7 @@
         <v>134</v>
       </c>
       <c r="L99" s="8" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="100" spans="1:12">
@@ -7467,7 +7467,7 @@
         <v>136</v>
       </c>
       <c r="L100" s="8" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="101" spans="1:12">
@@ -7499,12 +7499,12 @@
         <v>137</v>
       </c>
       <c r="L101" s="8" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="102" spans="1:12">
       <c r="A102" s="12" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B102" s="12" t="s">
         <v>17</v>
@@ -7531,12 +7531,12 @@
         <v>140</v>
       </c>
       <c r="L102" s="8" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="103" spans="1:12">
       <c r="A103" s="12" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B103" s="12" t="s">
         <v>30</v>
@@ -7563,12 +7563,12 @@
         <v>139</v>
       </c>
       <c r="L103" s="8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="104" spans="1:12">
       <c r="A104" s="12" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B104" s="12" t="s">
         <v>30</v>
@@ -7595,7 +7595,7 @@
         <v>141</v>
       </c>
       <c r="L104" s="8" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="105" spans="1:12">
@@ -7627,7 +7627,7 @@
         <v>142</v>
       </c>
       <c r="L105" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="106" spans="1:12">
@@ -7657,7 +7657,7 @@
         <v>147</v>
       </c>
       <c r="L106" s="8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="107" spans="1:12">
@@ -7687,7 +7687,7 @@
         <v>148</v>
       </c>
       <c r="L107" s="8" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="108" spans="1:12">
@@ -7717,7 +7717,7 @@
         <v>149</v>
       </c>
       <c r="L108" s="8" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="109" spans="1:12">
@@ -7747,7 +7747,7 @@
         <v>145</v>
       </c>
       <c r="L109" s="8" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="110" spans="1:12">
@@ -7777,7 +7777,7 @@
         <v>146</v>
       </c>
       <c r="L110" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="111" spans="1:12">
@@ -7807,7 +7807,7 @@
         <v>152</v>
       </c>
       <c r="L111" s="8" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="112" spans="1:12">
@@ -7837,7 +7837,7 @@
         <v>160</v>
       </c>
       <c r="L112" s="8" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="113" spans="1:12">
@@ -7867,7 +7867,7 @@
         <v>153</v>
       </c>
       <c r="L113" s="8" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="114" spans="1:12">
@@ -7897,7 +7897,7 @@
         <v>154</v>
       </c>
       <c r="L114" s="8" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="115" spans="1:12">
@@ -7927,7 +7927,7 @@
         <v>155</v>
       </c>
       <c r="L115" s="8" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="116" spans="1:12">
@@ -7957,7 +7957,7 @@
         <v>156</v>
       </c>
       <c r="L116" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="117" spans="1:12">
@@ -7987,7 +7987,7 @@
         <v>157</v>
       </c>
       <c r="L117" s="8" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="118" spans="1:12">
@@ -8017,7 +8017,7 @@
         <v>158</v>
       </c>
       <c r="L118" s="8" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="119" spans="1:12">
@@ -8047,7 +8047,7 @@
         <v>159</v>
       </c>
       <c r="L119" s="8" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="120" spans="1:12">
@@ -8077,7 +8077,7 @@
         <v>161</v>
       </c>
       <c r="L120" s="8" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="121" spans="1:12">
@@ -8109,7 +8109,7 @@
         <v>163</v>
       </c>
       <c r="L121" s="8" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="122" spans="1:12">
@@ -8141,7 +8141,7 @@
         <v>164</v>
       </c>
       <c r="L122" s="8" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="123" spans="1:12">
@@ -8173,7 +8173,7 @@
         <v>165</v>
       </c>
       <c r="L123" s="8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="124" spans="1:12">
@@ -8205,7 +8205,7 @@
         <v>166</v>
       </c>
       <c r="L124" s="8" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modify menus, capitalization, and programm pages
- add capitalize_all plugin for single source tags
- add css capitalization for multiple source list items
- add sidebar CTA to program pages
</commit_message>
<xml_diff>
--- a/_data/_data.xlsx
+++ b/_data/_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26330"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="1820" yWindow="0" windowWidth="32280" windowHeight="19540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="navigation" sheetId="4" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1312" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1316" uniqueCount="329">
   <si>
     <t>label</t>
   </si>
@@ -1010,6 +1010,9 @@
   </si>
   <si>
     <t>Explore Programs</t>
+  </si>
+  <si>
+    <t>inactive</t>
   </si>
 </sst>
 </file>
@@ -2024,7 +2027,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2035,7 +2038,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="F8" sqref="F8:F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2078,7 +2081,9 @@
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
-      <c r="F2" s="2"/>
+      <c r="F2" s="2" t="s">
+        <v>328</v>
+      </c>
       <c r="G2" s="1"/>
       <c r="H2" s="2"/>
     </row>
@@ -2135,6 +2140,9 @@
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
+      <c r="F8" t="s">
+        <v>328</v>
+      </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
@@ -2146,6 +2154,9 @@
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
+      <c r="F9" t="s">
+        <v>328</v>
+      </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
@@ -2153,6 +2164,9 @@
       </c>
       <c r="B10" s="5" t="s">
         <v>4</v>
+      </c>
+      <c r="F10" t="s">
+        <v>328</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reorder spreadsheet for alphebetical order
Ordered spreadsheet first by page name (A-Z) then program
(A-Z). This creates alphebetical lists throughout the prototype.
</commit_message>
<xml_diff>
--- a/_data/_data.xlsx
+++ b/_data/_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26330"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1820" yWindow="0" windowWidth="32280" windowHeight="19540" tabRatio="500"/>
+    <workbookView xWindow="1820" yWindow="60" windowWidth="32280" windowHeight="19580" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="navigation" sheetId="4" r:id="rId1"/>
@@ -1025,6 +1025,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2027,7 +2028,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2037,7 +2038,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8:F10"/>
     </sheetView>
   </sheetViews>
@@ -4355,8 +4356,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L124"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
@@ -4449,7 +4450,7 @@
         <v>21</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C3" s="12" t="s">
         <v>23</v>
@@ -4457,7 +4458,7 @@
       <c r="D3" s="12"/>
       <c r="E3" s="12"/>
       <c r="F3" s="12" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="G3" s="12"/>
       <c r="H3" s="12" t="s">
@@ -4470,10 +4471,10 @@
         <v>20</v>
       </c>
       <c r="K3" s="12" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -4481,7 +4482,7 @@
         <v>21</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>23</v>
@@ -4489,7 +4490,7 @@
       <c r="D4" s="12"/>
       <c r="E4" s="12"/>
       <c r="F4" s="12" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="G4" s="12"/>
       <c r="H4" s="12" t="s">
@@ -4502,10 +4503,10 @@
         <v>20</v>
       </c>
       <c r="K4" s="12" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>210</v>
+        <v>326</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -4513,7 +4514,7 @@
         <v>21</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>23</v>
@@ -4521,9 +4522,9 @@
       <c r="D5" s="12"/>
       <c r="E5" s="12"/>
       <c r="F5" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="G5" s="14"/>
+        <v>27</v>
+      </c>
+      <c r="G5" s="12"/>
       <c r="H5" s="12" t="s">
         <v>21</v>
       </c>
@@ -4534,10 +4535,10 @@
         <v>20</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -4545,7 +4546,7 @@
         <v>21</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>23</v>
@@ -4553,9 +4554,9 @@
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
       <c r="F6" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="G6" s="14"/>
+        <v>28</v>
+      </c>
+      <c r="G6" s="12"/>
       <c r="H6" s="12" t="s">
         <v>21</v>
       </c>
@@ -4566,10 +4567,10 @@
         <v>20</v>
       </c>
       <c r="K6" s="12" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -4585,9 +4586,9 @@
       <c r="D7" s="12"/>
       <c r="E7" s="12"/>
       <c r="F7" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="G7" s="14"/>
+        <v>29</v>
+      </c>
+      <c r="G7" s="12"/>
       <c r="H7" s="12" t="s">
         <v>21</v>
       </c>
@@ -4598,10 +4599,10 @@
         <v>20</v>
       </c>
       <c r="K7" s="12" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="L7" s="8" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -4609,7 +4610,7 @@
         <v>21</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>23</v>
@@ -4617,7 +4618,7 @@
       <c r="D8" s="12"/>
       <c r="E8" s="12"/>
       <c r="F8" s="12" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="G8" s="12"/>
       <c r="H8" s="12" t="s">
@@ -4630,10 +4631,10 @@
         <v>20</v>
       </c>
       <c r="K8" s="12" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -4641,7 +4642,7 @@
         <v>21</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C9" s="12" t="s">
         <v>23</v>
@@ -4649,7 +4650,7 @@
       <c r="D9" s="12"/>
       <c r="E9" s="12"/>
       <c r="F9" s="12" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="G9" s="12"/>
       <c r="H9" s="12" t="s">
@@ -4662,10 +4663,10 @@
         <v>20</v>
       </c>
       <c r="K9" s="12" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>326</v>
+        <v>210</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -4673,7 +4674,7 @@
         <v>21</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C10" s="12" t="s">
         <v>23</v>
@@ -4681,9 +4682,9 @@
       <c r="D10" s="12"/>
       <c r="E10" s="12"/>
       <c r="F10" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="G10" s="12"/>
+        <v>33</v>
+      </c>
+      <c r="G10" s="14"/>
       <c r="H10" s="12" t="s">
         <v>21</v>
       </c>
@@ -4694,10 +4695,10 @@
         <v>20</v>
       </c>
       <c r="K10" s="12" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -4705,7 +4706,7 @@
         <v>21</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>23</v>
@@ -4713,9 +4714,9 @@
       <c r="D11" s="12"/>
       <c r="E11" s="12"/>
       <c r="F11" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="G11" s="12"/>
+        <v>34</v>
+      </c>
+      <c r="G11" s="14"/>
       <c r="H11" s="12" t="s">
         <v>21</v>
       </c>
@@ -4726,10 +4727,10 @@
         <v>20</v>
       </c>
       <c r="K11" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -4737,7 +4738,7 @@
         <v>21</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="C12" s="12" t="s">
         <v>23</v>
@@ -4745,9 +4746,9 @@
       <c r="D12" s="12"/>
       <c r="E12" s="12"/>
       <c r="F12" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="G12" s="12"/>
+        <v>35</v>
+      </c>
+      <c r="G12" s="14"/>
       <c r="H12" s="12" t="s">
         <v>21</v>
       </c>
@@ -4758,10 +4759,10 @@
         <v>20</v>
       </c>
       <c r="K12" s="12" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="L12" s="8" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -4961,7 +4962,7 @@
         <v>40</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="C19" s="12" t="s">
         <v>18</v>
@@ -4969,9 +4970,9 @@
       <c r="D19" s="12"/>
       <c r="E19" s="12"/>
       <c r="F19" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="G19" s="14"/>
+        <v>46</v>
+      </c>
+      <c r="G19" s="12"/>
       <c r="H19" s="12" t="s">
         <v>40</v>
       </c>
@@ -4982,10 +4983,10 @@
         <v>20</v>
       </c>
       <c r="K19" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L19" s="8" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -5001,9 +5002,9 @@
       <c r="D20" s="12"/>
       <c r="E20" s="12"/>
       <c r="F20" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="G20" s="12"/>
+        <v>47</v>
+      </c>
+      <c r="G20" s="14"/>
       <c r="H20" s="12" t="s">
         <v>40</v>
       </c>
@@ -5014,10 +5015,10 @@
         <v>20</v>
       </c>
       <c r="K20" s="12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="L20" s="8" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -5025,7 +5026,7 @@
         <v>40</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="C21" s="12" t="s">
         <v>18</v>
@@ -5033,7 +5034,7 @@
       <c r="D21" s="12"/>
       <c r="E21" s="12"/>
       <c r="F21" s="12" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G21" s="12"/>
       <c r="H21" s="12" t="s">
@@ -5046,10 +5047,10 @@
         <v>20</v>
       </c>
       <c r="K21" s="12" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="L21" s="8" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
     </row>
     <row r="22" spans="1:12">
@@ -5057,7 +5058,7 @@
         <v>40</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C22" s="12" t="s">
         <v>18</v>
@@ -5065,7 +5066,7 @@
       <c r="D22" s="12"/>
       <c r="E22" s="12"/>
       <c r="F22" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G22" s="12"/>
       <c r="H22" s="12" t="s">
@@ -5078,10 +5079,10 @@
         <v>20</v>
       </c>
       <c r="K22" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L22" s="8" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="23" spans="1:12">
@@ -5089,7 +5090,7 @@
         <v>40</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="C23" s="12" t="s">
         <v>18</v>
@@ -5097,7 +5098,7 @@
       <c r="D23" s="12"/>
       <c r="E23" s="12"/>
       <c r="F23" s="12" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="G23" s="12"/>
       <c r="H23" s="12" t="s">
@@ -5110,10 +5111,10 @@
         <v>20</v>
       </c>
       <c r="K23" s="12" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="L23" s="8" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -5121,7 +5122,7 @@
         <v>40</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="C24" s="12" t="s">
         <v>18</v>
@@ -5129,7 +5130,7 @@
       <c r="D24" s="12"/>
       <c r="E24" s="12"/>
       <c r="F24" s="12" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="G24" s="12"/>
       <c r="H24" s="12" t="s">
@@ -5142,10 +5143,10 @@
         <v>20</v>
       </c>
       <c r="K24" s="12" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="L24" s="8" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="25" spans="1:12">
@@ -5377,15 +5378,15 @@
         <v>58</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="C32" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="D32" s="18"/>
+      <c r="D32" s="12"/>
       <c r="E32" s="12"/>
-      <c r="F32" s="18" t="s">
-        <v>58</v>
+      <c r="F32" s="12" t="s">
+        <v>60</v>
       </c>
       <c r="G32" s="12"/>
       <c r="H32" s="12" t="s">
@@ -5397,11 +5398,11 @@
       <c r="J32" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="K32" s="18" t="s">
-        <v>58</v>
+      <c r="K32" s="12" t="s">
+        <v>60</v>
       </c>
       <c r="L32" s="8" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="33" spans="1:12">
@@ -5409,15 +5410,15 @@
         <v>58</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="C33" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="D33" s="12"/>
+      <c r="D33" s="18"/>
       <c r="E33" s="12"/>
-      <c r="F33" s="12" t="s">
-        <v>60</v>
+      <c r="F33" s="18" t="s">
+        <v>58</v>
       </c>
       <c r="G33" s="12"/>
       <c r="H33" s="12" t="s">
@@ -5429,11 +5430,11 @@
       <c r="J33" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="K33" s="12" t="s">
-        <v>60</v>
+      <c r="K33" s="18" t="s">
+        <v>58</v>
       </c>
       <c r="L33" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="34" spans="1:12">
@@ -5632,26 +5633,26 @@
         <v>77</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="D40" s="12" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E40" s="12"/>
       <c r="F40" s="15"/>
       <c r="G40" s="14"/>
       <c r="H40" s="12"/>
-      <c r="I40" s="12" t="s">
-        <v>72</v>
+      <c r="I40" s="13" t="s">
+        <v>61</v>
       </c>
       <c r="J40" s="12" t="s">
         <v>73</v>
       </c>
       <c r="K40" s="12" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="L40" s="8" t="s">
-        <v>241</v>
+        <v>266</v>
       </c>
     </row>
     <row r="41" spans="1:12">
@@ -5662,26 +5663,26 @@
         <v>77</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D41" s="12"/>
-      <c r="E41" s="12" t="s">
-        <v>117</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="D41" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="E41" s="12"/>
       <c r="F41" s="15"/>
-      <c r="G41" s="12"/>
+      <c r="G41" s="14"/>
       <c r="H41" s="12"/>
-      <c r="I41" s="12" t="s">
-        <v>19</v>
+      <c r="I41" s="13" t="s">
+        <v>61</v>
       </c>
       <c r="J41" s="12" t="s">
         <v>73</v>
       </c>
       <c r="K41" s="12" t="s">
-        <v>117</v>
+        <v>84</v>
       </c>
       <c r="L41" s="8" t="s">
-        <v>242</v>
+        <v>267</v>
       </c>
     </row>
     <row r="42" spans="1:12">
@@ -5692,26 +5693,26 @@
         <v>77</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D42" s="12"/>
-      <c r="E42" s="12" t="s">
-        <v>18</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="D42" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="E42" s="12"/>
       <c r="F42" s="15"/>
-      <c r="G42" s="12"/>
+      <c r="G42" s="14"/>
       <c r="H42" s="12"/>
       <c r="I42" s="12" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="J42" s="12" t="s">
         <v>73</v>
       </c>
       <c r="K42" s="12" t="s">
-        <v>18</v>
+        <v>85</v>
       </c>
       <c r="L42" s="8" t="s">
-        <v>243</v>
+        <v>268</v>
       </c>
     </row>
     <row r="43" spans="1:12">
@@ -5722,14 +5723,14 @@
         <v>77</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D43" s="12" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="E43" s="12"/>
       <c r="F43" s="15"/>
-      <c r="G43" s="12"/>
+      <c r="G43" s="14"/>
       <c r="H43" s="12"/>
       <c r="I43" s="12" t="s">
         <v>61</v>
@@ -5738,10 +5739,10 @@
         <v>73</v>
       </c>
       <c r="K43" s="12" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="L43" s="8" t="s">
-        <v>244</v>
+        <v>269</v>
       </c>
     </row>
     <row r="44" spans="1:12">
@@ -5752,26 +5753,26 @@
         <v>77</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>65</v>
+        <v>23</v>
       </c>
       <c r="D44" s="12" t="s">
-        <v>113</v>
+        <v>87</v>
       </c>
       <c r="E44" s="12"/>
       <c r="F44" s="15"/>
-      <c r="G44" s="12"/>
+      <c r="G44" s="14"/>
       <c r="H44" s="12"/>
       <c r="I44" s="12" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="J44" s="12" t="s">
         <v>73</v>
       </c>
       <c r="K44" s="12" t="s">
-        <v>113</v>
+        <v>87</v>
       </c>
       <c r="L44" s="8" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="45" spans="1:12">
@@ -5782,26 +5783,26 @@
         <v>77</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="D45" s="12" t="s">
-        <v>204</v>
+        <v>88</v>
       </c>
       <c r="E45" s="12"/>
-      <c r="F45" s="18"/>
-      <c r="G45" s="12"/>
+      <c r="F45" s="12"/>
+      <c r="G45" s="14"/>
       <c r="H45" s="12"/>
       <c r="I45" s="12" t="s">
-        <v>39</v>
+        <v>72</v>
       </c>
       <c r="J45" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="K45" s="18" t="s">
-        <v>204</v>
+      <c r="K45" s="12" t="s">
+        <v>88</v>
       </c>
       <c r="L45" s="8" t="s">
-        <v>246</v>
+        <v>255</v>
       </c>
     </row>
     <row r="46" spans="1:12">
@@ -5812,26 +5813,26 @@
         <v>77</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D46" s="12" t="s">
-        <v>206</v>
+        <v>89</v>
       </c>
       <c r="E46" s="12"/>
-      <c r="F46" s="18"/>
+      <c r="F46" s="12"/>
       <c r="G46" s="12"/>
       <c r="H46" s="12"/>
       <c r="I46" s="12" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="J46" s="12" t="s">
         <v>73</v>
       </c>
       <c r="K46" s="12" t="s">
-        <v>206</v>
+        <v>89</v>
       </c>
       <c r="L46" s="8" t="s">
-        <v>247</v>
+        <v>270</v>
       </c>
     </row>
     <row r="47" spans="1:12">
@@ -5842,26 +5843,26 @@
         <v>77</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="D47" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="E47" s="12"/>
+        <v>18</v>
+      </c>
+      <c r="D47" s="12"/>
+      <c r="E47" s="12" t="s">
+        <v>18</v>
+      </c>
       <c r="F47" s="18"/>
       <c r="G47" s="12"/>
       <c r="H47" s="12"/>
       <c r="I47" s="12" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="J47" s="12" t="s">
         <v>73</v>
       </c>
       <c r="K47" s="12" t="s">
-        <v>100</v>
+        <v>18</v>
       </c>
       <c r="L47" s="8" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
     </row>
     <row r="48" spans="1:12">
@@ -5872,26 +5873,26 @@
         <v>77</v>
       </c>
       <c r="C48" s="12" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="D48" s="12" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="E48" s="12"/>
-      <c r="F48" s="18"/>
-      <c r="G48" s="12"/>
+      <c r="F48" s="12"/>
+      <c r="G48" s="14"/>
       <c r="H48" s="12"/>
       <c r="I48" s="12" t="s">
-        <v>39</v>
+        <v>72</v>
       </c>
       <c r="J48" s="12" t="s">
         <v>73</v>
       </c>
       <c r="K48" s="12" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="L48" s="8" t="s">
-        <v>248</v>
+        <v>256</v>
       </c>
     </row>
     <row r="49" spans="1:12">
@@ -5902,26 +5903,26 @@
         <v>77</v>
       </c>
       <c r="C49" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="D49" s="12"/>
+        <v>70</v>
+      </c>
+      <c r="D49" s="12" t="s">
+        <v>91</v>
+      </c>
       <c r="E49" s="12"/>
-      <c r="F49" s="18"/>
-      <c r="G49" s="12" t="s">
-        <v>78</v>
-      </c>
+      <c r="F49" s="12"/>
+      <c r="G49" s="14"/>
       <c r="H49" s="12"/>
       <c r="I49" s="12" t="s">
-        <v>39</v>
+        <v>72</v>
       </c>
       <c r="J49" s="12" t="s">
         <v>73</v>
       </c>
       <c r="K49" s="12" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="L49" s="8" t="s">
-        <v>249</v>
+        <v>257</v>
       </c>
     </row>
     <row r="50" spans="1:12">
@@ -5932,14 +5933,14 @@
         <v>77</v>
       </c>
       <c r="C50" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="D50" s="12"/>
+        <v>37</v>
+      </c>
+      <c r="D50" s="18" t="s">
+        <v>92</v>
+      </c>
       <c r="E50" s="12"/>
-      <c r="F50" s="18"/>
-      <c r="G50" s="12" t="s">
-        <v>79</v>
-      </c>
+      <c r="F50" s="12"/>
+      <c r="G50" s="14"/>
       <c r="H50" s="12"/>
       <c r="I50" s="12" t="s">
         <v>39</v>
@@ -5947,11 +5948,11 @@
       <c r="J50" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="K50" s="12" t="s">
-        <v>79</v>
+      <c r="K50" s="18" t="s">
+        <v>92</v>
       </c>
       <c r="L50" s="8" t="s">
-        <v>250</v>
+        <v>264</v>
       </c>
     </row>
     <row r="51" spans="1:12">
@@ -5962,26 +5963,26 @@
         <v>77</v>
       </c>
       <c r="C51" s="12" t="s">
-        <v>63</v>
+        <v>23</v>
       </c>
       <c r="D51" s="12"/>
-      <c r="E51" s="12"/>
+      <c r="E51" s="12" t="s">
+        <v>117</v>
+      </c>
       <c r="F51" s="18"/>
-      <c r="G51" s="12" t="s">
-        <v>80</v>
-      </c>
+      <c r="G51" s="12"/>
       <c r="H51" s="12"/>
       <c r="I51" s="12" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="J51" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="K51" s="18" t="s">
-        <v>80</v>
+      <c r="K51" s="12" t="s">
+        <v>117</v>
       </c>
       <c r="L51" s="8" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
     </row>
     <row r="52" spans="1:12">
@@ -5992,26 +5993,28 @@
         <v>77</v>
       </c>
       <c r="C52" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="D52" s="12"/>
-      <c r="E52" s="12" t="s">
-        <v>118</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="D52" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="E52" s="12"/>
       <c r="F52" s="18"/>
       <c r="G52" s="12"/>
-      <c r="H52" s="12"/>
+      <c r="H52" s="12" t="s">
+        <v>94</v>
+      </c>
       <c r="I52" s="12" t="s">
-        <v>39</v>
+        <v>72</v>
       </c>
       <c r="J52" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="K52" s="12" t="s">
-        <v>118</v>
+      <c r="K52" s="18" t="s">
+        <v>93</v>
       </c>
       <c r="L52" s="8" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
     </row>
     <row r="53" spans="1:12">
@@ -6022,26 +6025,26 @@
         <v>77</v>
       </c>
       <c r="C53" s="12" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D53" s="12" t="s">
-        <v>112</v>
+        <v>58</v>
       </c>
       <c r="E53" s="12"/>
       <c r="F53" s="18"/>
       <c r="G53" s="12"/>
       <c r="H53" s="12"/>
       <c r="I53" s="12" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="J53" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="K53" s="12" t="s">
-        <v>112</v>
+      <c r="K53" s="18" t="s">
+        <v>58</v>
       </c>
       <c r="L53" s="8" t="s">
-        <v>253</v>
+        <v>271</v>
       </c>
     </row>
     <row r="54" spans="1:12">
@@ -6054,12 +6057,12 @@
       <c r="C54" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="D54" s="12"/>
+      <c r="D54" s="12" t="s">
+        <v>204</v>
+      </c>
       <c r="E54" s="12"/>
       <c r="F54" s="18"/>
-      <c r="G54" s="12" t="s">
-        <v>82</v>
-      </c>
+      <c r="G54" s="12"/>
       <c r="H54" s="12"/>
       <c r="I54" s="12" t="s">
         <v>39</v>
@@ -6067,11 +6070,11 @@
       <c r="J54" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="K54" s="12" t="s">
-        <v>82</v>
+      <c r="K54" s="18" t="s">
+        <v>204</v>
       </c>
       <c r="L54" s="8" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
     </row>
     <row r="55" spans="1:12">
@@ -6085,11 +6088,11 @@
         <v>70</v>
       </c>
       <c r="D55" s="12" t="s">
-        <v>88</v>
+        <v>205</v>
       </c>
       <c r="E55" s="12"/>
       <c r="F55" s="12"/>
-      <c r="G55" s="14"/>
+      <c r="G55" s="12"/>
       <c r="H55" s="12"/>
       <c r="I55" s="12" t="s">
         <v>72</v>
@@ -6098,10 +6101,10 @@
         <v>73</v>
       </c>
       <c r="K55" s="12" t="s">
-        <v>88</v>
+        <v>205</v>
       </c>
       <c r="L55" s="8" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
     </row>
     <row r="56" spans="1:12">
@@ -6112,26 +6115,26 @@
         <v>77</v>
       </c>
       <c r="C56" s="12" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="D56" s="12" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="E56" s="12"/>
       <c r="F56" s="12"/>
-      <c r="G56" s="14"/>
+      <c r="G56" s="12"/>
       <c r="H56" s="12"/>
       <c r="I56" s="12" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="J56" s="12" t="s">
         <v>73</v>
       </c>
       <c r="K56" s="12" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="L56" s="8" t="s">
-        <v>256</v>
+        <v>272</v>
       </c>
     </row>
     <row r="57" spans="1:12">
@@ -6142,26 +6145,26 @@
         <v>77</v>
       </c>
       <c r="C57" s="12" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D57" s="12" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="E57" s="12"/>
-      <c r="F57" s="12"/>
-      <c r="G57" s="14"/>
+      <c r="F57" s="18"/>
+      <c r="G57" s="12"/>
       <c r="H57" s="12"/>
       <c r="I57" s="12" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="J57" s="12" t="s">
         <v>73</v>
       </c>
       <c r="K57" s="12" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="L57" s="8" t="s">
-        <v>257</v>
+        <v>244</v>
       </c>
     </row>
     <row r="58" spans="1:12">
@@ -6172,28 +6175,26 @@
         <v>77</v>
       </c>
       <c r="C58" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="D58" s="18" t="s">
-        <v>93</v>
+        <v>59</v>
+      </c>
+      <c r="D58" s="12" t="s">
+        <v>97</v>
       </c>
       <c r="E58" s="12"/>
-      <c r="F58" s="18"/>
+      <c r="F58" s="12"/>
       <c r="G58" s="12"/>
-      <c r="H58" s="12" t="s">
-        <v>94</v>
-      </c>
+      <c r="H58" s="12"/>
       <c r="I58" s="12" t="s">
-        <v>72</v>
+        <v>39</v>
       </c>
       <c r="J58" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="K58" s="18" t="s">
-        <v>93</v>
+      <c r="K58" s="12" t="s">
+        <v>97</v>
       </c>
       <c r="L58" s="8" t="s">
-        <v>258</v>
+        <v>273</v>
       </c>
     </row>
     <row r="59" spans="1:12">
@@ -6204,26 +6205,26 @@
         <v>77</v>
       </c>
       <c r="C59" s="12" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="D59" s="12" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E59" s="12"/>
-      <c r="F59" s="12"/>
+      <c r="F59" s="18"/>
       <c r="G59" s="12"/>
       <c r="H59" s="12"/>
       <c r="I59" s="12" t="s">
-        <v>72</v>
+        <v>39</v>
       </c>
       <c r="J59" s="12" t="s">
         <v>73</v>
       </c>
       <c r="K59" s="12" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="L59" s="8" t="s">
-        <v>259</v>
+        <v>247</v>
       </c>
     </row>
     <row r="60" spans="1:12">
@@ -6234,26 +6235,26 @@
         <v>77</v>
       </c>
       <c r="C60" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="D60" s="18" t="s">
-        <v>70</v>
+        <v>59</v>
+      </c>
+      <c r="D60" s="12" t="s">
+        <v>98</v>
       </c>
       <c r="E60" s="12"/>
       <c r="F60" s="12"/>
       <c r="G60" s="12"/>
       <c r="H60" s="12"/>
       <c r="I60" s="12" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="J60" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="K60" s="18" t="s">
-        <v>70</v>
+      <c r="K60" s="12" t="s">
+        <v>98</v>
       </c>
       <c r="L60" s="8" t="s">
-        <v>260</v>
+        <v>274</v>
       </c>
     </row>
     <row r="61" spans="1:12">
@@ -6264,28 +6265,26 @@
         <v>77</v>
       </c>
       <c r="C61" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="D61" s="12" t="s">
-        <v>104</v>
+        <v>59</v>
+      </c>
+      <c r="D61" s="18" t="s">
+        <v>99</v>
       </c>
       <c r="E61" s="12"/>
       <c r="F61" s="12"/>
       <c r="G61" s="12"/>
-      <c r="H61" s="12" t="s">
-        <v>94</v>
-      </c>
+      <c r="H61" s="12"/>
       <c r="I61" s="12" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="J61" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="K61" s="12" t="s">
-        <v>104</v>
+      <c r="K61" s="18" t="s">
+        <v>99</v>
       </c>
       <c r="L61" s="8" t="s">
-        <v>261</v>
+        <v>275</v>
       </c>
     </row>
     <row r="62" spans="1:12">
@@ -6296,28 +6295,26 @@
         <v>77</v>
       </c>
       <c r="C62" s="12" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="D62" s="12" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E62" s="12"/>
-      <c r="F62" s="12"/>
+      <c r="F62" s="18"/>
       <c r="G62" s="12"/>
-      <c r="H62" s="12" t="s">
-        <v>94</v>
-      </c>
+      <c r="H62" s="12"/>
       <c r="I62" s="12" t="s">
-        <v>72</v>
+        <v>39</v>
       </c>
       <c r="J62" s="12" t="s">
         <v>73</v>
       </c>
       <c r="K62" s="12" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="L62" s="8" t="s">
-        <v>262</v>
+        <v>240</v>
       </c>
     </row>
     <row r="63" spans="1:12">
@@ -6328,26 +6325,26 @@
         <v>77</v>
       </c>
       <c r="C63" s="12" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="D63" s="12" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="E63" s="12"/>
       <c r="F63" s="12"/>
       <c r="G63" s="12"/>
       <c r="H63" s="12"/>
       <c r="I63" s="12" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="J63" s="12" t="s">
         <v>73</v>
       </c>
       <c r="K63" s="12" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="L63" s="8" t="s">
-        <v>263</v>
+        <v>276</v>
       </c>
     </row>
     <row r="64" spans="1:12">
@@ -6358,26 +6355,26 @@
         <v>77</v>
       </c>
       <c r="C64" s="12" t="s">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="D64" s="16" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
       <c r="E64" s="12"/>
       <c r="F64" s="12"/>
-      <c r="G64" s="14"/>
+      <c r="G64" s="12"/>
       <c r="H64" s="12"/>
       <c r="I64" s="12" t="s">
-        <v>39</v>
+        <v>72</v>
       </c>
       <c r="J64" s="12" t="s">
         <v>73</v>
       </c>
       <c r="K64" s="16" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
       <c r="L64" s="8" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
     </row>
     <row r="65" spans="1:12">
@@ -6388,26 +6385,26 @@
         <v>77</v>
       </c>
       <c r="C65" s="12" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="D65" s="12" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E65" s="12"/>
       <c r="F65" s="12"/>
       <c r="G65" s="12"/>
       <c r="H65" s="12"/>
       <c r="I65" s="12" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="J65" s="12" t="s">
         <v>73</v>
       </c>
       <c r="K65" s="12" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="L65" s="8" t="s">
-        <v>265</v>
+        <v>277</v>
       </c>
     </row>
     <row r="66" spans="1:12">
@@ -6421,23 +6418,23 @@
         <v>59</v>
       </c>
       <c r="D66" s="12" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="E66" s="12"/>
-      <c r="F66" s="18"/>
-      <c r="G66" s="14"/>
+      <c r="F66" s="12"/>
+      <c r="G66" s="12"/>
       <c r="H66" s="12"/>
-      <c r="I66" s="13" t="s">
+      <c r="I66" s="12" t="s">
         <v>61</v>
       </c>
       <c r="J66" s="12" t="s">
         <v>73</v>
       </c>
       <c r="K66" s="12" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="L66" s="8" t="s">
-        <v>266</v>
+        <v>278</v>
       </c>
     </row>
     <row r="67" spans="1:12">
@@ -6448,26 +6445,28 @@
         <v>77</v>
       </c>
       <c r="C67" s="12" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="D67" s="12" t="s">
-        <v>84</v>
+        <v>104</v>
       </c>
       <c r="E67" s="12"/>
-      <c r="F67" s="18"/>
-      <c r="G67" s="14"/>
-      <c r="H67" s="12"/>
-      <c r="I67" s="13" t="s">
-        <v>61</v>
+      <c r="F67" s="12"/>
+      <c r="G67" s="12"/>
+      <c r="H67" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="I67" s="12" t="s">
+        <v>72</v>
       </c>
       <c r="J67" s="12" t="s">
         <v>73</v>
       </c>
       <c r="K67" s="12" t="s">
-        <v>84</v>
+        <v>104</v>
       </c>
       <c r="L67" s="8" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
     </row>
     <row r="68" spans="1:12">
@@ -6478,26 +6477,28 @@
         <v>77</v>
       </c>
       <c r="C68" s="12" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="D68" s="12" t="s">
-        <v>85</v>
+        <v>105</v>
       </c>
       <c r="E68" s="12"/>
-      <c r="F68" s="18"/>
-      <c r="G68" s="14"/>
-      <c r="H68" s="12"/>
+      <c r="F68" s="12"/>
+      <c r="G68" s="12"/>
+      <c r="H68" s="12" t="s">
+        <v>94</v>
+      </c>
       <c r="I68" s="12" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="J68" s="12" t="s">
         <v>73</v>
       </c>
       <c r="K68" s="12" t="s">
-        <v>85</v>
+        <v>105</v>
       </c>
       <c r="L68" s="8" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="69" spans="1:12">
@@ -6508,26 +6509,26 @@
         <v>77</v>
       </c>
       <c r="C69" s="12" t="s">
-        <v>59</v>
+        <v>37</v>
       </c>
       <c r="D69" s="12" t="s">
-        <v>86</v>
+        <v>106</v>
       </c>
       <c r="E69" s="12"/>
-      <c r="F69" s="18"/>
-      <c r="G69" s="14"/>
+      <c r="F69" s="12"/>
+      <c r="G69" s="12"/>
       <c r="H69" s="12"/>
       <c r="I69" s="12" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="J69" s="12" t="s">
         <v>73</v>
       </c>
       <c r="K69" s="12" t="s">
-        <v>86</v>
+        <v>106</v>
       </c>
       <c r="L69" s="8" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="70" spans="1:12">
@@ -6538,26 +6539,26 @@
         <v>77</v>
       </c>
       <c r="C70" s="12" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="D70" s="12" t="s">
-        <v>89</v>
+        <v>107</v>
       </c>
       <c r="E70" s="12"/>
       <c r="F70" s="12"/>
       <c r="G70" s="12"/>
       <c r="H70" s="12"/>
       <c r="I70" s="12" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="J70" s="12" t="s">
         <v>73</v>
       </c>
       <c r="K70" s="12" t="s">
-        <v>89</v>
+        <v>107</v>
       </c>
       <c r="L70" s="8" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
     </row>
     <row r="71" spans="1:12">
@@ -6568,26 +6569,26 @@
         <v>77</v>
       </c>
       <c r="C71" s="12" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D71" s="12" t="s">
-        <v>58</v>
+        <v>108</v>
       </c>
       <c r="E71" s="12"/>
       <c r="F71" s="18"/>
       <c r="G71" s="12"/>
       <c r="H71" s="12"/>
       <c r="I71" s="12" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="J71" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="K71" s="18" t="s">
-        <v>58</v>
+      <c r="K71" s="12" t="s">
+        <v>108</v>
       </c>
       <c r="L71" s="8" t="s">
-        <v>271</v>
+        <v>248</v>
       </c>
     </row>
     <row r="72" spans="1:12">
@@ -6598,26 +6599,26 @@
         <v>77</v>
       </c>
       <c r="C72" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="D72" s="12" t="s">
-        <v>95</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="D72" s="12"/>
       <c r="E72" s="12"/>
-      <c r="F72" s="12"/>
-      <c r="G72" s="12"/>
+      <c r="F72" s="18"/>
+      <c r="G72" s="12" t="s">
+        <v>78</v>
+      </c>
       <c r="H72" s="12"/>
       <c r="I72" s="12" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="J72" s="12" t="s">
         <v>73</v>
       </c>
       <c r="K72" s="12" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="L72" s="8" t="s">
-        <v>272</v>
+        <v>249</v>
       </c>
     </row>
     <row r="73" spans="1:12">
@@ -6631,23 +6632,23 @@
         <v>59</v>
       </c>
       <c r="D73" s="12" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="E73" s="12"/>
       <c r="F73" s="12"/>
       <c r="G73" s="12"/>
       <c r="H73" s="12"/>
       <c r="I73" s="12" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="J73" s="12" t="s">
         <v>73</v>
       </c>
       <c r="K73" s="12" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="L73" s="8" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
     </row>
     <row r="74" spans="1:12">
@@ -6658,26 +6659,26 @@
         <v>77</v>
       </c>
       <c r="C74" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="D74" s="12" t="s">
-        <v>98</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="D74" s="12"/>
       <c r="E74" s="12"/>
-      <c r="F74" s="12"/>
-      <c r="G74" s="12"/>
+      <c r="F74" s="18"/>
+      <c r="G74" s="12" t="s">
+        <v>79</v>
+      </c>
       <c r="H74" s="12"/>
       <c r="I74" s="12" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="J74" s="12" t="s">
         <v>73</v>
       </c>
       <c r="K74" s="12" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="L74" s="8" t="s">
-        <v>274</v>
+        <v>250</v>
       </c>
     </row>
     <row r="75" spans="1:12">
@@ -6688,26 +6689,26 @@
         <v>77</v>
       </c>
       <c r="C75" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="D75" s="18" t="s">
-        <v>99</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="D75" s="12"/>
       <c r="E75" s="12"/>
-      <c r="F75" s="12"/>
-      <c r="G75" s="12"/>
+      <c r="F75" s="18"/>
+      <c r="G75" s="12" t="s">
+        <v>80</v>
+      </c>
       <c r="H75" s="12"/>
       <c r="I75" s="12" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="J75" s="12" t="s">
         <v>73</v>
       </c>
       <c r="K75" s="18" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="L75" s="8" t="s">
-        <v>275</v>
+        <v>251</v>
       </c>
     </row>
     <row r="76" spans="1:12">
@@ -6721,10 +6722,10 @@
         <v>59</v>
       </c>
       <c r="D76" s="12" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="E76" s="12"/>
-      <c r="F76" s="12"/>
+      <c r="F76" s="18"/>
       <c r="G76" s="12"/>
       <c r="H76" s="12"/>
       <c r="I76" s="12" t="s">
@@ -6733,11 +6734,11 @@
       <c r="J76" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="K76" s="12" t="s">
-        <v>101</v>
+      <c r="K76" s="18" t="s">
+        <v>110</v>
       </c>
       <c r="L76" s="8" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
     </row>
     <row r="77" spans="1:12">
@@ -6750,24 +6751,24 @@
       <c r="C77" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="D77" s="12" t="s">
-        <v>102</v>
-      </c>
+      <c r="D77" s="12"/>
       <c r="E77" s="12"/>
-      <c r="F77" s="12"/>
-      <c r="G77" s="12"/>
+      <c r="F77" s="18"/>
+      <c r="G77" s="12" t="s">
+        <v>81</v>
+      </c>
       <c r="H77" s="12"/>
       <c r="I77" s="12" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="J77" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="K77" s="12" t="s">
-        <v>102</v>
+      <c r="K77" s="18" t="s">
+        <v>81</v>
       </c>
       <c r="L77" s="8" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
     </row>
     <row r="78" spans="1:12">
@@ -6778,26 +6779,26 @@
         <v>77</v>
       </c>
       <c r="C78" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="D78" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="E78" s="12"/>
-      <c r="F78" s="12"/>
+        <v>63</v>
+      </c>
+      <c r="D78" s="12"/>
+      <c r="E78" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="F78" s="18"/>
       <c r="G78" s="12"/>
       <c r="H78" s="12"/>
       <c r="I78" s="12" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="J78" s="12" t="s">
         <v>73</v>
       </c>
       <c r="K78" s="12" t="s">
-        <v>103</v>
+        <v>118</v>
       </c>
       <c r="L78" s="8" t="s">
-        <v>278</v>
+        <v>252</v>
       </c>
     </row>
     <row r="79" spans="1:12">
@@ -6811,10 +6812,10 @@
         <v>59</v>
       </c>
       <c r="D79" s="12" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="E79" s="12"/>
-      <c r="F79" s="12"/>
+      <c r="F79" s="18"/>
       <c r="G79" s="12"/>
       <c r="H79" s="12"/>
       <c r="I79" s="12" t="s">
@@ -6824,10 +6825,10 @@
         <v>73</v>
       </c>
       <c r="K79" s="12" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="L79" s="8" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
     </row>
     <row r="80" spans="1:12">
@@ -6838,26 +6839,26 @@
         <v>77</v>
       </c>
       <c r="C80" s="12" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D80" s="12" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E80" s="12"/>
       <c r="F80" s="18"/>
       <c r="G80" s="12"/>
       <c r="H80" s="12"/>
       <c r="I80" s="12" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="J80" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="K80" s="18" t="s">
-        <v>110</v>
+      <c r="K80" s="12" t="s">
+        <v>112</v>
       </c>
       <c r="L80" s="8" t="s">
-        <v>280</v>
+        <v>253</v>
       </c>
     </row>
     <row r="81" spans="1:12">
@@ -6868,26 +6869,26 @@
         <v>77</v>
       </c>
       <c r="C81" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="D81" s="12"/>
+        <v>65</v>
+      </c>
+      <c r="D81" s="12" t="s">
+        <v>113</v>
+      </c>
       <c r="E81" s="12"/>
       <c r="F81" s="18"/>
-      <c r="G81" s="12" t="s">
-        <v>81</v>
-      </c>
+      <c r="G81" s="12"/>
       <c r="H81" s="12"/>
       <c r="I81" s="12" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="J81" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="K81" s="18" t="s">
-        <v>81</v>
+      <c r="K81" s="12" t="s">
+        <v>113</v>
       </c>
       <c r="L81" s="8" t="s">
-        <v>281</v>
+        <v>245</v>
       </c>
     </row>
     <row r="82" spans="1:12">
@@ -6901,7 +6902,7 @@
         <v>59</v>
       </c>
       <c r="D82" s="12" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="E82" s="12"/>
       <c r="F82" s="18"/>
@@ -6914,10 +6915,10 @@
         <v>73</v>
       </c>
       <c r="K82" s="12" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="L82" s="8" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="83" spans="1:12">
@@ -6931,10 +6932,10 @@
         <v>59</v>
       </c>
       <c r="D83" s="12" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E83" s="12"/>
-      <c r="F83" s="18"/>
+      <c r="F83" s="12"/>
       <c r="G83" s="12"/>
       <c r="H83" s="12"/>
       <c r="I83" s="12" t="s">
@@ -6944,10 +6945,10 @@
         <v>73</v>
       </c>
       <c r="K83" s="12" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="L83" s="8" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="84" spans="1:12">
@@ -6958,26 +6959,26 @@
         <v>77</v>
       </c>
       <c r="C84" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="D84" s="12" t="s">
-        <v>115</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="D84" s="12"/>
       <c r="E84" s="12"/>
-      <c r="F84" s="12"/>
-      <c r="G84" s="12"/>
+      <c r="F84" s="18"/>
+      <c r="G84" s="12" t="s">
+        <v>82</v>
+      </c>
       <c r="H84" s="12"/>
       <c r="I84" s="12" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="J84" s="12" t="s">
         <v>73</v>
       </c>
       <c r="K84" s="12" t="s">
-        <v>115</v>
+        <v>82</v>
       </c>
       <c r="L84" s="8" t="s">
-        <v>284</v>
+        <v>254</v>
       </c>
     </row>
     <row r="85" spans="1:12">
@@ -7297,7 +7298,7 @@
         <v>127</v>
       </c>
       <c r="B95" s="12" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="C95" s="12" t="s">
         <v>70</v>
@@ -7305,7 +7306,7 @@
       <c r="D95" s="12"/>
       <c r="E95" s="12"/>
       <c r="F95" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G95" s="12"/>
       <c r="H95" s="12" t="s">
@@ -7318,10 +7319,10 @@
         <v>20</v>
       </c>
       <c r="K95" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L95" s="8" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
     </row>
     <row r="96" spans="1:12">
@@ -7337,7 +7338,7 @@
       <c r="D96" s="12"/>
       <c r="E96" s="12"/>
       <c r="F96" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G96" s="12"/>
       <c r="H96" s="12" t="s">
@@ -7350,10 +7351,10 @@
         <v>20</v>
       </c>
       <c r="K96" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L96" s="8" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="97" spans="1:12">
@@ -7361,7 +7362,7 @@
         <v>127</v>
       </c>
       <c r="B97" s="12" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="C97" s="12" t="s">
         <v>70</v>
@@ -7369,7 +7370,7 @@
       <c r="D97" s="12"/>
       <c r="E97" s="12"/>
       <c r="F97" s="12" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="G97" s="12"/>
       <c r="H97" s="12" t="s">
@@ -7382,10 +7383,10 @@
         <v>20</v>
       </c>
       <c r="K97" s="12" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="L97" s="8" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="98" spans="1:12">
@@ -7521,15 +7522,15 @@
         <v>203</v>
       </c>
       <c r="B102" s="12" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="C102" s="12" t="s">
         <v>70</v>
       </c>
       <c r="D102" s="12"/>
       <c r="E102" s="12"/>
-      <c r="F102" s="18" t="s">
-        <v>140</v>
+      <c r="F102" s="12" t="s">
+        <v>139</v>
       </c>
       <c r="G102" s="12"/>
       <c r="H102" s="12" t="s">
@@ -7542,10 +7543,10 @@
         <v>20</v>
       </c>
       <c r="K102" s="12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L102" s="8" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="103" spans="1:12">
@@ -7553,15 +7554,15 @@
         <v>203</v>
       </c>
       <c r="B103" s="12" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="C103" s="12" t="s">
         <v>70</v>
       </c>
       <c r="D103" s="12"/>
       <c r="E103" s="12"/>
-      <c r="F103" s="12" t="s">
-        <v>139</v>
+      <c r="F103" s="18" t="s">
+        <v>140</v>
       </c>
       <c r="G103" s="12"/>
       <c r="H103" s="12" t="s">
@@ -7574,10 +7575,10 @@
         <v>20</v>
       </c>
       <c r="K103" s="12" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="L103" s="8" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="104" spans="1:12">
@@ -7802,14 +7803,14 @@
         <v>151</v>
       </c>
       <c r="C111" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="D111" s="12"/>
+        <v>37</v>
+      </c>
+      <c r="D111" s="12" t="s">
+        <v>156</v>
+      </c>
       <c r="E111" s="12"/>
-      <c r="F111" s="18"/>
-      <c r="G111" s="12" t="s">
-        <v>152</v>
-      </c>
+      <c r="F111" s="12"/>
+      <c r="G111" s="12"/>
       <c r="H111" s="12"/>
       <c r="I111" s="12" t="s">
         <v>39</v>
@@ -7818,10 +7819,10 @@
         <v>73</v>
       </c>
       <c r="K111" s="12" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="L111" s="8" t="s">
-        <v>311</v>
+        <v>316</v>
       </c>
     </row>
     <row r="112" spans="1:12">
@@ -7832,10 +7833,10 @@
         <v>151</v>
       </c>
       <c r="C112" s="12" t="s">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="D112" s="12" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E112" s="12"/>
       <c r="F112" s="12"/>
@@ -7848,10 +7849,10 @@
         <v>73</v>
       </c>
       <c r="K112" s="12" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="L112" s="8" t="s">
-        <v>312</v>
+        <v>317</v>
       </c>
     </row>
     <row r="113" spans="1:12">
@@ -7866,9 +7867,9 @@
       </c>
       <c r="D113" s="12"/>
       <c r="E113" s="12"/>
-      <c r="F113" s="12"/>
+      <c r="F113" s="18"/>
       <c r="G113" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H113" s="12"/>
       <c r="I113" s="12" t="s">
@@ -7878,10 +7879,10 @@
         <v>73</v>
       </c>
       <c r="K113" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="L113" s="8" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="114" spans="1:12">
@@ -7892,14 +7893,14 @@
         <v>151</v>
       </c>
       <c r="C114" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="D114" s="12"/>
+        <v>37</v>
+      </c>
+      <c r="D114" s="12" t="s">
+        <v>158</v>
+      </c>
       <c r="E114" s="12"/>
       <c r="F114" s="12"/>
-      <c r="G114" s="12" t="s">
-        <v>154</v>
-      </c>
+      <c r="G114" s="12"/>
       <c r="H114" s="12"/>
       <c r="I114" s="12" t="s">
         <v>39</v>
@@ -7908,10 +7909,10 @@
         <v>73</v>
       </c>
       <c r="K114" s="12" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="L114" s="8" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
     </row>
     <row r="115" spans="1:12">
@@ -7922,14 +7923,14 @@
         <v>151</v>
       </c>
       <c r="C115" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="D115" s="12"/>
+        <v>37</v>
+      </c>
+      <c r="D115" s="12" t="s">
+        <v>159</v>
+      </c>
       <c r="E115" s="12"/>
       <c r="F115" s="12"/>
-      <c r="G115" s="12" t="s">
-        <v>155</v>
-      </c>
+      <c r="G115" s="12"/>
       <c r="H115" s="12"/>
       <c r="I115" s="12" t="s">
         <v>39</v>
@@ -7938,10 +7939,10 @@
         <v>73</v>
       </c>
       <c r="K115" s="12" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="L115" s="8" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
     </row>
     <row r="116" spans="1:12">
@@ -7952,10 +7953,10 @@
         <v>151</v>
       </c>
       <c r="C116" s="12" t="s">
-        <v>37</v>
+        <v>63</v>
       </c>
       <c r="D116" s="12" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="E116" s="12"/>
       <c r="F116" s="12"/>
@@ -7968,10 +7969,10 @@
         <v>73</v>
       </c>
       <c r="K116" s="12" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="L116" s="8" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="117" spans="1:12">
@@ -7982,14 +7983,14 @@
         <v>151</v>
       </c>
       <c r="C117" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="D117" s="12" t="s">
-        <v>157</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="D117" s="12"/>
       <c r="E117" s="12"/>
       <c r="F117" s="12"/>
-      <c r="G117" s="12"/>
+      <c r="G117" s="12" t="s">
+        <v>153</v>
+      </c>
       <c r="H117" s="12"/>
       <c r="I117" s="12" t="s">
         <v>39</v>
@@ -7998,10 +7999,10 @@
         <v>73</v>
       </c>
       <c r="K117" s="12" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="L117" s="8" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
     </row>
     <row r="118" spans="1:12">
@@ -8015,7 +8016,7 @@
         <v>37</v>
       </c>
       <c r="D118" s="12" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="E118" s="12"/>
       <c r="F118" s="12"/>
@@ -8028,10 +8029,10 @@
         <v>73</v>
       </c>
       <c r="K118" s="12" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="L118" s="8" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
     </row>
     <row r="119" spans="1:12">
@@ -8042,14 +8043,14 @@
         <v>151</v>
       </c>
       <c r="C119" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="D119" s="12" t="s">
-        <v>159</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="D119" s="12"/>
       <c r="E119" s="12"/>
       <c r="F119" s="12"/>
-      <c r="G119" s="12"/>
+      <c r="G119" s="12" t="s">
+        <v>154</v>
+      </c>
       <c r="H119" s="12"/>
       <c r="I119" s="12" t="s">
         <v>39</v>
@@ -8058,10 +8059,10 @@
         <v>73</v>
       </c>
       <c r="K119" s="12" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="L119" s="8" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
     </row>
     <row r="120" spans="1:12">
@@ -8072,14 +8073,14 @@
         <v>151</v>
       </c>
       <c r="C120" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="D120" s="12" t="s">
-        <v>161</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="D120" s="12"/>
       <c r="E120" s="12"/>
       <c r="F120" s="12"/>
-      <c r="G120" s="12"/>
+      <c r="G120" s="12" t="s">
+        <v>155</v>
+      </c>
       <c r="H120" s="12"/>
       <c r="I120" s="12" t="s">
         <v>39</v>
@@ -8088,10 +8089,10 @@
         <v>73</v>
       </c>
       <c r="K120" s="12" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="L120" s="8" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
     </row>
     <row r="121" spans="1:12">
@@ -8223,7 +8224,11 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L1"/>
+  <autoFilter ref="A1:L1">
+    <sortState ref="A2:L124">
+      <sortCondition ref="A1:A124"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>

<commit_message>
Add credential, industry, and division vocabularies
</commit_message>
<xml_diff>
--- a/_data/_data.xlsx
+++ b/_data/_data.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26330"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1820" yWindow="60" windowWidth="32280" windowHeight="19580" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16160" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="navigation" sheetId="4" r:id="rId1"/>
     <sheet name="programs" sheetId="1" r:id="rId2"/>
     <sheet name="planning-guides" sheetId="5" r:id="rId3"/>
+    <sheet name="vocabularies" sheetId="6" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">navigation!$A$1:$F$1</definedName>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1316" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1340" uniqueCount="329">
   <si>
     <t>label</t>
   </si>
@@ -1025,7 +1026,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="128"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1125,7 +1126,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="289">
+  <cellStyleXfs count="301">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1188,6 +1189,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1472,7 +1485,7 @@
       <alignment horizontal="right" vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="289">
+  <cellStyles count="301">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1626,6 +1639,12 @@
     <cellStyle name="Followed Hyperlink" xfId="284" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="286" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="288" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="290" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="292" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="294" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="296" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="298" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="300" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1761,6 +1780,12 @@
     <cellStyle name="Hyperlink" xfId="283" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="285" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="287" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="289" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="291" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="293" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="295" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="297" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="299" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2028,7 +2053,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2188,7 +2213,7 @@
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4356,9 +4381,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L124"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C101" activeCellId="5" sqref="C15:C16 C35 C39 C61 C87 C101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8237,4 +8262,165 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C21"/>
+  <sheetViews>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="2" max="2" width="36" customWidth="1"/>
+    <col min="3" max="3" width="48" customWidth="1"/>
+    <col min="4" max="7" width="24" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="12"/>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="12"/>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="12"/>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="12"/>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="B11" s="12"/>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+    </row>
+    <row r="17" spans="2:3">
+      <c r="B17" s="12"/>
+    </row>
+    <row r="18" spans="2:3">
+      <c r="C18" s="12"/>
+    </row>
+    <row r="19" spans="2:3">
+      <c r="C19" s="12"/>
+    </row>
+    <row r="20" spans="2:3">
+      <c r="C20" s="12"/>
+    </row>
+    <row r="21" spans="2:3">
+      <c r="C21" s="12"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Remove "Pathways" from prototype (by removing them from _data.xlsx)
</commit_message>
<xml_diff>
--- a/_data/_data.xlsx
+++ b/_data/_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26330"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16160" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="0" windowWidth="37340" windowHeight="19300" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="navigation" sheetId="4" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'planning-guides'!$A$1:$L$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">programs!$A$1:$L$124</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001" refMode="R1C1" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1340" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1268" uniqueCount="313">
   <si>
     <t>label</t>
   </si>
@@ -266,18 +266,6 @@
     <t>occupational therapy</t>
   </si>
   <si>
-    <t>physical therapy</t>
-  </si>
-  <si>
-    <t>physician assistant</t>
-  </si>
-  <si>
-    <t>pre-law</t>
-  </si>
-  <si>
-    <t>speech and hearing sciences</t>
-  </si>
-  <si>
     <t>african studies</t>
   </si>
   <si>
@@ -488,15 +476,6 @@
     <t>dentistry</t>
   </si>
   <si>
-    <t>medicine</t>
-  </si>
-  <si>
-    <t>pharmacy</t>
-  </si>
-  <si>
-    <t>veterinary medicine</t>
-  </si>
-  <si>
     <t>biological sciences</t>
   </si>
   <si>
@@ -776,24 +755,12 @@
     <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MPS-AA-Nutrition-and-Food-Science.pdf</t>
   </si>
   <si>
-    <t>http://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MPS-AA-Occupational-Therapy.pdf</t>
-  </si>
-  <si>
-    <t>http://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MPS-AA-Physical-Therapy.pdf</t>
-  </si>
-  <si>
-    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MPS-AA-Physician-Assistant.pdf</t>
-  </si>
-  <si>
     <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/AA-Pre-Nursing-MRP.pdf</t>
   </si>
   <si>
     <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MPS-AA-Public-and-Community-Health.pdf</t>
   </si>
   <si>
-    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MPS-AA-Speech-and-Hearing-Sciences.pdf</t>
-  </si>
-  <si>
     <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MPS-AA-Art-History.pdf</t>
   </si>
   <si>
@@ -872,9 +839,6 @@
     <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MPS-AA-Political-Science.pdf</t>
   </si>
   <si>
-    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MPS-AA-Pre-Law.pdf</t>
-  </si>
-  <si>
     <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MPS-AA-Psychology.pdf</t>
   </si>
   <si>
@@ -962,19 +926,7 @@
     <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MPS-AST2-Physics.pdf</t>
   </si>
   <si>
-    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MPS-AST1-Dentistry-Pathway.pdf</t>
-  </si>
-  <si>
     <t>http://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MPS-AST1-Medical-Laboratory-Science-Pathway.pdf</t>
-  </si>
-  <si>
-    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MPS-AST1-Medicine-Pathway.pdf</t>
-  </si>
-  <si>
-    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MPS-AST1-Pharmacy-Pathway.pdf</t>
-  </si>
-  <si>
-    <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MPS-AST1-Veterinary-Medicine-Pathway.pdf</t>
   </si>
   <si>
     <t>https://www.shoreline.edu/areas-of-study/documents/majorPlanningSheets/MPS-AST1-Biological-Science.pdf</t>
@@ -1026,7 +978,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="134"/>
+      <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2053,7 +2005,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2088,10 +2040,10 @@
         <v>3</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>1</v>
@@ -2099,7 +2051,7 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>4</v>
@@ -2108,20 +2060,20 @@
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="2" t="s">
-        <v>328</v>
+        <v>312</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="17" t="s">
-        <v>327</v>
+        <v>311</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -2129,10 +2081,10 @@
     <row r="4" spans="1:8">
       <c r="A4" s="17"/>
       <c r="D4" s="5" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -2158,7 +2110,7 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>4</v>
@@ -2167,12 +2119,12 @@
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" t="s">
-        <v>328</v>
+        <v>312</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>4</v>
@@ -2181,18 +2133,18 @@
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" t="s">
-        <v>328</v>
+        <v>312</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>4</v>
       </c>
       <c r="F10" t="s">
-        <v>328</v>
+        <v>312</v>
       </c>
     </row>
   </sheetData>
@@ -2211,7 +2163,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M124"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -2242,10 +2194,10 @@
         <v>14</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="G1" s="11" t="s">
         <v>6</v>
@@ -2280,10 +2232,10 @@
         <v>20</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="G2" s="12" t="s">
         <v>17</v>
@@ -2298,7 +2250,7 @@
       </c>
       <c r="L2" s="14"/>
       <c r="M2" s="8" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -2315,10 +2267,10 @@
         <v>20</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="G3" s="12" t="s">
         <v>22</v>
@@ -2333,7 +2285,7 @@
       </c>
       <c r="L3" s="12"/>
       <c r="M3" s="8" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -2350,10 +2302,10 @@
         <v>20</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="G4" s="12" t="s">
         <v>17</v>
@@ -2368,7 +2320,7 @@
       </c>
       <c r="L4" s="12"/>
       <c r="M4" s="8" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -2385,10 +2337,10 @@
         <v>20</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="G5" s="12" t="s">
         <v>17</v>
@@ -2403,7 +2355,7 @@
       </c>
       <c r="L5" s="14"/>
       <c r="M5" s="8" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -2420,10 +2372,10 @@
         <v>20</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="G6" s="12" t="s">
         <v>17</v>
@@ -2438,7 +2390,7 @@
       </c>
       <c r="L6" s="12"/>
       <c r="M6" s="8" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -2455,10 +2407,10 @@
         <v>20</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="G7" s="12" t="s">
         <v>17</v>
@@ -2473,7 +2425,7 @@
       </c>
       <c r="L7" s="12"/>
       <c r="M7" s="8" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -2490,10 +2442,10 @@
         <v>20</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="G8" s="12" t="s">
         <v>45</v>
@@ -2508,7 +2460,7 @@
       </c>
       <c r="L8" s="12"/>
       <c r="M8" s="8" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -2525,10 +2477,10 @@
         <v>20</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="G9" s="12" t="s">
         <v>17</v>
@@ -2543,7 +2495,7 @@
       </c>
       <c r="L9" s="12"/>
       <c r="M9" s="8" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -2560,10 +2512,10 @@
         <v>20</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="G10" s="12" t="s">
         <v>17</v>
@@ -2578,7 +2530,7 @@
       </c>
       <c r="L10" s="12"/>
       <c r="M10" s="8" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -2595,10 +2547,10 @@
         <v>73</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="G11" s="12" t="s">
         <v>69</v>
@@ -2611,7 +2563,7 @@
       </c>
       <c r="L11" s="12"/>
       <c r="M11" s="8" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
     </row>
     <row r="12" spans="1:13">
@@ -2628,10 +2580,10 @@
         <v>20</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="G12" s="12" t="s">
         <v>17</v>
@@ -2646,7 +2598,7 @@
       </c>
       <c r="L12" s="14"/>
       <c r="M12" s="8" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
     </row>
     <row r="13" spans="1:13">
@@ -2663,10 +2615,10 @@
         <v>73</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="G13" s="12" t="s">
         <v>77</v>
@@ -2679,12 +2631,12 @@
         <v>78</v>
       </c>
       <c r="M13" s="8" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
     </row>
     <row r="14" spans="1:13">
       <c r="A14" s="12" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B14" s="12" t="s">
         <v>23</v>
@@ -2696,30 +2648,30 @@
         <v>20</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="G14" s="12" t="s">
         <v>17</v>
       </c>
       <c r="H14" s="12" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="I14" s="12"/>
       <c r="J14" s="12"/>
       <c r="K14" s="12" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="L14" s="12"/>
       <c r="M14" s="8" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
     </row>
     <row r="15" spans="1:13">
       <c r="A15" s="12" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B15" s="12" t="s">
         <v>63</v>
@@ -2731,30 +2683,30 @@
         <v>20</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="G15" s="12" t="s">
         <v>17</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="I15" s="12"/>
       <c r="J15" s="12"/>
       <c r="K15" s="12" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="L15" s="12"/>
       <c r="M15" s="8" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
     </row>
     <row r="16" spans="1:13">
       <c r="A16" s="12" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B16" s="12" t="s">
         <v>70</v>
@@ -2766,28 +2718,28 @@
         <v>73</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="H16" s="12"/>
       <c r="I16" s="12"/>
       <c r="J16" s="12"/>
       <c r="K16" s="12" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="L16" s="12"/>
       <c r="M16" s="8" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
     </row>
     <row r="17" spans="1:13">
       <c r="A17" s="12" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B17" s="12" t="s">
         <v>70</v>
@@ -2799,30 +2751,30 @@
         <v>20</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="G17" s="12" t="s">
         <v>17</v>
       </c>
       <c r="H17" s="12" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="I17" s="12"/>
       <c r="J17" s="12"/>
       <c r="K17" s="12" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="L17" s="12"/>
       <c r="M17" s="8" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
     </row>
     <row r="18" spans="1:13" s="7" customFormat="1">
       <c r="A18" s="12" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B18" s="12" t="s">
         <v>63</v>
@@ -2834,30 +2786,30 @@
         <v>20</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="G18" s="12" t="s">
         <v>17</v>
       </c>
       <c r="H18" s="12" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="I18" s="12"/>
       <c r="J18" s="12"/>
       <c r="K18" s="12" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="L18" s="14"/>
       <c r="M18" s="8" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
     </row>
     <row r="19" spans="1:13">
       <c r="A19" s="12" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B19" s="12" t="s">
         <v>59</v>
@@ -2869,30 +2821,30 @@
         <v>20</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="G19" s="12" t="s">
         <v>45</v>
       </c>
       <c r="H19" s="12" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="I19" s="12"/>
       <c r="J19" s="12"/>
       <c r="K19" s="12" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="L19" s="12"/>
       <c r="M19" s="8" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
     </row>
     <row r="20" spans="1:13">
       <c r="A20" s="12" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="B20" s="12" t="s">
         <v>70</v>
@@ -2904,30 +2856,30 @@
         <v>20</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="G20" s="12" t="s">
         <v>30</v>
       </c>
       <c r="H20" s="12" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="I20" s="12"/>
       <c r="J20" s="12"/>
       <c r="K20" s="12" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="L20" s="12"/>
       <c r="M20" s="8" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
     </row>
     <row r="21" spans="1:13">
       <c r="A21" s="12" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B21" s="12" t="s">
         <v>18</v>
@@ -2939,30 +2891,30 @@
         <v>20</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="G21" s="12" t="s">
         <v>17</v>
       </c>
       <c r="H21" s="12" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="I21" s="12"/>
       <c r="J21" s="12"/>
       <c r="K21" s="12" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="L21" s="12"/>
       <c r="M21" s="8" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
     </row>
     <row r="22" spans="1:13">
       <c r="A22" s="12" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B22" s="12" t="s">
         <v>37</v>
@@ -2974,28 +2926,28 @@
         <v>73</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="G22" s="12" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="H22" s="12"/>
       <c r="I22" s="12" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="J22" s="12"/>
       <c r="K22" s="12"/>
       <c r="L22" s="12"/>
       <c r="M22" s="8" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
     </row>
     <row r="23" spans="1:13">
       <c r="A23" s="12" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B23" s="12" t="s">
         <v>37</v>
@@ -3007,28 +2959,28 @@
         <v>73</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="G23" s="12" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="H23" s="12"/>
       <c r="I23" s="12"/>
       <c r="J23" s="12"/>
       <c r="K23" s="12"/>
       <c r="L23" s="12" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="M23" s="8" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
     </row>
     <row r="24" spans="1:13">
       <c r="A24" s="12" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="B24" s="12" t="s">
         <v>70</v>
@@ -3040,25 +2992,25 @@
         <v>20</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="G24" s="12" t="s">
         <v>17</v>
       </c>
       <c r="H24" s="12" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="I24" s="12"/>
       <c r="J24" s="12"/>
       <c r="K24" s="12" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="L24" s="12"/>
       <c r="M24" s="8" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
     </row>
     <row r="25" spans="1:13">
@@ -4379,11 +4331,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L124"/>
+  <dimension ref="A1:L115"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C101" activeCellId="5" sqref="C15:C16 C35 C39 C61 C87 C101"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4435,7 +4387,7 @@
         <v>15</v>
       </c>
       <c r="L1" s="9" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -4467,7 +4419,7 @@
         <v>16</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -4499,7 +4451,7 @@
         <v>24</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -4531,7 +4483,7 @@
         <v>26</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>326</v>
+        <v>310</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -4563,7 +4515,7 @@
         <v>27</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -4595,7 +4547,7 @@
         <v>28</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -4627,7 +4579,7 @@
         <v>29</v>
       </c>
       <c r="L7" s="8" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -4659,10 +4611,10 @@
         <v>31</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="7" customFormat="1">
       <c r="A9" s="12" t="s">
         <v>21</v>
       </c>
@@ -4691,7 +4643,7 @@
         <v>32</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -4723,7 +4675,7 @@
         <v>33</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -4755,7 +4707,7 @@
         <v>34</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -4787,7 +4739,7 @@
         <v>35</v>
       </c>
       <c r="L12" s="8" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -4819,7 +4771,7 @@
         <v>38</v>
       </c>
       <c r="L13" s="8" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -4851,7 +4803,7 @@
         <v>38</v>
       </c>
       <c r="L14" s="8" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -4883,7 +4835,7 @@
         <v>41</v>
       </c>
       <c r="L15" s="8" t="s">
-        <v>325</v>
+        <v>309</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -4915,7 +4867,7 @@
         <v>42</v>
       </c>
       <c r="L16" s="8" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -4947,10 +4899,10 @@
         <v>43</v>
       </c>
       <c r="L17" s="8" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" s="7" customFormat="1">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
       <c r="A18" s="12" t="s">
         <v>40</v>
       </c>
@@ -4979,7 +4931,7 @@
         <v>44</v>
       </c>
       <c r="L18" s="8" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -5011,7 +4963,7 @@
         <v>46</v>
       </c>
       <c r="L19" s="8" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -5043,7 +4995,7 @@
         <v>47</v>
       </c>
       <c r="L20" s="8" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -5075,7 +5027,7 @@
         <v>48</v>
       </c>
       <c r="L21" s="8" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
     </row>
     <row r="22" spans="1:12">
@@ -5107,7 +5059,7 @@
         <v>49</v>
       </c>
       <c r="L22" s="8" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
     </row>
     <row r="23" spans="1:12">
@@ -5139,7 +5091,7 @@
         <v>50</v>
       </c>
       <c r="L23" s="8" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -5171,7 +5123,7 @@
         <v>51</v>
       </c>
       <c r="L24" s="8" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
     </row>
     <row r="25" spans="1:12">
@@ -5203,7 +5155,7 @@
         <v>52</v>
       </c>
       <c r="L25" s="8" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
     </row>
     <row r="26" spans="1:12">
@@ -5235,7 +5187,7 @@
         <v>53</v>
       </c>
       <c r="L26" s="8" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -5267,7 +5219,7 @@
         <v>53</v>
       </c>
       <c r="L27" s="8" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
     </row>
     <row r="28" spans="1:12">
@@ -5282,7 +5234,7 @@
       </c>
       <c r="D28" s="12"/>
       <c r="E28" s="12"/>
-      <c r="F28" s="12" t="s">
+      <c r="F28" s="15" t="s">
         <v>53</v>
       </c>
       <c r="G28" s="12"/>
@@ -5295,11 +5247,11 @@
       <c r="J28" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="K28" s="12" t="s">
+      <c r="K28" s="15" t="s">
         <v>53</v>
       </c>
       <c r="L28" s="8" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
     </row>
     <row r="29" spans="1:12">
@@ -5314,7 +5266,7 @@
       </c>
       <c r="D29" s="12"/>
       <c r="E29" s="12"/>
-      <c r="F29" s="12" t="s">
+      <c r="F29" s="15" t="s">
         <v>54</v>
       </c>
       <c r="G29" s="12"/>
@@ -5327,11 +5279,11 @@
       <c r="J29" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="K29" s="12" t="s">
+      <c r="K29" s="15" t="s">
         <v>54</v>
       </c>
       <c r="L29" s="8" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
     </row>
     <row r="30" spans="1:12">
@@ -5346,7 +5298,7 @@
       </c>
       <c r="D30" s="12"/>
       <c r="E30" s="12"/>
-      <c r="F30" s="12" t="s">
+      <c r="F30" s="15" t="s">
         <v>55</v>
       </c>
       <c r="G30" s="12"/>
@@ -5359,11 +5311,11 @@
       <c r="J30" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="K30" s="12" t="s">
+      <c r="K30" s="15" t="s">
         <v>55</v>
       </c>
       <c r="L30" s="8" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
     </row>
     <row r="31" spans="1:12">
@@ -5378,7 +5330,7 @@
       </c>
       <c r="D31" s="12"/>
       <c r="E31" s="12"/>
-      <c r="F31" s="12" t="s">
+      <c r="F31" s="15" t="s">
         <v>57</v>
       </c>
       <c r="G31" s="12"/>
@@ -5395,7 +5347,7 @@
         <v>57</v>
       </c>
       <c r="L31" s="8" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
     </row>
     <row r="32" spans="1:12">
@@ -5410,7 +5362,7 @@
       </c>
       <c r="D32" s="12"/>
       <c r="E32" s="12"/>
-      <c r="F32" s="12" t="s">
+      <c r="F32" s="15" t="s">
         <v>60</v>
       </c>
       <c r="G32" s="12"/>
@@ -5427,7 +5379,7 @@
         <v>60</v>
       </c>
       <c r="L32" s="8" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
     </row>
     <row r="33" spans="1:12">
@@ -5442,7 +5394,7 @@
       </c>
       <c r="D33" s="18"/>
       <c r="E33" s="12"/>
-      <c r="F33" s="18" t="s">
+      <c r="F33" s="15" t="s">
         <v>58</v>
       </c>
       <c r="G33" s="12"/>
@@ -5459,7 +5411,7 @@
         <v>58</v>
       </c>
       <c r="L33" s="8" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
     </row>
     <row r="34" spans="1:12">
@@ -5474,7 +5426,7 @@
       </c>
       <c r="D34" s="12"/>
       <c r="E34" s="12"/>
-      <c r="F34" s="18" t="s">
+      <c r="F34" s="15" t="s">
         <v>62</v>
       </c>
       <c r="G34" s="12"/>
@@ -5491,7 +5443,7 @@
         <v>62</v>
       </c>
       <c r="L34" s="8" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
     </row>
     <row r="35" spans="1:12">
@@ -5506,7 +5458,7 @@
       </c>
       <c r="D35" s="12"/>
       <c r="E35" s="12"/>
-      <c r="F35" s="18" t="s">
+      <c r="F35" s="15" t="s">
         <v>66</v>
       </c>
       <c r="G35" s="12"/>
@@ -5523,7 +5475,7 @@
         <v>66</v>
       </c>
       <c r="L35" s="8" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
     </row>
     <row r="36" spans="1:12">
@@ -5555,7 +5507,7 @@
         <v>67</v>
       </c>
       <c r="L36" s="8" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
     </row>
     <row r="37" spans="1:12">
@@ -5570,7 +5522,7 @@
       </c>
       <c r="D37" s="12"/>
       <c r="E37" s="12"/>
-      <c r="F37" s="15" t="s">
+      <c r="F37" s="18" t="s">
         <v>71</v>
       </c>
       <c r="G37" s="12"/>
@@ -5581,11 +5533,11 @@
       <c r="J37" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="K37" s="15" t="s">
+      <c r="K37" s="18" t="s">
         <v>71</v>
       </c>
       <c r="L37" s="8" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
     </row>
     <row r="38" spans="1:12">
@@ -5600,7 +5552,7 @@
       </c>
       <c r="D38" s="12"/>
       <c r="E38" s="12"/>
-      <c r="F38" s="15" t="s">
+      <c r="F38" s="18" t="s">
         <v>74</v>
       </c>
       <c r="G38" s="12"/>
@@ -5611,11 +5563,11 @@
       <c r="J38" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="K38" s="15" t="s">
+      <c r="K38" s="18" t="s">
         <v>74</v>
       </c>
       <c r="L38" s="8" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
     </row>
     <row r="39" spans="1:12">
@@ -5630,7 +5582,7 @@
       </c>
       <c r="D39" s="12"/>
       <c r="E39" s="12"/>
-      <c r="F39" s="15" t="s">
+      <c r="F39" s="18" t="s">
         <v>75</v>
       </c>
       <c r="G39" s="14"/>
@@ -5643,11 +5595,11 @@
       <c r="J39" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="K39" s="15" t="s">
+      <c r="K39" s="18" t="s">
         <v>75</v>
       </c>
       <c r="L39" s="8" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
     </row>
     <row r="40" spans="1:12">
@@ -5661,10 +5613,10 @@
         <v>59</v>
       </c>
       <c r="D40" s="12" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E40" s="12"/>
-      <c r="F40" s="15"/>
+      <c r="F40" s="18"/>
       <c r="G40" s="14"/>
       <c r="H40" s="12"/>
       <c r="I40" s="13" t="s">
@@ -5674,10 +5626,10 @@
         <v>73</v>
       </c>
       <c r="K40" s="12" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="L40" s="8" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
     </row>
     <row r="41" spans="1:12">
@@ -5691,10 +5643,10 @@
         <v>59</v>
       </c>
       <c r="D41" s="12" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E41" s="12"/>
-      <c r="F41" s="15"/>
+      <c r="F41" s="18"/>
       <c r="G41" s="14"/>
       <c r="H41" s="12"/>
       <c r="I41" s="13" t="s">
@@ -5704,10 +5656,10 @@
         <v>73</v>
       </c>
       <c r="K41" s="12" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="L41" s="8" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
     </row>
     <row r="42" spans="1:12">
@@ -5721,10 +5673,10 @@
         <v>59</v>
       </c>
       <c r="D42" s="12" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E42" s="12"/>
-      <c r="F42" s="15"/>
+      <c r="F42" s="18"/>
       <c r="G42" s="14"/>
       <c r="H42" s="12"/>
       <c r="I42" s="12" t="s">
@@ -5734,10 +5686,10 @@
         <v>73</v>
       </c>
       <c r="K42" s="12" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="L42" s="8" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
     </row>
     <row r="43" spans="1:12">
@@ -5751,10 +5703,10 @@
         <v>59</v>
       </c>
       <c r="D43" s="12" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E43" s="12"/>
-      <c r="F43" s="15"/>
+      <c r="F43" s="18"/>
       <c r="G43" s="14"/>
       <c r="H43" s="12"/>
       <c r="I43" s="12" t="s">
@@ -5764,10 +5716,10 @@
         <v>73</v>
       </c>
       <c r="K43" s="12" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="L43" s="8" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
     </row>
     <row r="44" spans="1:12">
@@ -5781,10 +5733,10 @@
         <v>23</v>
       </c>
       <c r="D44" s="12" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E44" s="12"/>
-      <c r="F44" s="15"/>
+      <c r="F44" s="18"/>
       <c r="G44" s="14"/>
       <c r="H44" s="12"/>
       <c r="I44" s="12" t="s">
@@ -5794,10 +5746,10 @@
         <v>73</v>
       </c>
       <c r="K44" s="12" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="L44" s="8" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
     </row>
     <row r="45" spans="1:12">
@@ -5811,7 +5763,7 @@
         <v>70</v>
       </c>
       <c r="D45" s="12" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E45" s="12"/>
       <c r="F45" s="12"/>
@@ -5824,10 +5776,10 @@
         <v>73</v>
       </c>
       <c r="K45" s="12" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="L45" s="8" t="s">
-        <v>255</v>
+        <v>244</v>
       </c>
     </row>
     <row r="46" spans="1:12">
@@ -5841,7 +5793,7 @@
         <v>59</v>
       </c>
       <c r="D46" s="12" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E46" s="12"/>
       <c r="F46" s="12"/>
@@ -5854,10 +5806,10 @@
         <v>73</v>
       </c>
       <c r="K46" s="12" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="L46" s="8" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
     </row>
     <row r="47" spans="1:12">
@@ -5887,7 +5839,7 @@
         <v>18</v>
       </c>
       <c r="L47" s="8" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
     </row>
     <row r="48" spans="1:12">
@@ -5901,7 +5853,7 @@
         <v>70</v>
       </c>
       <c r="D48" s="12" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E48" s="12"/>
       <c r="F48" s="12"/>
@@ -5914,10 +5866,10 @@
         <v>73</v>
       </c>
       <c r="K48" s="12" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="L48" s="8" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="49" spans="1:12">
@@ -5931,7 +5883,7 @@
         <v>70</v>
       </c>
       <c r="D49" s="12" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E49" s="12"/>
       <c r="F49" s="12"/>
@@ -5944,10 +5896,10 @@
         <v>73</v>
       </c>
       <c r="K49" s="12" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="L49" s="8" t="s">
-        <v>257</v>
+        <v>246</v>
       </c>
     </row>
     <row r="50" spans="1:12">
@@ -5961,7 +5913,7 @@
         <v>37</v>
       </c>
       <c r="D50" s="18" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E50" s="12"/>
       <c r="F50" s="12"/>
@@ -5974,10 +5926,10 @@
         <v>73</v>
       </c>
       <c r="K50" s="18" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="L50" s="8" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
     </row>
     <row r="51" spans="1:12">
@@ -5992,7 +5944,7 @@
       </c>
       <c r="D51" s="12"/>
       <c r="E51" s="12" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F51" s="18"/>
       <c r="G51" s="12"/>
@@ -6004,10 +5956,10 @@
         <v>73</v>
       </c>
       <c r="K51" s="12" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="L51" s="8" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
     </row>
     <row r="52" spans="1:12">
@@ -6021,13 +5973,13 @@
         <v>70</v>
       </c>
       <c r="D52" s="18" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E52" s="12"/>
       <c r="F52" s="18"/>
       <c r="G52" s="12"/>
       <c r="H52" s="12" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="I52" s="12" t="s">
         <v>72</v>
@@ -6036,10 +5988,10 @@
         <v>73</v>
       </c>
       <c r="K52" s="18" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="L52" s="8" t="s">
-        <v>258</v>
+        <v>247</v>
       </c>
     </row>
     <row r="53" spans="1:12">
@@ -6069,7 +6021,7 @@
         <v>58</v>
       </c>
       <c r="L53" s="8" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
     </row>
     <row r="54" spans="1:12">
@@ -6083,7 +6035,7 @@
         <v>63</v>
       </c>
       <c r="D54" s="12" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="E54" s="12"/>
       <c r="F54" s="18"/>
@@ -6096,10 +6048,10 @@
         <v>73</v>
       </c>
       <c r="K54" s="18" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="L54" s="8" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
     </row>
     <row r="55" spans="1:12">
@@ -6112,8 +6064,8 @@
       <c r="C55" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="D55" s="12" t="s">
-        <v>205</v>
+      <c r="D55" s="16" t="s">
+        <v>198</v>
       </c>
       <c r="E55" s="12"/>
       <c r="F55" s="12"/>
@@ -6125,11 +6077,11 @@
       <c r="J55" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="K55" s="12" t="s">
-        <v>205</v>
+      <c r="K55" s="16" t="s">
+        <v>198</v>
       </c>
       <c r="L55" s="8" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
     </row>
     <row r="56" spans="1:12">
@@ -6143,7 +6095,7 @@
         <v>59</v>
       </c>
       <c r="D56" s="12" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E56" s="12"/>
       <c r="F56" s="12"/>
@@ -6156,10 +6108,10 @@
         <v>73</v>
       </c>
       <c r="K56" s="12" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="L56" s="8" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
     </row>
     <row r="57" spans="1:12">
@@ -6173,7 +6125,7 @@
         <v>65</v>
       </c>
       <c r="D57" s="12" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E57" s="12"/>
       <c r="F57" s="18"/>
@@ -6186,10 +6138,10 @@
         <v>73</v>
       </c>
       <c r="K57" s="12" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="L57" s="8" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
     </row>
     <row r="58" spans="1:12">
@@ -6203,7 +6155,7 @@
         <v>59</v>
       </c>
       <c r="D58" s="12" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E58" s="12"/>
       <c r="F58" s="12"/>
@@ -6216,10 +6168,10 @@
         <v>73</v>
       </c>
       <c r="K58" s="12" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="L58" s="8" t="s">
-        <v>273</v>
+        <v>262</v>
       </c>
     </row>
     <row r="59" spans="1:12">
@@ -6233,7 +6185,7 @@
         <v>63</v>
       </c>
       <c r="D59" s="12" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="E59" s="12"/>
       <c r="F59" s="18"/>
@@ -6246,10 +6198,10 @@
         <v>73</v>
       </c>
       <c r="K59" s="12" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="L59" s="8" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
     </row>
     <row r="60" spans="1:12">
@@ -6263,7 +6215,7 @@
         <v>59</v>
       </c>
       <c r="D60" s="12" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E60" s="12"/>
       <c r="F60" s="12"/>
@@ -6276,10 +6228,10 @@
         <v>73</v>
       </c>
       <c r="K60" s="12" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="L60" s="8" t="s">
-        <v>274</v>
+        <v>263</v>
       </c>
     </row>
     <row r="61" spans="1:12">
@@ -6293,7 +6245,7 @@
         <v>59</v>
       </c>
       <c r="D61" s="18" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E61" s="12"/>
       <c r="F61" s="12"/>
@@ -6306,10 +6258,10 @@
         <v>73</v>
       </c>
       <c r="K61" s="18" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="L61" s="8" t="s">
-        <v>275</v>
+        <v>264</v>
       </c>
     </row>
     <row r="62" spans="1:12">
@@ -6323,7 +6275,7 @@
         <v>63</v>
       </c>
       <c r="D62" s="12" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E62" s="12"/>
       <c r="F62" s="18"/>
@@ -6336,10 +6288,10 @@
         <v>73</v>
       </c>
       <c r="K62" s="12" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="L62" s="8" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
     </row>
     <row r="63" spans="1:12">
@@ -6353,7 +6305,7 @@
         <v>59</v>
       </c>
       <c r="D63" s="12" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="E63" s="12"/>
       <c r="F63" s="12"/>
@@ -6366,10 +6318,10 @@
         <v>73</v>
       </c>
       <c r="K63" s="12" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="L63" s="8" t="s">
-        <v>276</v>
+        <v>265</v>
       </c>
     </row>
     <row r="64" spans="1:12">
@@ -6382,7 +6334,7 @@
       <c r="C64" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="D64" s="16" t="s">
+      <c r="D64" s="18" t="s">
         <v>70</v>
       </c>
       <c r="E64" s="12"/>
@@ -6395,11 +6347,11 @@
       <c r="J64" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="K64" s="16" t="s">
+      <c r="K64" s="18" t="s">
         <v>70</v>
       </c>
       <c r="L64" s="8" t="s">
-        <v>260</v>
+        <v>249</v>
       </c>
     </row>
     <row r="65" spans="1:12">
@@ -6413,7 +6365,7 @@
         <v>59</v>
       </c>
       <c r="D65" s="12" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E65" s="12"/>
       <c r="F65" s="12"/>
@@ -6426,10 +6378,10 @@
         <v>73</v>
       </c>
       <c r="K65" s="12" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="L65" s="8" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
     </row>
     <row r="66" spans="1:12">
@@ -6443,7 +6395,7 @@
         <v>59</v>
       </c>
       <c r="D66" s="12" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E66" s="12"/>
       <c r="F66" s="12"/>
@@ -6456,10 +6408,10 @@
         <v>73</v>
       </c>
       <c r="K66" s="12" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="L66" s="8" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
     </row>
     <row r="67" spans="1:12">
@@ -6473,13 +6425,13 @@
         <v>70</v>
       </c>
       <c r="D67" s="12" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E67" s="12"/>
       <c r="F67" s="12"/>
       <c r="G67" s="12"/>
       <c r="H67" s="12" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="I67" s="12" t="s">
         <v>72</v>
@@ -6488,10 +6440,10 @@
         <v>73</v>
       </c>
       <c r="K67" s="12" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="L67" s="8" t="s">
-        <v>261</v>
+        <v>250</v>
       </c>
     </row>
     <row r="68" spans="1:12">
@@ -6505,13 +6457,13 @@
         <v>70</v>
       </c>
       <c r="D68" s="12" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E68" s="12"/>
       <c r="F68" s="12"/>
       <c r="G68" s="12"/>
       <c r="H68" s="12" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="I68" s="12" t="s">
         <v>72</v>
@@ -6520,10 +6472,10 @@
         <v>73</v>
       </c>
       <c r="K68" s="12" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="L68" s="8" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
     </row>
     <row r="69" spans="1:12">
@@ -6537,7 +6489,7 @@
         <v>37</v>
       </c>
       <c r="D69" s="12" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E69" s="12"/>
       <c r="F69" s="12"/>
@@ -6550,10 +6502,10 @@
         <v>73</v>
       </c>
       <c r="K69" s="12" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="L69" s="8" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
     </row>
     <row r="70" spans="1:12">
@@ -6567,7 +6519,7 @@
         <v>70</v>
       </c>
       <c r="D70" s="12" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E70" s="12"/>
       <c r="F70" s="12"/>
@@ -6580,10 +6532,10 @@
         <v>73</v>
       </c>
       <c r="K70" s="12" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="L70" s="8" t="s">
-        <v>263</v>
+        <v>252</v>
       </c>
     </row>
     <row r="71" spans="1:12">
@@ -6597,7 +6549,7 @@
         <v>63</v>
       </c>
       <c r="D71" s="12" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E71" s="12"/>
       <c r="F71" s="18"/>
@@ -6610,10 +6562,10 @@
         <v>73</v>
       </c>
       <c r="K71" s="12" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="L71" s="8" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
     </row>
     <row r="72" spans="1:12">
@@ -6624,26 +6576,26 @@
         <v>77</v>
       </c>
       <c r="C72" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="D72" s="12"/>
+        <v>59</v>
+      </c>
+      <c r="D72" s="12" t="s">
+        <v>105</v>
+      </c>
       <c r="E72" s="12"/>
-      <c r="F72" s="18"/>
-      <c r="G72" s="12" t="s">
-        <v>78</v>
-      </c>
+      <c r="F72" s="12"/>
+      <c r="G72" s="12"/>
       <c r="H72" s="12"/>
       <c r="I72" s="12" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="J72" s="12" t="s">
         <v>73</v>
       </c>
       <c r="K72" s="12" t="s">
-        <v>78</v>
+        <v>105</v>
       </c>
       <c r="L72" s="8" t="s">
-        <v>249</v>
+        <v>268</v>
       </c>
     </row>
     <row r="73" spans="1:12">
@@ -6657,10 +6609,10 @@
         <v>59</v>
       </c>
       <c r="D73" s="12" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E73" s="12"/>
-      <c r="F73" s="12"/>
+      <c r="F73" s="18"/>
       <c r="G73" s="12"/>
       <c r="H73" s="12"/>
       <c r="I73" s="12" t="s">
@@ -6669,11 +6621,11 @@
       <c r="J73" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="K73" s="12" t="s">
-        <v>109</v>
+      <c r="K73" s="18" t="s">
+        <v>106</v>
       </c>
       <c r="L73" s="8" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
     </row>
     <row r="74" spans="1:12">
@@ -6687,11 +6639,11 @@
         <v>63</v>
       </c>
       <c r="D74" s="12"/>
-      <c r="E74" s="12"/>
+      <c r="E74" s="12" t="s">
+        <v>114</v>
+      </c>
       <c r="F74" s="18"/>
-      <c r="G74" s="12" t="s">
-        <v>79</v>
-      </c>
+      <c r="G74" s="12"/>
       <c r="H74" s="12"/>
       <c r="I74" s="12" t="s">
         <v>39</v>
@@ -6700,10 +6652,10 @@
         <v>73</v>
       </c>
       <c r="K74" s="12" t="s">
-        <v>79</v>
+        <v>114</v>
       </c>
       <c r="L74" s="8" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
     </row>
     <row r="75" spans="1:12">
@@ -6714,26 +6666,26 @@
         <v>77</v>
       </c>
       <c r="C75" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="D75" s="12"/>
+        <v>59</v>
+      </c>
+      <c r="D75" s="12" t="s">
+        <v>107</v>
+      </c>
       <c r="E75" s="12"/>
       <c r="F75" s="18"/>
-      <c r="G75" s="12" t="s">
-        <v>80</v>
-      </c>
+      <c r="G75" s="12"/>
       <c r="H75" s="12"/>
       <c r="I75" s="12" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="J75" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="K75" s="18" t="s">
-        <v>80</v>
+      <c r="K75" s="12" t="s">
+        <v>107</v>
       </c>
       <c r="L75" s="8" t="s">
-        <v>251</v>
+        <v>270</v>
       </c>
     </row>
     <row r="76" spans="1:12">
@@ -6744,26 +6696,26 @@
         <v>77</v>
       </c>
       <c r="C76" s="12" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D76" s="12" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E76" s="12"/>
       <c r="F76" s="18"/>
       <c r="G76" s="12"/>
       <c r="H76" s="12"/>
       <c r="I76" s="12" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="J76" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="K76" s="18" t="s">
-        <v>110</v>
+      <c r="K76" s="12" t="s">
+        <v>108</v>
       </c>
       <c r="L76" s="8" t="s">
-        <v>280</v>
+        <v>243</v>
       </c>
     </row>
     <row r="77" spans="1:12">
@@ -6774,26 +6726,26 @@
         <v>77</v>
       </c>
       <c r="C77" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="D77" s="12"/>
+        <v>65</v>
+      </c>
+      <c r="D77" s="12" t="s">
+        <v>109</v>
+      </c>
       <c r="E77" s="12"/>
       <c r="F77" s="18"/>
-      <c r="G77" s="12" t="s">
-        <v>81</v>
-      </c>
+      <c r="G77" s="12"/>
       <c r="H77" s="12"/>
       <c r="I77" s="12" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="J77" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="K77" s="18" t="s">
-        <v>81</v>
+      <c r="K77" s="12" t="s">
+        <v>109</v>
       </c>
       <c r="L77" s="8" t="s">
-        <v>281</v>
+        <v>238</v>
       </c>
     </row>
     <row r="78" spans="1:12">
@@ -6804,26 +6756,26 @@
         <v>77</v>
       </c>
       <c r="C78" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="D78" s="12"/>
-      <c r="E78" s="12" t="s">
-        <v>118</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="D78" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="E78" s="12"/>
       <c r="F78" s="18"/>
       <c r="G78" s="12"/>
       <c r="H78" s="12"/>
       <c r="I78" s="12" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="J78" s="12" t="s">
         <v>73</v>
       </c>
       <c r="K78" s="12" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="L78" s="8" t="s">
-        <v>252</v>
+        <v>271</v>
       </c>
     </row>
     <row r="79" spans="1:12">
@@ -6840,7 +6792,7 @@
         <v>111</v>
       </c>
       <c r="E79" s="12"/>
-      <c r="F79" s="18"/>
+      <c r="F79" s="12"/>
       <c r="G79" s="12"/>
       <c r="H79" s="12"/>
       <c r="I79" s="12" t="s">
@@ -6853,7 +6805,7 @@
         <v>111</v>
       </c>
       <c r="L79" s="8" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
     </row>
     <row r="80" spans="1:12">
@@ -6864,17 +6816,17 @@
         <v>77</v>
       </c>
       <c r="C80" s="12" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D80" s="12" t="s">
         <v>112</v>
       </c>
       <c r="E80" s="12"/>
-      <c r="F80" s="18"/>
+      <c r="F80" s="12"/>
       <c r="G80" s="12"/>
       <c r="H80" s="12"/>
       <c r="I80" s="12" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="J80" s="12" t="s">
         <v>73</v>
@@ -6883,293 +6835,297 @@
         <v>112</v>
       </c>
       <c r="L80" s="8" t="s">
-        <v>253</v>
+        <v>273</v>
       </c>
     </row>
     <row r="81" spans="1:12">
       <c r="A81" s="12" t="s">
-        <v>76</v>
+        <v>115</v>
       </c>
       <c r="B81" s="12" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="C81" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="D81" s="12" t="s">
-        <v>113</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="D81" s="12"/>
       <c r="E81" s="12"/>
-      <c r="F81" s="18"/>
+      <c r="F81" s="12" t="s">
+        <v>116</v>
+      </c>
       <c r="G81" s="12"/>
-      <c r="H81" s="12"/>
+      <c r="H81" s="12" t="s">
+        <v>115</v>
+      </c>
       <c r="I81" s="12" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="J81" s="12" t="s">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="K81" s="12" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="L81" s="8" t="s">
-        <v>245</v>
+        <v>274</v>
       </c>
     </row>
     <row r="82" spans="1:12">
       <c r="A82" s="12" t="s">
-        <v>76</v>
+        <v>117</v>
       </c>
       <c r="B82" s="12" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="C82" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="D82" s="12" t="s">
-        <v>114</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="D82" s="12"/>
       <c r="E82" s="12"/>
-      <c r="F82" s="18"/>
+      <c r="F82" s="12" t="s">
+        <v>117</v>
+      </c>
       <c r="G82" s="12"/>
-      <c r="H82" s="12"/>
+      <c r="H82" s="12" t="s">
+        <v>117</v>
+      </c>
       <c r="I82" s="12" t="s">
-        <v>61</v>
+        <v>19</v>
       </c>
       <c r="J82" s="12" t="s">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="K82" s="12" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="L82" s="8" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
     </row>
     <row r="83" spans="1:12">
       <c r="A83" s="12" t="s">
-        <v>76</v>
+        <v>117</v>
       </c>
       <c r="B83" s="12" t="s">
-        <v>77</v>
+        <v>30</v>
       </c>
       <c r="C83" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="D83" s="12" t="s">
-        <v>115</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="D83" s="12"/>
       <c r="E83" s="12"/>
-      <c r="F83" s="12"/>
+      <c r="F83" s="12" t="s">
+        <v>117</v>
+      </c>
       <c r="G83" s="12"/>
-      <c r="H83" s="12"/>
+      <c r="H83" s="12" t="s">
+        <v>117</v>
+      </c>
       <c r="I83" s="12" t="s">
-        <v>61</v>
+        <v>19</v>
       </c>
       <c r="J83" s="12" t="s">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="K83" s="12" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="L83" s="8" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
     </row>
     <row r="84" spans="1:12">
       <c r="A84" s="12" t="s">
-        <v>76</v>
+        <v>117</v>
       </c>
       <c r="B84" s="12" t="s">
-        <v>77</v>
+        <v>45</v>
       </c>
       <c r="C84" s="12" t="s">
         <v>63</v>
       </c>
       <c r="D84" s="12"/>
       <c r="E84" s="12"/>
-      <c r="F84" s="18"/>
-      <c r="G84" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="H84" s="12"/>
+      <c r="F84" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="G84" s="12"/>
+      <c r="H84" s="12" t="s">
+        <v>117</v>
+      </c>
       <c r="I84" s="12" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="J84" s="12" t="s">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="K84" s="12" t="s">
-        <v>82</v>
+        <v>277</v>
       </c>
       <c r="L84" s="8" t="s">
-        <v>254</v>
+        <v>276</v>
       </c>
     </row>
     <row r="85" spans="1:12">
       <c r="A85" s="12" t="s">
-        <v>76</v>
+        <v>103</v>
       </c>
       <c r="B85" s="12" t="s">
-        <v>77</v>
+        <v>119</v>
       </c>
       <c r="C85" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="D85" s="12" t="s">
-        <v>116</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="D85" s="12"/>
       <c r="E85" s="12"/>
-      <c r="F85" s="12"/>
+      <c r="F85" s="12" t="s">
+        <v>120</v>
+      </c>
       <c r="G85" s="12"/>
       <c r="H85" s="12"/>
       <c r="I85" s="12" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="J85" s="12" t="s">
         <v>73</v>
       </c>
       <c r="K85" s="12" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="L85" s="8" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
     </row>
     <row r="86" spans="1:12">
       <c r="A86" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="B86" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="B86" s="12" t="s">
-        <v>17</v>
-      </c>
       <c r="C86" s="12" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
       <c r="D86" s="12"/>
       <c r="E86" s="12"/>
       <c r="F86" s="12" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G86" s="12"/>
-      <c r="H86" s="12" t="s">
-        <v>119</v>
-      </c>
+      <c r="H86" s="12"/>
       <c r="I86" s="12" t="s">
-        <v>39</v>
+        <v>72</v>
       </c>
       <c r="J86" s="12" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="K86" s="12" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="L86" s="8" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
     </row>
     <row r="87" spans="1:12">
       <c r="A87" s="12" t="s">
-        <v>121</v>
+        <v>103</v>
       </c>
       <c r="B87" s="12" t="s">
-        <v>17</v>
+        <v>119</v>
       </c>
       <c r="C87" s="12" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="D87" s="12"/>
       <c r="E87" s="12"/>
       <c r="F87" s="12" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="G87" s="12"/>
-      <c r="H87" s="12" t="s">
-        <v>121</v>
-      </c>
+      <c r="H87" s="12"/>
       <c r="I87" s="12" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
       <c r="J87" s="12" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="K87" s="12" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="L87" s="8" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
     </row>
     <row r="88" spans="1:12">
       <c r="A88" s="12" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B88" s="12" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="C88" s="12" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="D88" s="12"/>
       <c r="E88" s="12"/>
-      <c r="F88" s="12" t="s">
-        <v>121</v>
+      <c r="F88" s="18" t="s">
+        <v>124</v>
       </c>
       <c r="G88" s="12"/>
       <c r="H88" s="12" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="I88" s="12" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
       <c r="J88" s="12" t="s">
         <v>20</v>
       </c>
       <c r="K88" s="12" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="L88" s="8" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
     </row>
     <row r="89" spans="1:12">
       <c r="A89" s="12" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B89" s="12" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="C89" s="12" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="D89" s="12"/>
       <c r="E89" s="12"/>
       <c r="F89" s="12" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="G89" s="12"/>
       <c r="H89" s="12" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="I89" s="12" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
       <c r="J89" s="12" t="s">
         <v>20</v>
       </c>
       <c r="K89" s="12" t="s">
-        <v>289</v>
+        <v>125</v>
       </c>
       <c r="L89" s="8" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
     </row>
     <row r="90" spans="1:12">
       <c r="A90" s="12" t="s">
-        <v>107</v>
+        <v>123</v>
       </c>
       <c r="B90" s="12" t="s">
-        <v>123</v>
+        <v>45</v>
       </c>
       <c r="C90" s="12" t="s">
         <v>70</v>
@@ -7177,29 +7133,31 @@
       <c r="D90" s="12"/>
       <c r="E90" s="12"/>
       <c r="F90" s="12" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="G90" s="12"/>
-      <c r="H90" s="12"/>
+      <c r="H90" s="12" t="s">
+        <v>123</v>
+      </c>
       <c r="I90" s="12" t="s">
         <v>72</v>
       </c>
       <c r="J90" s="12" t="s">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="K90" s="12" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="L90" s="8" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
     </row>
     <row r="91" spans="1:12">
       <c r="A91" s="12" t="s">
-        <v>107</v>
+        <v>123</v>
       </c>
       <c r="B91" s="12" t="s">
-        <v>123</v>
+        <v>17</v>
       </c>
       <c r="C91" s="12" t="s">
         <v>70</v>
@@ -7207,29 +7165,31 @@
       <c r="D91" s="12"/>
       <c r="E91" s="12"/>
       <c r="F91" s="12" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="G91" s="12"/>
-      <c r="H91" s="12"/>
+      <c r="H91" s="12" t="s">
+        <v>123</v>
+      </c>
       <c r="I91" s="12" t="s">
         <v>72</v>
       </c>
       <c r="J91" s="12" t="s">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="K91" s="12" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="L91" s="8" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
     </row>
     <row r="92" spans="1:12">
       <c r="A92" s="12" t="s">
-        <v>107</v>
+        <v>123</v>
       </c>
       <c r="B92" s="12" t="s">
-        <v>123</v>
+        <v>17</v>
       </c>
       <c r="C92" s="12" t="s">
         <v>70</v>
@@ -7237,157 +7197,159 @@
       <c r="D92" s="12"/>
       <c r="E92" s="12"/>
       <c r="F92" s="12" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="G92" s="12"/>
-      <c r="H92" s="12"/>
+      <c r="H92" s="12" t="s">
+        <v>123</v>
+      </c>
       <c r="I92" s="12" t="s">
         <v>72</v>
       </c>
       <c r="J92" s="12" t="s">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="K92" s="12" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="L92" s="8" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
     </row>
     <row r="93" spans="1:12">
       <c r="A93" s="12" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B93" s="12" t="s">
         <v>17</v>
       </c>
       <c r="C93" s="12" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="D93" s="12"/>
       <c r="E93" s="12"/>
-      <c r="F93" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="G93" s="12"/>
+      <c r="F93" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="G93" s="14"/>
       <c r="H93" s="12" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="I93" s="12" t="s">
-        <v>72</v>
+        <v>19</v>
       </c>
       <c r="J93" s="12" t="s">
         <v>20</v>
       </c>
       <c r="K93" s="12" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="L93" s="8" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
     </row>
     <row r="94" spans="1:12">
       <c r="A94" s="12" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B94" s="12" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="C94" s="12" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="D94" s="12"/>
       <c r="E94" s="12"/>
       <c r="F94" s="12" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="G94" s="12"/>
       <c r="H94" s="12" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="I94" s="12" t="s">
-        <v>72</v>
+        <v>19</v>
       </c>
       <c r="J94" s="12" t="s">
         <v>20</v>
       </c>
       <c r="K94" s="12" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="L94" s="8" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
     </row>
     <row r="95" spans="1:12">
       <c r="A95" s="12" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B95" s="12" t="s">
         <v>45</v>
       </c>
       <c r="C95" s="12" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="D95" s="12"/>
       <c r="E95" s="12"/>
       <c r="F95" s="12" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="G95" s="12"/>
       <c r="H95" s="12" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="I95" s="12" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="J95" s="12" t="s">
         <v>20</v>
       </c>
       <c r="K95" s="12" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="L95" s="8" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
     </row>
     <row r="96" spans="1:12">
       <c r="A96" s="12" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B96" s="12" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="C96" s="12" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="D96" s="12"/>
       <c r="E96" s="12"/>
       <c r="F96" s="12" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="G96" s="12"/>
       <c r="H96" s="12" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="I96" s="12" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="J96" s="12" t="s">
         <v>20</v>
       </c>
       <c r="K96" s="12" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="L96" s="8" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
     </row>
     <row r="97" spans="1:12">
       <c r="A97" s="12" t="s">
-        <v>127</v>
+        <v>196</v>
       </c>
       <c r="B97" s="12" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="C97" s="12" t="s">
         <v>70</v>
@@ -7395,11 +7357,11 @@
       <c r="D97" s="12"/>
       <c r="E97" s="12"/>
       <c r="F97" s="12" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="G97" s="12"/>
       <c r="H97" s="12" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="I97" s="12" t="s">
         <v>72</v>
@@ -7408,282 +7370,272 @@
         <v>20</v>
       </c>
       <c r="K97" s="12" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="L97" s="8" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
     </row>
     <row r="98" spans="1:12">
       <c r="A98" s="12" t="s">
-        <v>133</v>
+        <v>196</v>
       </c>
       <c r="B98" s="12" t="s">
         <v>17</v>
       </c>
       <c r="C98" s="12" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="D98" s="12"/>
       <c r="E98" s="12"/>
-      <c r="F98" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="G98" s="14"/>
+      <c r="F98" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="G98" s="12"/>
       <c r="H98" s="12" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="I98" s="12" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
       <c r="J98" s="12" t="s">
         <v>20</v>
       </c>
       <c r="K98" s="12" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="L98" s="8" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
     </row>
     <row r="99" spans="1:12">
       <c r="A99" s="12" t="s">
-        <v>133</v>
+        <v>196</v>
       </c>
       <c r="B99" s="12" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="C99" s="12" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="D99" s="12"/>
       <c r="E99" s="12"/>
       <c r="F99" s="12" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="G99" s="12"/>
       <c r="H99" s="12" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="I99" s="12" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
       <c r="J99" s="12" t="s">
         <v>20</v>
       </c>
       <c r="K99" s="12" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="L99" s="8" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
     </row>
     <row r="100" spans="1:12">
       <c r="A100" s="12" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="B100" s="12" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="C100" s="12" t="s">
-        <v>59</v>
+        <v>18</v>
       </c>
       <c r="D100" s="12"/>
       <c r="E100" s="12"/>
       <c r="F100" s="12" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="G100" s="12"/>
       <c r="H100" s="12" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="I100" s="12" t="s">
-        <v>61</v>
+        <v>19</v>
       </c>
       <c r="J100" s="12" t="s">
         <v>20</v>
       </c>
       <c r="K100" s="12" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="L100" s="8" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
     </row>
     <row r="101" spans="1:12">
       <c r="A101" s="12" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="B101" s="12" t="s">
-        <v>45</v>
+        <v>140</v>
       </c>
       <c r="C101" s="12" t="s">
-        <v>59</v>
+        <v>37</v>
       </c>
       <c r="D101" s="12"/>
-      <c r="E101" s="12"/>
-      <c r="F101" s="12" t="s">
-        <v>137</v>
-      </c>
+      <c r="E101" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="F101" s="12"/>
       <c r="G101" s="12"/>
-      <c r="H101" s="12" t="s">
-        <v>135</v>
-      </c>
+      <c r="H101" s="12"/>
       <c r="I101" s="12" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="J101" s="12" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="K101" s="12" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="L101" s="8" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
     </row>
     <row r="102" spans="1:12">
       <c r="A102" s="12" t="s">
-        <v>203</v>
+        <v>139</v>
       </c>
       <c r="B102" s="12" t="s">
-        <v>30</v>
+        <v>140</v>
       </c>
       <c r="C102" s="12" t="s">
-        <v>70</v>
+        <v>37</v>
       </c>
       <c r="D102" s="12"/>
-      <c r="E102" s="12"/>
-      <c r="F102" s="12" t="s">
-        <v>139</v>
-      </c>
+      <c r="E102" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="F102" s="12"/>
       <c r="G102" s="12"/>
-      <c r="H102" s="12" t="s">
-        <v>138</v>
-      </c>
+      <c r="H102" s="12"/>
       <c r="I102" s="12" t="s">
-        <v>72</v>
+        <v>39</v>
       </c>
       <c r="J102" s="12" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="K102" s="12" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="L102" s="8" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
     </row>
     <row r="103" spans="1:12">
       <c r="A103" s="12" t="s">
-        <v>203</v>
+        <v>139</v>
       </c>
       <c r="B103" s="12" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="C103" s="12" t="s">
-        <v>70</v>
+        <v>37</v>
       </c>
       <c r="D103" s="12"/>
-      <c r="E103" s="12"/>
-      <c r="F103" s="18" t="s">
-        <v>140</v>
-      </c>
+      <c r="E103" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="F103" s="12"/>
       <c r="G103" s="12"/>
-      <c r="H103" s="12" t="s">
-        <v>138</v>
-      </c>
+      <c r="H103" s="12"/>
       <c r="I103" s="12" t="s">
-        <v>72</v>
+        <v>39</v>
       </c>
       <c r="J103" s="12" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="K103" s="12" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="L103" s="8" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
     </row>
     <row r="104" spans="1:12">
       <c r="A104" s="12" t="s">
-        <v>203</v>
+        <v>139</v>
       </c>
       <c r="B104" s="12" t="s">
-        <v>30</v>
+        <v>140</v>
       </c>
       <c r="C104" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="D104" s="12"/>
+        <v>37</v>
+      </c>
+      <c r="D104" s="12" t="s">
+        <v>141</v>
+      </c>
       <c r="E104" s="12"/>
-      <c r="F104" s="12" t="s">
-        <v>141</v>
-      </c>
+      <c r="F104" s="12"/>
       <c r="G104" s="12"/>
-      <c r="H104" s="12" t="s">
-        <v>138</v>
-      </c>
+      <c r="H104" s="12"/>
       <c r="I104" s="12" t="s">
-        <v>72</v>
+        <v>39</v>
       </c>
       <c r="J104" s="12" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="K104" s="12" t="s">
         <v>141</v>
       </c>
       <c r="L104" s="8" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
     </row>
     <row r="105" spans="1:12">
       <c r="A105" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="B105" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="C105" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D105" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="B105" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C105" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D105" s="12"/>
       <c r="E105" s="12"/>
-      <c r="F105" s="12" t="s">
-        <v>142</v>
-      </c>
+      <c r="F105" s="12"/>
       <c r="G105" s="12"/>
-      <c r="H105" s="12" t="s">
-        <v>142</v>
-      </c>
+      <c r="H105" s="12"/>
       <c r="I105" s="12" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="J105" s="12" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="K105" s="12" t="s">
         <v>142</v>
       </c>
       <c r="L105" s="8" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
     </row>
     <row r="106" spans="1:12">
       <c r="A106" s="12" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B106" s="12" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="C106" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D106" s="12"/>
-      <c r="E106" s="12" t="s">
-        <v>147</v>
-      </c>
+      <c r="D106" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="E106" s="12"/>
       <c r="F106" s="12"/>
       <c r="G106" s="12"/>
       <c r="H106" s="12"/>
@@ -7694,26 +7646,26 @@
         <v>73</v>
       </c>
       <c r="K106" s="12" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="L106" s="8" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
     </row>
     <row r="107" spans="1:12">
       <c r="A107" s="12" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B107" s="12" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="C107" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D107" s="12"/>
-      <c r="E107" s="12" t="s">
-        <v>148</v>
-      </c>
+      <c r="D107" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="E107" s="12"/>
       <c r="F107" s="12"/>
       <c r="G107" s="12"/>
       <c r="H107" s="12"/>
@@ -7724,26 +7676,26 @@
         <v>73</v>
       </c>
       <c r="K107" s="12" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="L107" s="8" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
     </row>
     <row r="108" spans="1:12">
       <c r="A108" s="12" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B108" s="12" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="C108" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D108" s="12"/>
-      <c r="E108" s="12" t="s">
-        <v>149</v>
-      </c>
+      <c r="D108" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="E108" s="12"/>
       <c r="F108" s="12"/>
       <c r="G108" s="12"/>
       <c r="H108" s="12"/>
@@ -7754,24 +7706,24 @@
         <v>73</v>
       </c>
       <c r="K108" s="12" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="L108" s="8" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
     </row>
     <row r="109" spans="1:12">
       <c r="A109" s="12" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B109" s="12" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="C109" s="12" t="s">
         <v>37</v>
       </c>
       <c r="D109" s="12" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="E109" s="12"/>
       <c r="F109" s="12"/>
@@ -7784,24 +7736,24 @@
         <v>73</v>
       </c>
       <c r="K109" s="12" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="L109" s="8" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
     </row>
     <row r="110" spans="1:12">
       <c r="A110" s="12" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B110" s="12" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="C110" s="12" t="s">
-        <v>37</v>
+        <v>63</v>
       </c>
       <c r="D110" s="12" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="E110" s="12"/>
       <c r="F110" s="12"/>
@@ -7814,24 +7766,24 @@
         <v>73</v>
       </c>
       <c r="K110" s="12" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="L110" s="8" t="s">
-        <v>310</v>
+        <v>299</v>
       </c>
     </row>
     <row r="111" spans="1:12">
       <c r="A111" s="12" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B111" s="12" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C111" s="12" t="s">
         <v>37</v>
       </c>
       <c r="D111" s="12" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E111" s="12"/>
       <c r="F111" s="12"/>
@@ -7844,414 +7796,144 @@
         <v>73</v>
       </c>
       <c r="K111" s="12" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="L111" s="8" t="s">
-        <v>316</v>
+        <v>304</v>
       </c>
     </row>
     <row r="112" spans="1:12">
       <c r="A112" s="12" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="B112" s="12" t="s">
-        <v>151</v>
+        <v>17</v>
       </c>
       <c r="C112" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="D112" s="12" t="s">
-        <v>157</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="D112" s="12"/>
       <c r="E112" s="12"/>
-      <c r="F112" s="12"/>
+      <c r="F112" s="12" t="s">
+        <v>156</v>
+      </c>
       <c r="G112" s="12"/>
-      <c r="H112" s="12"/>
+      <c r="H112" s="12" t="s">
+        <v>155</v>
+      </c>
       <c r="I112" s="12" t="s">
-        <v>39</v>
+        <v>72</v>
       </c>
       <c r="J112" s="12" t="s">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="K112" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="L112" s="8" t="s">
-        <v>317</v>
+        <v>305</v>
       </c>
     </row>
     <row r="113" spans="1:12">
       <c r="A113" s="12" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="B113" s="12" t="s">
-        <v>151</v>
+        <v>17</v>
       </c>
       <c r="C113" s="12" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="D113" s="12"/>
       <c r="E113" s="12"/>
-      <c r="F113" s="18"/>
-      <c r="G113" s="12" t="s">
-        <v>152</v>
-      </c>
-      <c r="H113" s="12"/>
+      <c r="F113" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="G113" s="12"/>
+      <c r="H113" s="12" t="s">
+        <v>155</v>
+      </c>
       <c r="I113" s="12" t="s">
-        <v>39</v>
+        <v>72</v>
       </c>
       <c r="J113" s="12" t="s">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="K113" s="12" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="L113" s="8" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
     </row>
     <row r="114" spans="1:12">
       <c r="A114" s="12" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="B114" s="12" t="s">
-        <v>151</v>
+        <v>17</v>
       </c>
       <c r="C114" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="D114" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D114" s="12"/>
+      <c r="E114" s="12"/>
+      <c r="F114" s="12" t="s">
         <v>158</v>
       </c>
-      <c r="E114" s="12"/>
-      <c r="F114" s="12"/>
       <c r="G114" s="12"/>
-      <c r="H114" s="12"/>
+      <c r="H114" s="12" t="s">
+        <v>155</v>
+      </c>
       <c r="I114" s="12" t="s">
-        <v>39</v>
+        <v>72</v>
       </c>
       <c r="J114" s="12" t="s">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="K114" s="12" t="s">
         <v>158</v>
       </c>
       <c r="L114" s="8" t="s">
-        <v>318</v>
+        <v>307</v>
       </c>
     </row>
     <row r="115" spans="1:12">
       <c r="A115" s="12" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="B115" s="12" t="s">
-        <v>151</v>
+        <v>17</v>
       </c>
       <c r="C115" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="D115" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D115" s="12"/>
+      <c r="E115" s="12"/>
+      <c r="F115" s="12" t="s">
         <v>159</v>
       </c>
-      <c r="E115" s="12"/>
-      <c r="F115" s="12"/>
       <c r="G115" s="12"/>
-      <c r="H115" s="12"/>
+      <c r="H115" s="12" t="s">
+        <v>155</v>
+      </c>
       <c r="I115" s="12" t="s">
-        <v>39</v>
+        <v>72</v>
       </c>
       <c r="J115" s="12" t="s">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="K115" s="12" t="s">
         <v>159</v>
       </c>
       <c r="L115" s="8" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="116" spans="1:12">
-      <c r="A116" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="B116" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="C116" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="D116" s="12" t="s">
-        <v>160</v>
-      </c>
-      <c r="E116" s="12"/>
-      <c r="F116" s="12"/>
-      <c r="G116" s="12"/>
-      <c r="H116" s="12"/>
-      <c r="I116" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="J116" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="K116" s="12" t="s">
-        <v>160</v>
-      </c>
-      <c r="L116" s="8" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="117" spans="1:12">
-      <c r="A117" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="B117" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="C117" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="D117" s="12"/>
-      <c r="E117" s="12"/>
-      <c r="F117" s="12"/>
-      <c r="G117" s="12" t="s">
-        <v>153</v>
-      </c>
-      <c r="H117" s="12"/>
-      <c r="I117" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="J117" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="K117" s="12" t="s">
-        <v>153</v>
-      </c>
-      <c r="L117" s="8" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="118" spans="1:12">
-      <c r="A118" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="B118" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="C118" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="D118" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="E118" s="12"/>
-      <c r="F118" s="12"/>
-      <c r="G118" s="12"/>
-      <c r="H118" s="12"/>
-      <c r="I118" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="J118" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="K118" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="L118" s="8" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="119" spans="1:12">
-      <c r="A119" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="B119" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="C119" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="D119" s="12"/>
-      <c r="E119" s="12"/>
-      <c r="F119" s="12"/>
-      <c r="G119" s="12" t="s">
-        <v>154</v>
-      </c>
-      <c r="H119" s="12"/>
-      <c r="I119" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="J119" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="K119" s="12" t="s">
-        <v>154</v>
-      </c>
-      <c r="L119" s="8" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="120" spans="1:12">
-      <c r="A120" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="B120" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="C120" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="D120" s="12"/>
-      <c r="E120" s="12"/>
-      <c r="F120" s="12"/>
-      <c r="G120" s="12" t="s">
-        <v>155</v>
-      </c>
-      <c r="H120" s="12"/>
-      <c r="I120" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="J120" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="K120" s="12" t="s">
-        <v>155</v>
-      </c>
-      <c r="L120" s="8" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="121" spans="1:12">
-      <c r="A121" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="B121" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C121" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="D121" s="12"/>
-      <c r="E121" s="12"/>
-      <c r="F121" s="12" t="s">
-        <v>163</v>
-      </c>
-      <c r="G121" s="12"/>
-      <c r="H121" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="I121" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="J121" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="K121" s="12" t="s">
-        <v>163</v>
-      </c>
-      <c r="L121" s="8" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="122" spans="1:12">
-      <c r="A122" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="B122" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C122" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="D122" s="12"/>
-      <c r="E122" s="12"/>
-      <c r="F122" s="12" t="s">
-        <v>164</v>
-      </c>
-      <c r="G122" s="12"/>
-      <c r="H122" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="I122" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="J122" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="K122" s="12" t="s">
-        <v>164</v>
-      </c>
-      <c r="L122" s="8" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="123" spans="1:12">
-      <c r="A123" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="B123" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C123" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="D123" s="12"/>
-      <c r="E123" s="12"/>
-      <c r="F123" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="G123" s="12"/>
-      <c r="H123" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="I123" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="J123" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="K123" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="L123" s="8" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="124" spans="1:12">
-      <c r="A124" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="B124" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C124" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="D124" s="12"/>
-      <c r="E124" s="12"/>
-      <c r="F124" s="12" t="s">
-        <v>166</v>
-      </c>
-      <c r="G124" s="12"/>
-      <c r="H124" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="I124" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="J124" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="K124" s="12" t="s">
-        <v>166</v>
-      </c>
-      <c r="L124" s="8" t="s">
-        <v>324</v>
+        <v>308</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:L1">
-    <sortState ref="A2:L124">
-      <sortCondition ref="A1:A124"/>
+    <sortState ref="A2:L115">
+      <sortCondition ref="A1:A115"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8326,7 +8008,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="12" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>63</v>
@@ -8337,7 +8019,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="12" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>70</v>
@@ -8348,7 +8030,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="12" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
Data file test update.
</commit_message>
<xml_diff>
--- a/_data/_data.xlsx
+++ b/_data/_data.xlsx
@@ -1044,6 +1044,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2070,7 +2071,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2231,7 +2232,7 @@
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
+      <selection pane="bottomLeft" activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2336,7 +2337,7 @@
       <c r="F3" s="12" t="s">
         <v>175</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="16" t="s">
         <v>17</v>
       </c>
       <c r="H3" s="12" t="s">
@@ -4406,7 +4407,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
update left nav to programmatically pull nav items from _data.xlsx
</commit_message>
<xml_diff>
--- a/_data/_data.xlsx
+++ b/_data/_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26330"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-460" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="! Instructions" sheetId="7" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1385" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1377" uniqueCount="349">
   <si>
     <t>label</t>
   </si>
@@ -1056,18 +1056,6 @@
     <t>class</t>
   </si>
   <si>
-    <t>sub-one</t>
-  </si>
-  <si>
-    <t>sub-two</t>
-  </si>
-  <si>
-    <t>sub-three</t>
-  </si>
-  <si>
-    <t>sub-four</t>
-  </si>
-  <si>
     <t>/fields-industries.html</t>
   </si>
   <si>
@@ -1077,7 +1065,16 @@
     <t>/university-transfer.html</t>
   </si>
   <si>
-    <t>/prof-techs.html</t>
+    <t>secondary</t>
+  </si>
+  <si>
+    <t>programs</t>
+  </si>
+  <si>
+    <t>/prof-tech.html</t>
+  </si>
+  <si>
+    <t>#</t>
   </si>
 </sst>
 </file>
@@ -1205,7 +1202,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="301">
+  <cellStyleXfs count="303">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1268,6 +1265,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1569,7 +1568,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="301">
+  <cellStyles count="303">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1729,6 +1728,7 @@
     <cellStyle name="Followed Hyperlink" xfId="296" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="298" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="300" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="302" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1870,6 +1870,7 @@
     <cellStyle name="Hyperlink" xfId="295" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="297" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="299" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="301" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2147,7 +2148,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData/>
@@ -2162,10 +2163,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2173,9 +2174,8 @@
     <col min="1" max="1" width="24" customWidth="1"/>
     <col min="2" max="2" width="27" customWidth="1"/>
     <col min="3" max="3" width="9.33203125" customWidth="1"/>
-    <col min="4" max="4" width="19.1640625" customWidth="1"/>
-    <col min="5" max="5" width="32.1640625" customWidth="1"/>
-    <col min="6" max="6" width="48" customWidth="1"/>
+    <col min="4" max="6" width="24" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -2197,6 +2197,9 @@
       <c r="F1" s="4" t="s">
         <v>341</v>
       </c>
+      <c r="G1" s="4" t="s">
+        <v>345</v>
+      </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
@@ -2236,6 +2239,9 @@
         <v>333</v>
       </c>
       <c r="E4" s="5" t="s">
+        <v>342</v>
+      </c>
+      <c r="G4" t="s">
         <v>346</v>
       </c>
     </row>
@@ -2249,7 +2255,10 @@
         <v>334</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>347</v>
+        <v>343</v>
+      </c>
+      <c r="G5" t="s">
+        <v>346</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -2262,7 +2271,10 @@
         <v>335</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>348</v>
+        <v>344</v>
+      </c>
+      <c r="G6" t="s">
+        <v>346</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -2275,7 +2287,10 @@
         <v>336</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>349</v>
+        <v>347</v>
+      </c>
+      <c r="G7" t="s">
+        <v>346</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -2288,10 +2303,13 @@
         <v>337</v>
       </c>
       <c r="E8" s="22" t="s">
-        <v>3</v>
+        <v>348</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>325</v>
+      </c>
+      <c r="G8" t="s">
+        <v>346</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -2304,10 +2322,13 @@
         <v>338</v>
       </c>
       <c r="E9" s="22" t="s">
-        <v>3</v>
+        <v>348</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>325</v>
+      </c>
+      <c r="G9" t="s">
+        <v>346</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -2320,10 +2341,13 @@
         <v>339</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>3</v>
+        <v>348</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>325</v>
+      </c>
+      <c r="G10" t="s">
+        <v>346</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -2336,10 +2360,13 @@
         <v>340</v>
       </c>
       <c r="E11" s="22" t="s">
-        <v>3</v>
+        <v>348</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>325</v>
+      </c>
+      <c r="G11" t="s">
+        <v>346</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -2349,9 +2376,7 @@
       <c r="B12" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>170</v>
-      </c>
+      <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6" t="s">
@@ -2360,90 +2385,26 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>167</v>
-      </c>
-      <c r="B13" s="5"/>
+        <v>168</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>3</v>
+      </c>
       <c r="C13" s="6"/>
-      <c r="D13" s="6" t="s">
-        <v>342</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>3</v>
-      </c>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
       <c r="F13" s="6" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>167</v>
-      </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6" t="s">
-        <v>343</v>
-      </c>
-      <c r="E14" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>3</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" t="s">
-        <v>167</v>
-      </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6" t="s">
-        <v>344</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" t="s">
-        <v>167</v>
-      </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6" t="s">
-        <v>345</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" t="s">
-        <v>168</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" t="s">
-        <v>169</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F18" s="6" t="s">
         <v>325</v>
       </c>
     </row>

</xml_diff>